<commit_message>
Updated coal retirments to avoid double counting Sherco 3 and updated reference scenario to use PMCCS instead of RPS policy for additional wind and solar
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\PMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Minnesota\MN_mod\InputData\elec\PMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1129EB43-53CA-4DBE-AD5F-8CAE781283C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="11565"/>
+    <workbookView xWindow="3075" yWindow="1770" windowWidth="23850" windowHeight="13710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="PMCCS" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="PMCCS" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>PMCCS Policy Mandated Capacity Construction Schedule</t>
   </si>
@@ -95,13 +108,43 @@
   </si>
   <si>
     <t>municipal solid waste</t>
+  </si>
+  <si>
+    <t>Xcel IRP</t>
+  </si>
+  <si>
+    <t>https://www.greentechmedia.com/articles/read/xcel-energy-accelerates-coal-plant-closures-to-meet-100-clean-energy-goal</t>
+  </si>
+  <si>
+    <t>https://www.xcelenergy.com/staticfiles/xe-responsive/Company/Rates%20&amp;%20Regulations/The-Resource-Plan-No-Appendices.pdf</t>
+  </si>
+  <si>
+    <t>Additional capacity:</t>
+  </si>
+  <si>
+    <t>In Minnesota</t>
+  </si>
+  <si>
+    <t>solar pv</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>already have 1000 MW of solar</t>
+  </si>
+  <si>
+    <t>https://www.greentechmedia.com/articles/read/xcel-targets-1.4b-in-wind-solar-investments-outlines-broader-carbon-reduction-goals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,13 +160,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF313131"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,9 +193,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,6 +214,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>589683</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>113819</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B63054-7A12-430D-BE43-D031E4B40FDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11944350" y="647700"/>
+          <a:ext cx="6933333" cy="3847619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>227831</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEC915B4-35B8-4896-B271-1A35E886D8BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5657850" y="857250"/>
+          <a:ext cx="6152381" cy="3457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>142113</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114074</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EAA7526-2650-4B17-B1FB-9A8D24EC0D87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5629275" y="4467225"/>
+          <a:ext cx="6095238" cy="1809524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -234,6 +429,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -269,6 +481,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,10 +673,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -496,14 +725,128 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF686BE5-FC61-4D3A-AC20-612E5D71A1AB}">
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>2025</v>
+      </c>
+      <c r="D8">
+        <v>2030</v>
+      </c>
+      <c r="E8">
+        <v>2034</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>450</v>
+      </c>
+      <c r="D9">
+        <f>4000-C9</f>
+        <v>3550</v>
+      </c>
+      <c r="F9" s="3">
+        <f>SUM(C9:E9)</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>650</v>
+      </c>
+      <c r="E10">
+        <f>1850-C10</f>
+        <v>1200</v>
+      </c>
+      <c r="F10" s="3">
+        <f>SUM(E10:E10)</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="26" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J32" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1418,8 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <f>Sheet1!C10</f>
+        <v>650</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1102,7 +1446,8 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <f>Sheet1!E10</f>
+        <v>1200</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1182,7 +1527,8 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <f>Sheet1!C9</f>
+        <v>450</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1197,7 +1543,8 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <f>Sheet1!D9</f>
+        <v>3550</v>
       </c>
       <c r="P7">
         <v>0</v>

</xml_diff>

<commit_message>
Update linear phase in PMCCS
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Minnesota\MN_mod\InputData\elec\PMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C559F1-2A0B-4CAC-9888-DF7AA5958654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FCD70C-5506-49AF-B266-C9EBE6F83EAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="615" windowWidth="25620" windowHeight="14595" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="480" windowWidth="24810" windowHeight="16350" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="MN IRP" sheetId="3" r:id="rId2"/>
     <sheet name="BPMCCS" sheetId="4" r:id="rId3"/>
     <sheet name="PMCCS" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>PMCCS Policy Mandated Capacity Construction Schedule</t>
   </si>
@@ -143,6 +143,9 @@
   <si>
     <t>Mandated Construction (MW)</t>
   </si>
+  <si>
+    <t>per year</t>
+  </si>
 </sst>
 </file>
 
@@ -185,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -193,16 +196,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,16 +243,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>129117</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>430933</xdr:colOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>356850</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>50319</xdr:rowOff>
+      <xdr:rowOff>82069</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -256,8 +275,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16490950" y="203200"/>
-          <a:ext cx="6863483" cy="3847619"/>
+          <a:off x="17316450" y="234950"/>
+          <a:ext cx="6979900" cy="3847619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -312,16 +331,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>358775</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411692</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:rowOff>115359</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>358013</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>410929</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>41049</xdr:rowOff>
+      <xdr:rowOff>19883</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -344,8 +363,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5184775" y="898525"/>
-          <a:ext cx="6031738" cy="1809524"/>
+          <a:off x="4708525" y="877359"/>
+          <a:ext cx="6137571" cy="1809524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -732,33 +751,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF686BE5-FC61-4D3A-AC20-612E5D71A1AB}">
   <dimension ref="A1:AG46"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -766,53 +785,67 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
         <v>2025</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>2030</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>2034</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>450</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <f>4000-C9</f>
         <v>3550</v>
       </c>
-      <c r="F9" s="3">
+      <c r="E9" s="4"/>
+      <c r="F9" s="5">
         <f>SUM(C9:E9)</f>
         <v>4000</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="G9">
+        <f>D9/(30-25)</f>
+        <v>710</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>650</v>
       </c>
-      <c r="E10">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
         <f>1850-C10</f>
         <v>1200</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <f>SUM(E10:E10)</f>
         <v>1200</v>
+      </c>
+      <c r="G10">
+        <f>F10/(34-25)</f>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
@@ -944,9 +977,41 @@
         <f>C10</f>
         <v>650</v>
       </c>
+      <c r="I32">
+        <f>$G$10</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32:Q32" si="0">$G$10</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
+      </c>
       <c r="Q32">
-        <f>E10</f>
-        <v>1200</v>
+        <f t="shared" si="0"/>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -957,9 +1022,25 @@
         <f>C9</f>
         <v>450</v>
       </c>
+      <c r="I33">
+        <f>$G$9</f>
+        <v>710</v>
+      </c>
+      <c r="J33">
+        <f t="shared" ref="J33:M33" si="1">$G$9</f>
+        <v>710</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>710</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>710</v>
+      </c>
       <c r="M33">
-        <f>D9</f>
-        <v>3550</v>
+        <f t="shared" si="1"/>
+        <v>710</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -996,38 +1077,39 @@
       <c r="A40" t="s">
         <v>21</v>
       </c>
-      <c r="J40" s="4"/>
+      <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="4"/>
+      <c r="J41" s="3"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="4"/>
+      <c r="J42" s="3"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="4"/>
+      <c r="J43" s="3"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J44" s="4"/>
+      <c r="J44" s="3"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J45" s="4"/>
+      <c r="J45" s="3"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J46" s="4"/>
+      <c r="J46" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1036,7 +1118,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AG1"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,8 +2852,8 @@
   </sheetPr>
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:AI17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,131 +2979,131 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>SUM(BPMCCS!B2,Sheet1!B28)</f>
+        <f>SUM(BPMCCS!B2,'MN IRP'!B28)</f>
         <v>22.599999999999909</v>
       </c>
       <c r="E2">
-        <f>SUM(BPMCCS!C2,Sheet1!C28)</f>
+        <f>SUM(BPMCCS!C2,'MN IRP'!C28)</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>SUM(BPMCCS!D2,Sheet1!D28)</f>
+        <f>SUM(BPMCCS!D2,'MN IRP'!D28)</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUM(BPMCCS!E2,Sheet1!E28)</f>
+        <f>SUM(BPMCCS!E2,'MN IRP'!E28)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>SUM(BPMCCS!F2,Sheet1!F28)</f>
+        <f>SUM(BPMCCS!F2,'MN IRP'!F28)</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>SUM(BPMCCS!G2,Sheet1!G28)</f>
+        <f>SUM(BPMCCS!G2,'MN IRP'!G28)</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>SUM(BPMCCS!H2,Sheet1!H28)</f>
+        <f>SUM(BPMCCS!H2,'MN IRP'!H28)</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>SUM(BPMCCS!I2,Sheet1!I28)</f>
+        <f>SUM(BPMCCS!I2,'MN IRP'!I28)</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>SUM(BPMCCS!J2,Sheet1!J28)</f>
+        <f>SUM(BPMCCS!J2,'MN IRP'!J28)</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>SUM(BPMCCS!K2,Sheet1!K28)</f>
+        <f>SUM(BPMCCS!K2,'MN IRP'!K28)</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>SUM(BPMCCS!L2,Sheet1!L28)</f>
+        <f>SUM(BPMCCS!L2,'MN IRP'!L28)</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f>SUM(BPMCCS!M2,Sheet1!M28)</f>
+        <f>SUM(BPMCCS!M2,'MN IRP'!M28)</f>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>SUM(BPMCCS!N2,Sheet1!N28)</f>
+        <f>SUM(BPMCCS!N2,'MN IRP'!N28)</f>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>SUM(BPMCCS!O2,Sheet1!O28)</f>
+        <f>SUM(BPMCCS!O2,'MN IRP'!O28)</f>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>SUM(BPMCCS!P2,Sheet1!P28)</f>
+        <f>SUM(BPMCCS!P2,'MN IRP'!P28)</f>
         <v>0</v>
       </c>
       <c r="S2">
-        <f>SUM(BPMCCS!Q2,Sheet1!Q28)</f>
+        <f>SUM(BPMCCS!Q2,'MN IRP'!Q28)</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f>SUM(BPMCCS!R2,Sheet1!R28)</f>
+        <f>SUM(BPMCCS!R2,'MN IRP'!R28)</f>
         <v>0</v>
       </c>
       <c r="U2">
-        <f>SUM(BPMCCS!S2,Sheet1!S28)</f>
+        <f>SUM(BPMCCS!S2,'MN IRP'!S28)</f>
         <v>0</v>
       </c>
       <c r="V2">
-        <f>SUM(BPMCCS!T2,Sheet1!T28)</f>
+        <f>SUM(BPMCCS!T2,'MN IRP'!T28)</f>
         <v>0</v>
       </c>
       <c r="W2">
-        <f>SUM(BPMCCS!U2,Sheet1!U28)</f>
+        <f>SUM(BPMCCS!U2,'MN IRP'!U28)</f>
         <v>0</v>
       </c>
       <c r="X2">
-        <f>SUM(BPMCCS!V2,Sheet1!V28)</f>
+        <f>SUM(BPMCCS!V2,'MN IRP'!V28)</f>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f>SUM(BPMCCS!W2,Sheet1!W28)</f>
+        <f>SUM(BPMCCS!W2,'MN IRP'!W28)</f>
         <v>0</v>
       </c>
       <c r="Z2">
-        <f>SUM(BPMCCS!X2,Sheet1!X28)</f>
+        <f>SUM(BPMCCS!X2,'MN IRP'!X28)</f>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f>SUM(BPMCCS!Y2,Sheet1!Y28)</f>
+        <f>SUM(BPMCCS!Y2,'MN IRP'!Y28)</f>
         <v>0</v>
       </c>
       <c r="AB2">
-        <f>SUM(BPMCCS!Z2,Sheet1!Z28)</f>
+        <f>SUM(BPMCCS!Z2,'MN IRP'!Z28)</f>
         <v>0</v>
       </c>
       <c r="AC2">
-        <f>SUM(BPMCCS!AA2,Sheet1!AA28)</f>
+        <f>SUM(BPMCCS!AA2,'MN IRP'!AA28)</f>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f>SUM(BPMCCS!AB2,Sheet1!AB28)</f>
+        <f>SUM(BPMCCS!AB2,'MN IRP'!AB28)</f>
         <v>0</v>
       </c>
       <c r="AE2">
-        <f>SUM(BPMCCS!AC2,Sheet1!AC28)</f>
+        <f>SUM(BPMCCS!AC2,'MN IRP'!AC28)</f>
         <v>0</v>
       </c>
       <c r="AF2">
-        <f>SUM(BPMCCS!AD2,Sheet1!AD28)</f>
+        <f>SUM(BPMCCS!AD2,'MN IRP'!AD28)</f>
         <v>0</v>
       </c>
       <c r="AG2">
-        <f>SUM(BPMCCS!AE2,Sheet1!AE28)</f>
+        <f>SUM(BPMCCS!AE2,'MN IRP'!AE28)</f>
         <v>0</v>
       </c>
       <c r="AH2">
-        <f>SUM(BPMCCS!AF2,Sheet1!AF28)</f>
+        <f>SUM(BPMCCS!AF2,'MN IRP'!AF28)</f>
         <v>0</v>
       </c>
       <c r="AI2">
-        <f>SUM(BPMCCS!AG2,Sheet1!AG28)</f>
+        <f>SUM(BPMCCS!AG2,'MN IRP'!AG28)</f>
         <v>0</v>
       </c>
     </row>
@@ -3036,131 +3118,131 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>SUM(BPMCCS!B3,Sheet1!B29)</f>
+        <f>SUM(BPMCCS!B3,'MN IRP'!B29)</f>
         <v>324</v>
       </c>
       <c r="E3">
-        <f>SUM(BPMCCS!C3,Sheet1!C29)</f>
+        <f>SUM(BPMCCS!C3,'MN IRP'!C29)</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f>SUM(BPMCCS!D3,Sheet1!D29)</f>
+        <f>SUM(BPMCCS!D3,'MN IRP'!D29)</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f>SUM(BPMCCS!E3,Sheet1!E29)</f>
+        <f>SUM(BPMCCS!E3,'MN IRP'!E29)</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f>SUM(BPMCCS!F3,Sheet1!F29)</f>
+        <f>SUM(BPMCCS!F3,'MN IRP'!F29)</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f>SUM(BPMCCS!G3,Sheet1!G29)</f>
+        <f>SUM(BPMCCS!G3,'MN IRP'!G29)</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f>SUM(BPMCCS!H3,Sheet1!H29)</f>
+        <f>SUM(BPMCCS!H3,'MN IRP'!H29)</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f>SUM(BPMCCS!I3,Sheet1!I29)</f>
+        <f>SUM(BPMCCS!I3,'MN IRP'!I29)</f>
         <v>0</v>
       </c>
       <c r="L3">
-        <f>SUM(BPMCCS!J3,Sheet1!J29)</f>
+        <f>SUM(BPMCCS!J3,'MN IRP'!J29)</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f>SUM(BPMCCS!K3,Sheet1!K29)</f>
+        <f>SUM(BPMCCS!K3,'MN IRP'!K29)</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>SUM(BPMCCS!L3,Sheet1!L29)</f>
+        <f>SUM(BPMCCS!L3,'MN IRP'!L29)</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f>SUM(BPMCCS!M3,Sheet1!M29)</f>
+        <f>SUM(BPMCCS!M3,'MN IRP'!M29)</f>
         <v>0</v>
       </c>
       <c r="P3">
-        <f>SUM(BPMCCS!N3,Sheet1!N29)</f>
+        <f>SUM(BPMCCS!N3,'MN IRP'!N29)</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f>SUM(BPMCCS!O3,Sheet1!O29)</f>
+        <f>SUM(BPMCCS!O3,'MN IRP'!O29)</f>
         <v>0</v>
       </c>
       <c r="R3">
-        <f>SUM(BPMCCS!P3,Sheet1!P29)</f>
+        <f>SUM(BPMCCS!P3,'MN IRP'!P29)</f>
         <v>0</v>
       </c>
       <c r="S3">
-        <f>SUM(BPMCCS!Q3,Sheet1!Q29)</f>
+        <f>SUM(BPMCCS!Q3,'MN IRP'!Q29)</f>
         <v>0</v>
       </c>
       <c r="T3">
-        <f>SUM(BPMCCS!R3,Sheet1!R29)</f>
+        <f>SUM(BPMCCS!R3,'MN IRP'!R29)</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f>SUM(BPMCCS!S3,Sheet1!S29)</f>
+        <f>SUM(BPMCCS!S3,'MN IRP'!S29)</f>
         <v>0</v>
       </c>
       <c r="V3">
-        <f>SUM(BPMCCS!T3,Sheet1!T29)</f>
+        <f>SUM(BPMCCS!T3,'MN IRP'!T29)</f>
         <v>0</v>
       </c>
       <c r="W3">
-        <f>SUM(BPMCCS!U3,Sheet1!U29)</f>
+        <f>SUM(BPMCCS!U3,'MN IRP'!U29)</f>
         <v>0</v>
       </c>
       <c r="X3">
-        <f>SUM(BPMCCS!V3,Sheet1!V29)</f>
+        <f>SUM(BPMCCS!V3,'MN IRP'!V29)</f>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f>SUM(BPMCCS!W3,Sheet1!W29)</f>
+        <f>SUM(BPMCCS!W3,'MN IRP'!W29)</f>
         <v>0</v>
       </c>
       <c r="Z3">
-        <f>SUM(BPMCCS!X3,Sheet1!X29)</f>
+        <f>SUM(BPMCCS!X3,'MN IRP'!X29)</f>
         <v>0</v>
       </c>
       <c r="AA3">
-        <f>SUM(BPMCCS!Y3,Sheet1!Y29)</f>
+        <f>SUM(BPMCCS!Y3,'MN IRP'!Y29)</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f>SUM(BPMCCS!Z3,Sheet1!Z29)</f>
+        <f>SUM(BPMCCS!Z3,'MN IRP'!Z29)</f>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f>SUM(BPMCCS!AA3,Sheet1!AA29)</f>
+        <f>SUM(BPMCCS!AA3,'MN IRP'!AA29)</f>
         <v>0</v>
       </c>
       <c r="AD3">
-        <f>SUM(BPMCCS!AB3,Sheet1!AB29)</f>
+        <f>SUM(BPMCCS!AB3,'MN IRP'!AB29)</f>
         <v>0</v>
       </c>
       <c r="AE3">
-        <f>SUM(BPMCCS!AC3,Sheet1!AC29)</f>
+        <f>SUM(BPMCCS!AC3,'MN IRP'!AC29)</f>
         <v>0</v>
       </c>
       <c r="AF3">
-        <f>SUM(BPMCCS!AD3,Sheet1!AD29)</f>
+        <f>SUM(BPMCCS!AD3,'MN IRP'!AD29)</f>
         <v>0</v>
       </c>
       <c r="AG3">
-        <f>SUM(BPMCCS!AE3,Sheet1!AE29)</f>
+        <f>SUM(BPMCCS!AE3,'MN IRP'!AE29)</f>
         <v>0</v>
       </c>
       <c r="AH3">
-        <f>SUM(BPMCCS!AF3,Sheet1!AF29)</f>
+        <f>SUM(BPMCCS!AF3,'MN IRP'!AF29)</f>
         <v>0</v>
       </c>
       <c r="AI3">
-        <f>SUM(BPMCCS!AG3,Sheet1!AG29)</f>
+        <f>SUM(BPMCCS!AG3,'MN IRP'!AG29)</f>
         <v>0</v>
       </c>
     </row>
@@ -3175,131 +3257,131 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>SUM(BPMCCS!B4,Sheet1!B30)</f>
+        <f>SUM(BPMCCS!B4,'MN IRP'!B30)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>SUM(BPMCCS!C4,Sheet1!C30)</f>
+        <f>SUM(BPMCCS!C4,'MN IRP'!C30)</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>SUM(BPMCCS!D4,Sheet1!D30)</f>
+        <f>SUM(BPMCCS!D4,'MN IRP'!D30)</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUM(BPMCCS!E4,Sheet1!E30)</f>
+        <f>SUM(BPMCCS!E4,'MN IRP'!E30)</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>SUM(BPMCCS!F4,Sheet1!F30)</f>
+        <f>SUM(BPMCCS!F4,'MN IRP'!F30)</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>SUM(BPMCCS!G4,Sheet1!G30)</f>
+        <f>SUM(BPMCCS!G4,'MN IRP'!G30)</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>SUM(BPMCCS!H4,Sheet1!H30)</f>
+        <f>SUM(BPMCCS!H4,'MN IRP'!H30)</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>SUM(BPMCCS!I4,Sheet1!I30)</f>
+        <f>SUM(BPMCCS!I4,'MN IRP'!I30)</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>SUM(BPMCCS!J4,Sheet1!J30)</f>
+        <f>SUM(BPMCCS!J4,'MN IRP'!J30)</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f>SUM(BPMCCS!K4,Sheet1!K30)</f>
+        <f>SUM(BPMCCS!K4,'MN IRP'!K30)</f>
         <v>0</v>
       </c>
       <c r="N4">
-        <f>SUM(BPMCCS!L4,Sheet1!L30)</f>
+        <f>SUM(BPMCCS!L4,'MN IRP'!L30)</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>SUM(BPMCCS!M4,Sheet1!M30)</f>
+        <f>SUM(BPMCCS!M4,'MN IRP'!M30)</f>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>SUM(BPMCCS!N4,Sheet1!N30)</f>
+        <f>SUM(BPMCCS!N4,'MN IRP'!N30)</f>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>SUM(BPMCCS!O4,Sheet1!O30)</f>
+        <f>SUM(BPMCCS!O4,'MN IRP'!O30)</f>
         <v>0</v>
       </c>
       <c r="R4">
-        <f>SUM(BPMCCS!P4,Sheet1!P30)</f>
+        <f>SUM(BPMCCS!P4,'MN IRP'!P30)</f>
         <v>0</v>
       </c>
       <c r="S4">
-        <f>SUM(BPMCCS!Q4,Sheet1!Q30)</f>
+        <f>SUM(BPMCCS!Q4,'MN IRP'!Q30)</f>
         <v>0</v>
       </c>
       <c r="T4">
-        <f>SUM(BPMCCS!R4,Sheet1!R30)</f>
+        <f>SUM(BPMCCS!R4,'MN IRP'!R30)</f>
         <v>0</v>
       </c>
       <c r="U4">
-        <f>SUM(BPMCCS!S4,Sheet1!S30)</f>
+        <f>SUM(BPMCCS!S4,'MN IRP'!S30)</f>
         <v>0</v>
       </c>
       <c r="V4">
-        <f>SUM(BPMCCS!T4,Sheet1!T30)</f>
+        <f>SUM(BPMCCS!T4,'MN IRP'!T30)</f>
         <v>0</v>
       </c>
       <c r="W4">
-        <f>SUM(BPMCCS!U4,Sheet1!U30)</f>
+        <f>SUM(BPMCCS!U4,'MN IRP'!U30)</f>
         <v>0</v>
       </c>
       <c r="X4">
-        <f>SUM(BPMCCS!V4,Sheet1!V30)</f>
+        <f>SUM(BPMCCS!V4,'MN IRP'!V30)</f>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f>SUM(BPMCCS!W4,Sheet1!W30)</f>
+        <f>SUM(BPMCCS!W4,'MN IRP'!W30)</f>
         <v>0</v>
       </c>
       <c r="Z4">
-        <f>SUM(BPMCCS!X4,Sheet1!X30)</f>
+        <f>SUM(BPMCCS!X4,'MN IRP'!X30)</f>
         <v>0</v>
       </c>
       <c r="AA4">
-        <f>SUM(BPMCCS!Y4,Sheet1!Y30)</f>
+        <f>SUM(BPMCCS!Y4,'MN IRP'!Y30)</f>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f>SUM(BPMCCS!Z4,Sheet1!Z30)</f>
+        <f>SUM(BPMCCS!Z4,'MN IRP'!Z30)</f>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f>SUM(BPMCCS!AA4,Sheet1!AA30)</f>
+        <f>SUM(BPMCCS!AA4,'MN IRP'!AA30)</f>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f>SUM(BPMCCS!AB4,Sheet1!AB30)</f>
+        <f>SUM(BPMCCS!AB4,'MN IRP'!AB30)</f>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>SUM(BPMCCS!AC4,Sheet1!AC30)</f>
+        <f>SUM(BPMCCS!AC4,'MN IRP'!AC30)</f>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f>SUM(BPMCCS!AD4,Sheet1!AD30)</f>
+        <f>SUM(BPMCCS!AD4,'MN IRP'!AD30)</f>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f>SUM(BPMCCS!AE4,Sheet1!AE30)</f>
+        <f>SUM(BPMCCS!AE4,'MN IRP'!AE30)</f>
         <v>0</v>
       </c>
       <c r="AH4">
-        <f>SUM(BPMCCS!AF4,Sheet1!AF30)</f>
+        <f>SUM(BPMCCS!AF4,'MN IRP'!AF30)</f>
         <v>0</v>
       </c>
       <c r="AI4">
-        <f>SUM(BPMCCS!AG4,Sheet1!AG30)</f>
+        <f>SUM(BPMCCS!AG4,'MN IRP'!AG30)</f>
         <v>0</v>
       </c>
     </row>
@@ -3314,131 +3396,131 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>SUM(BPMCCS!B5,Sheet1!B31)</f>
+        <f>SUM(BPMCCS!B5,'MN IRP'!B31)</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>SUM(BPMCCS!C5,Sheet1!C31)</f>
+        <f>SUM(BPMCCS!C5,'MN IRP'!C31)</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>SUM(BPMCCS!D5,Sheet1!D31)</f>
+        <f>SUM(BPMCCS!D5,'MN IRP'!D31)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>SUM(BPMCCS!E5,Sheet1!E31)</f>
+        <f>SUM(BPMCCS!E5,'MN IRP'!E31)</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>SUM(BPMCCS!F5,Sheet1!F31)</f>
+        <f>SUM(BPMCCS!F5,'MN IRP'!F31)</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f>SUM(BPMCCS!G5,Sheet1!G31)</f>
+        <f>SUM(BPMCCS!G5,'MN IRP'!G31)</f>
         <v>0</v>
       </c>
       <c r="J5">
-        <f>SUM(BPMCCS!H5,Sheet1!H31)</f>
+        <f>SUM(BPMCCS!H5,'MN IRP'!H31)</f>
         <v>0</v>
       </c>
       <c r="K5">
-        <f>SUM(BPMCCS!I5,Sheet1!I31)</f>
+        <f>SUM(BPMCCS!I5,'MN IRP'!I31)</f>
         <v>0</v>
       </c>
       <c r="L5">
-        <f>SUM(BPMCCS!J5,Sheet1!J31)</f>
+        <f>SUM(BPMCCS!J5,'MN IRP'!J31)</f>
         <v>0</v>
       </c>
       <c r="M5">
-        <f>SUM(BPMCCS!K5,Sheet1!K31)</f>
+        <f>SUM(BPMCCS!K5,'MN IRP'!K31)</f>
         <v>0</v>
       </c>
       <c r="N5">
-        <f>SUM(BPMCCS!L5,Sheet1!L31)</f>
+        <f>SUM(BPMCCS!L5,'MN IRP'!L31)</f>
         <v>0</v>
       </c>
       <c r="O5">
-        <f>SUM(BPMCCS!M5,Sheet1!M31)</f>
+        <f>SUM(BPMCCS!M5,'MN IRP'!M31)</f>
         <v>0</v>
       </c>
       <c r="P5">
-        <f>SUM(BPMCCS!N5,Sheet1!N31)</f>
+        <f>SUM(BPMCCS!N5,'MN IRP'!N31)</f>
         <v>0</v>
       </c>
       <c r="Q5">
-        <f>SUM(BPMCCS!O5,Sheet1!O31)</f>
+        <f>SUM(BPMCCS!O5,'MN IRP'!O31)</f>
         <v>0</v>
       </c>
       <c r="R5">
-        <f>SUM(BPMCCS!P5,Sheet1!P31)</f>
+        <f>SUM(BPMCCS!P5,'MN IRP'!P31)</f>
         <v>0</v>
       </c>
       <c r="S5">
-        <f>SUM(BPMCCS!Q5,Sheet1!Q31)</f>
+        <f>SUM(BPMCCS!Q5,'MN IRP'!Q31)</f>
         <v>0</v>
       </c>
       <c r="T5">
-        <f>SUM(BPMCCS!R5,Sheet1!R31)</f>
+        <f>SUM(BPMCCS!R5,'MN IRP'!R31)</f>
         <v>0</v>
       </c>
       <c r="U5">
-        <f>SUM(BPMCCS!S5,Sheet1!S31)</f>
+        <f>SUM(BPMCCS!S5,'MN IRP'!S31)</f>
         <v>0</v>
       </c>
       <c r="V5">
-        <f>SUM(BPMCCS!T5,Sheet1!T31)</f>
+        <f>SUM(BPMCCS!T5,'MN IRP'!T31)</f>
         <v>0</v>
       </c>
       <c r="W5">
-        <f>SUM(BPMCCS!U5,Sheet1!U31)</f>
+        <f>SUM(BPMCCS!U5,'MN IRP'!U31)</f>
         <v>0</v>
       </c>
       <c r="X5">
-        <f>SUM(BPMCCS!V5,Sheet1!V31)</f>
+        <f>SUM(BPMCCS!V5,'MN IRP'!V31)</f>
         <v>0</v>
       </c>
       <c r="Y5">
-        <f>SUM(BPMCCS!W5,Sheet1!W31)</f>
+        <f>SUM(BPMCCS!W5,'MN IRP'!W31)</f>
         <v>0</v>
       </c>
       <c r="Z5">
-        <f>SUM(BPMCCS!X5,Sheet1!X31)</f>
+        <f>SUM(BPMCCS!X5,'MN IRP'!X31)</f>
         <v>0</v>
       </c>
       <c r="AA5">
-        <f>SUM(BPMCCS!Y5,Sheet1!Y31)</f>
+        <f>SUM(BPMCCS!Y5,'MN IRP'!Y31)</f>
         <v>0</v>
       </c>
       <c r="AB5">
-        <f>SUM(BPMCCS!Z5,Sheet1!Z31)</f>
+        <f>SUM(BPMCCS!Z5,'MN IRP'!Z31)</f>
         <v>0</v>
       </c>
       <c r="AC5">
-        <f>SUM(BPMCCS!AA5,Sheet1!AA31)</f>
+        <f>SUM(BPMCCS!AA5,'MN IRP'!AA31)</f>
         <v>0</v>
       </c>
       <c r="AD5">
-        <f>SUM(BPMCCS!AB5,Sheet1!AB31)</f>
+        <f>SUM(BPMCCS!AB5,'MN IRP'!AB31)</f>
         <v>0</v>
       </c>
       <c r="AE5">
-        <f>SUM(BPMCCS!AC5,Sheet1!AC31)</f>
+        <f>SUM(BPMCCS!AC5,'MN IRP'!AC31)</f>
         <v>0</v>
       </c>
       <c r="AF5">
-        <f>SUM(BPMCCS!AD5,Sheet1!AD31)</f>
+        <f>SUM(BPMCCS!AD5,'MN IRP'!AD31)</f>
         <v>0</v>
       </c>
       <c r="AG5">
-        <f>SUM(BPMCCS!AE5,Sheet1!AE31)</f>
+        <f>SUM(BPMCCS!AE5,'MN IRP'!AE31)</f>
         <v>0</v>
       </c>
       <c r="AH5">
-        <f>SUM(BPMCCS!AF5,Sheet1!AF31)</f>
+        <f>SUM(BPMCCS!AF5,'MN IRP'!AF31)</f>
         <v>0</v>
       </c>
       <c r="AI5">
-        <f>SUM(BPMCCS!AG5,Sheet1!AG31)</f>
+        <f>SUM(BPMCCS!AG5,'MN IRP'!AG31)</f>
         <v>0</v>
       </c>
     </row>
@@ -3453,131 +3535,131 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>SUM(BPMCCS!B6,Sheet1!B32)</f>
+        <f>SUM(BPMCCS!B6,'MN IRP'!B32)</f>
         <v>79.200000000000728</v>
       </c>
       <c r="E6">
-        <f>SUM(BPMCCS!C6,Sheet1!C32)</f>
+        <f>SUM(BPMCCS!C6,'MN IRP'!C32)</f>
         <v>454.6</v>
       </c>
       <c r="F6">
-        <f>SUM(BPMCCS!D6,Sheet1!D32)</f>
+        <f>SUM(BPMCCS!D6,'MN IRP'!D32)</f>
         <v>400</v>
       </c>
       <c r="G6">
-        <f>SUM(BPMCCS!E6,Sheet1!E32)</f>
+        <f>SUM(BPMCCS!E6,'MN IRP'!E32)</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>SUM(BPMCCS!F6,Sheet1!F32)</f>
+        <f>SUM(BPMCCS!F6,'MN IRP'!F32)</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>SUM(BPMCCS!G6,Sheet1!G32)</f>
+        <f>SUM(BPMCCS!G6,'MN IRP'!G32)</f>
         <v>0</v>
       </c>
       <c r="J6">
-        <f>SUM(BPMCCS!H6,Sheet1!H32)</f>
+        <f>SUM(BPMCCS!H6,'MN IRP'!H32)</f>
         <v>650</v>
       </c>
       <c r="K6">
-        <f>SUM(BPMCCS!I6,Sheet1!I32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!I6,'MN IRP'!I32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="L6">
-        <f>SUM(BPMCCS!J6,Sheet1!J32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!J6,'MN IRP'!J32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M6">
-        <f>SUM(BPMCCS!K6,Sheet1!K32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!K6,'MN IRP'!K32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="N6">
-        <f>SUM(BPMCCS!L6,Sheet1!L32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!L6,'MN IRP'!L32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="O6">
-        <f>SUM(BPMCCS!M6,Sheet1!M32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!M6,'MN IRP'!M32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="P6">
-        <f>SUM(BPMCCS!N6,Sheet1!N32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!N6,'MN IRP'!N32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="Q6">
-        <f>SUM(BPMCCS!O6,Sheet1!O32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!O6,'MN IRP'!O32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="R6">
-        <f>SUM(BPMCCS!P6,Sheet1!P32)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!P6,'MN IRP'!P32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="S6">
-        <f>SUM(BPMCCS!Q6,Sheet1!Q32)</f>
-        <v>1200</v>
+        <f>SUM(BPMCCS!Q6,'MN IRP'!Q32)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="T6">
-        <f>SUM(BPMCCS!R6,Sheet1!R32)</f>
+        <f>SUM(BPMCCS!R6,'MN IRP'!R32)</f>
         <v>0</v>
       </c>
       <c r="U6">
-        <f>SUM(BPMCCS!S6,Sheet1!S32)</f>
+        <f>SUM(BPMCCS!S6,'MN IRP'!S32)</f>
         <v>0</v>
       </c>
       <c r="V6">
-        <f>SUM(BPMCCS!T6,Sheet1!T32)</f>
+        <f>SUM(BPMCCS!T6,'MN IRP'!T32)</f>
         <v>0</v>
       </c>
       <c r="W6">
-        <f>SUM(BPMCCS!U6,Sheet1!U32)</f>
+        <f>SUM(BPMCCS!U6,'MN IRP'!U32)</f>
         <v>0</v>
       </c>
       <c r="X6">
-        <f>SUM(BPMCCS!V6,Sheet1!V32)</f>
+        <f>SUM(BPMCCS!V6,'MN IRP'!V32)</f>
         <v>0</v>
       </c>
       <c r="Y6">
-        <f>SUM(BPMCCS!W6,Sheet1!W32)</f>
+        <f>SUM(BPMCCS!W6,'MN IRP'!W32)</f>
         <v>0</v>
       </c>
       <c r="Z6">
-        <f>SUM(BPMCCS!X6,Sheet1!X32)</f>
+        <f>SUM(BPMCCS!X6,'MN IRP'!X32)</f>
         <v>0</v>
       </c>
       <c r="AA6">
-        <f>SUM(BPMCCS!Y6,Sheet1!Y32)</f>
+        <f>SUM(BPMCCS!Y6,'MN IRP'!Y32)</f>
         <v>0</v>
       </c>
       <c r="AB6">
-        <f>SUM(BPMCCS!Z6,Sheet1!Z32)</f>
+        <f>SUM(BPMCCS!Z6,'MN IRP'!Z32)</f>
         <v>0</v>
       </c>
       <c r="AC6">
-        <f>SUM(BPMCCS!AA6,Sheet1!AA32)</f>
+        <f>SUM(BPMCCS!AA6,'MN IRP'!AA32)</f>
         <v>0</v>
       </c>
       <c r="AD6">
-        <f>SUM(BPMCCS!AB6,Sheet1!AB32)</f>
+        <f>SUM(BPMCCS!AB6,'MN IRP'!AB32)</f>
         <v>0</v>
       </c>
       <c r="AE6">
-        <f>SUM(BPMCCS!AC6,Sheet1!AC32)</f>
+        <f>SUM(BPMCCS!AC6,'MN IRP'!AC32)</f>
         <v>0</v>
       </c>
       <c r="AF6">
-        <f>SUM(BPMCCS!AD6,Sheet1!AD32)</f>
+        <f>SUM(BPMCCS!AD6,'MN IRP'!AD32)</f>
         <v>0</v>
       </c>
       <c r="AG6">
-        <f>SUM(BPMCCS!AE6,Sheet1!AE32)</f>
+        <f>SUM(BPMCCS!AE6,'MN IRP'!AE32)</f>
         <v>0</v>
       </c>
       <c r="AH6">
-        <f>SUM(BPMCCS!AF6,Sheet1!AF32)</f>
+        <f>SUM(BPMCCS!AF6,'MN IRP'!AF32)</f>
         <v>0</v>
       </c>
       <c r="AI6">
-        <f>SUM(BPMCCS!AG6,Sheet1!AG32)</f>
+        <f>SUM(BPMCCS!AG6,'MN IRP'!AG32)</f>
         <v>0</v>
       </c>
     </row>
@@ -3592,131 +3674,131 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>SUM(BPMCCS!B7,Sheet1!B33)</f>
+        <f>SUM(BPMCCS!B7,'MN IRP'!B33)</f>
         <v>107.79999999999995</v>
       </c>
       <c r="E7">
-        <f>SUM(BPMCCS!C7,Sheet1!C33)</f>
+        <f>SUM(BPMCCS!C7,'MN IRP'!C33)</f>
         <v>68.400000000000006</v>
       </c>
       <c r="F7">
-        <f>SUM(BPMCCS!D7,Sheet1!D33)</f>
+        <f>SUM(BPMCCS!D7,'MN IRP'!D33)</f>
         <v>97</v>
       </c>
       <c r="G7">
-        <f>SUM(BPMCCS!E7,Sheet1!E33)</f>
+        <f>SUM(BPMCCS!E7,'MN IRP'!E33)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>SUM(BPMCCS!F7,Sheet1!F33)</f>
+        <f>SUM(BPMCCS!F7,'MN IRP'!F33)</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>SUM(BPMCCS!G7,Sheet1!G33)</f>
+        <f>SUM(BPMCCS!G7,'MN IRP'!G33)</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f>SUM(BPMCCS!H7,Sheet1!H33)</f>
+        <f>SUM(BPMCCS!H7,'MN IRP'!H33)</f>
         <v>450</v>
       </c>
       <c r="K7">
-        <f>SUM(BPMCCS!I7,Sheet1!I33)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!I7,'MN IRP'!I33)</f>
+        <v>710</v>
       </c>
       <c r="L7">
-        <f>SUM(BPMCCS!J7,Sheet1!J33)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!J7,'MN IRP'!J33)</f>
+        <v>710</v>
       </c>
       <c r="M7">
-        <f>SUM(BPMCCS!K7,Sheet1!K33)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!K7,'MN IRP'!K33)</f>
+        <v>710</v>
       </c>
       <c r="N7">
-        <f>SUM(BPMCCS!L7,Sheet1!L33)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!L7,'MN IRP'!L33)</f>
+        <v>710</v>
       </c>
       <c r="O7">
-        <f>SUM(BPMCCS!M7,Sheet1!M33)</f>
-        <v>3550</v>
+        <f>SUM(BPMCCS!M7,'MN IRP'!M33)</f>
+        <v>710</v>
       </c>
       <c r="P7">
-        <f>SUM(BPMCCS!N7,Sheet1!N33)</f>
+        <f>SUM(BPMCCS!N7,'MN IRP'!N33)</f>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>SUM(BPMCCS!O7,Sheet1!O33)</f>
+        <f>SUM(BPMCCS!O7,'MN IRP'!O33)</f>
         <v>0</v>
       </c>
       <c r="R7">
-        <f>SUM(BPMCCS!P7,Sheet1!P33)</f>
+        <f>SUM(BPMCCS!P7,'MN IRP'!P33)</f>
         <v>0</v>
       </c>
       <c r="S7">
-        <f>SUM(BPMCCS!Q7,Sheet1!Q33)</f>
+        <f>SUM(BPMCCS!Q7,'MN IRP'!Q33)</f>
         <v>0</v>
       </c>
       <c r="T7">
-        <f>SUM(BPMCCS!R7,Sheet1!R33)</f>
+        <f>SUM(BPMCCS!R7,'MN IRP'!R33)</f>
         <v>0</v>
       </c>
       <c r="U7">
-        <f>SUM(BPMCCS!S7,Sheet1!S33)</f>
+        <f>SUM(BPMCCS!S7,'MN IRP'!S33)</f>
         <v>0</v>
       </c>
       <c r="V7">
-        <f>SUM(BPMCCS!T7,Sheet1!T33)</f>
+        <f>SUM(BPMCCS!T7,'MN IRP'!T33)</f>
         <v>0</v>
       </c>
       <c r="W7">
-        <f>SUM(BPMCCS!U7,Sheet1!U33)</f>
+        <f>SUM(BPMCCS!U7,'MN IRP'!U33)</f>
         <v>0</v>
       </c>
       <c r="X7">
-        <f>SUM(BPMCCS!V7,Sheet1!V33)</f>
+        <f>SUM(BPMCCS!V7,'MN IRP'!V33)</f>
         <v>0</v>
       </c>
       <c r="Y7">
-        <f>SUM(BPMCCS!W7,Sheet1!W33)</f>
+        <f>SUM(BPMCCS!W7,'MN IRP'!W33)</f>
         <v>0</v>
       </c>
       <c r="Z7">
-        <f>SUM(BPMCCS!X7,Sheet1!X33)</f>
+        <f>SUM(BPMCCS!X7,'MN IRP'!X33)</f>
         <v>0</v>
       </c>
       <c r="AA7">
-        <f>SUM(BPMCCS!Y7,Sheet1!Y33)</f>
+        <f>SUM(BPMCCS!Y7,'MN IRP'!Y33)</f>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f>SUM(BPMCCS!Z7,Sheet1!Z33)</f>
+        <f>SUM(BPMCCS!Z7,'MN IRP'!Z33)</f>
         <v>0</v>
       </c>
       <c r="AC7">
-        <f>SUM(BPMCCS!AA7,Sheet1!AA33)</f>
+        <f>SUM(BPMCCS!AA7,'MN IRP'!AA33)</f>
         <v>0</v>
       </c>
       <c r="AD7">
-        <f>SUM(BPMCCS!AB7,Sheet1!AB33)</f>
+        <f>SUM(BPMCCS!AB7,'MN IRP'!AB33)</f>
         <v>0</v>
       </c>
       <c r="AE7">
-        <f>SUM(BPMCCS!AC7,Sheet1!AC33)</f>
+        <f>SUM(BPMCCS!AC7,'MN IRP'!AC33)</f>
         <v>0</v>
       </c>
       <c r="AF7">
-        <f>SUM(BPMCCS!AD7,Sheet1!AD33)</f>
+        <f>SUM(BPMCCS!AD7,'MN IRP'!AD33)</f>
         <v>0</v>
       </c>
       <c r="AG7">
-        <f>SUM(BPMCCS!AE7,Sheet1!AE33)</f>
+        <f>SUM(BPMCCS!AE7,'MN IRP'!AE33)</f>
         <v>0</v>
       </c>
       <c r="AH7">
-        <f>SUM(BPMCCS!AF7,Sheet1!AF33)</f>
+        <f>SUM(BPMCCS!AF7,'MN IRP'!AF33)</f>
         <v>0</v>
       </c>
       <c r="AI7">
-        <f>SUM(BPMCCS!AG7,Sheet1!AG33)</f>
+        <f>SUM(BPMCCS!AG7,'MN IRP'!AG33)</f>
         <v>0</v>
       </c>
     </row>
@@ -3731,131 +3813,131 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>SUM(BPMCCS!B8,Sheet1!B34)</f>
+        <f>SUM(BPMCCS!B8,'MN IRP'!B34)</f>
         <v>0</v>
       </c>
       <c r="E8">
-        <f>SUM(BPMCCS!C8,Sheet1!C34)</f>
+        <f>SUM(BPMCCS!C8,'MN IRP'!C34)</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>SUM(BPMCCS!D8,Sheet1!D34)</f>
+        <f>SUM(BPMCCS!D8,'MN IRP'!D34)</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUM(BPMCCS!E8,Sheet1!E34)</f>
+        <f>SUM(BPMCCS!E8,'MN IRP'!E34)</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>SUM(BPMCCS!F8,Sheet1!F34)</f>
+        <f>SUM(BPMCCS!F8,'MN IRP'!F34)</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>SUM(BPMCCS!G8,Sheet1!G34)</f>
+        <f>SUM(BPMCCS!G8,'MN IRP'!G34)</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>SUM(BPMCCS!H8,Sheet1!H34)</f>
+        <f>SUM(BPMCCS!H8,'MN IRP'!H34)</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>SUM(BPMCCS!I8,Sheet1!I34)</f>
+        <f>SUM(BPMCCS!I8,'MN IRP'!I34)</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>SUM(BPMCCS!J8,Sheet1!J34)</f>
+        <f>SUM(BPMCCS!J8,'MN IRP'!J34)</f>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>SUM(BPMCCS!K8,Sheet1!K34)</f>
+        <f>SUM(BPMCCS!K8,'MN IRP'!K34)</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>SUM(BPMCCS!L8,Sheet1!L34)</f>
+        <f>SUM(BPMCCS!L8,'MN IRP'!L34)</f>
         <v>0</v>
       </c>
       <c r="O8">
-        <f>SUM(BPMCCS!M8,Sheet1!M34)</f>
+        <f>SUM(BPMCCS!M8,'MN IRP'!M34)</f>
         <v>0</v>
       </c>
       <c r="P8">
-        <f>SUM(BPMCCS!N8,Sheet1!N34)</f>
+        <f>SUM(BPMCCS!N8,'MN IRP'!N34)</f>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>SUM(BPMCCS!O8,Sheet1!O34)</f>
+        <f>SUM(BPMCCS!O8,'MN IRP'!O34)</f>
         <v>0</v>
       </c>
       <c r="R8">
-        <f>SUM(BPMCCS!P8,Sheet1!P34)</f>
+        <f>SUM(BPMCCS!P8,'MN IRP'!P34)</f>
         <v>0</v>
       </c>
       <c r="S8">
-        <f>SUM(BPMCCS!Q8,Sheet1!Q34)</f>
+        <f>SUM(BPMCCS!Q8,'MN IRP'!Q34)</f>
         <v>0</v>
       </c>
       <c r="T8">
-        <f>SUM(BPMCCS!R8,Sheet1!R34)</f>
+        <f>SUM(BPMCCS!R8,'MN IRP'!R34)</f>
         <v>0</v>
       </c>
       <c r="U8">
-        <f>SUM(BPMCCS!S8,Sheet1!S34)</f>
+        <f>SUM(BPMCCS!S8,'MN IRP'!S34)</f>
         <v>0</v>
       </c>
       <c r="V8">
-        <f>SUM(BPMCCS!T8,Sheet1!T34)</f>
+        <f>SUM(BPMCCS!T8,'MN IRP'!T34)</f>
         <v>0</v>
       </c>
       <c r="W8">
-        <f>SUM(BPMCCS!U8,Sheet1!U34)</f>
+        <f>SUM(BPMCCS!U8,'MN IRP'!U34)</f>
         <v>0</v>
       </c>
       <c r="X8">
-        <f>SUM(BPMCCS!V8,Sheet1!V34)</f>
+        <f>SUM(BPMCCS!V8,'MN IRP'!V34)</f>
         <v>0</v>
       </c>
       <c r="Y8">
-        <f>SUM(BPMCCS!W8,Sheet1!W34)</f>
+        <f>SUM(BPMCCS!W8,'MN IRP'!W34)</f>
         <v>0</v>
       </c>
       <c r="Z8">
-        <f>SUM(BPMCCS!X8,Sheet1!X34)</f>
+        <f>SUM(BPMCCS!X8,'MN IRP'!X34)</f>
         <v>0</v>
       </c>
       <c r="AA8">
-        <f>SUM(BPMCCS!Y8,Sheet1!Y34)</f>
+        <f>SUM(BPMCCS!Y8,'MN IRP'!Y34)</f>
         <v>0</v>
       </c>
       <c r="AB8">
-        <f>SUM(BPMCCS!Z8,Sheet1!Z34)</f>
+        <f>SUM(BPMCCS!Z8,'MN IRP'!Z34)</f>
         <v>0</v>
       </c>
       <c r="AC8">
-        <f>SUM(BPMCCS!AA8,Sheet1!AA34)</f>
+        <f>SUM(BPMCCS!AA8,'MN IRP'!AA34)</f>
         <v>0</v>
       </c>
       <c r="AD8">
-        <f>SUM(BPMCCS!AB8,Sheet1!AB34)</f>
+        <f>SUM(BPMCCS!AB8,'MN IRP'!AB34)</f>
         <v>0</v>
       </c>
       <c r="AE8">
-        <f>SUM(BPMCCS!AC8,Sheet1!AC34)</f>
+        <f>SUM(BPMCCS!AC8,'MN IRP'!AC34)</f>
         <v>0</v>
       </c>
       <c r="AF8">
-        <f>SUM(BPMCCS!AD8,Sheet1!AD34)</f>
+        <f>SUM(BPMCCS!AD8,'MN IRP'!AD34)</f>
         <v>0</v>
       </c>
       <c r="AG8">
-        <f>SUM(BPMCCS!AE8,Sheet1!AE34)</f>
+        <f>SUM(BPMCCS!AE8,'MN IRP'!AE34)</f>
         <v>0</v>
       </c>
       <c r="AH8">
-        <f>SUM(BPMCCS!AF8,Sheet1!AF34)</f>
+        <f>SUM(BPMCCS!AF8,'MN IRP'!AF34)</f>
         <v>0</v>
       </c>
       <c r="AI8">
-        <f>SUM(BPMCCS!AG8,Sheet1!AG34)</f>
+        <f>SUM(BPMCCS!AG8,'MN IRP'!AG34)</f>
         <v>0</v>
       </c>
     </row>
@@ -3870,131 +3952,131 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>SUM(BPMCCS!B9,Sheet1!B35)</f>
+        <f>SUM(BPMCCS!B9,'MN IRP'!B35)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>SUM(BPMCCS!C9,Sheet1!C35)</f>
+        <f>SUM(BPMCCS!C9,'MN IRP'!C35)</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>SUM(BPMCCS!D9,Sheet1!D35)</f>
+        <f>SUM(BPMCCS!D9,'MN IRP'!D35)</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>SUM(BPMCCS!E9,Sheet1!E35)</f>
+        <f>SUM(BPMCCS!E9,'MN IRP'!E35)</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>SUM(BPMCCS!F9,Sheet1!F35)</f>
+        <f>SUM(BPMCCS!F9,'MN IRP'!F35)</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>SUM(BPMCCS!G9,Sheet1!G35)</f>
+        <f>SUM(BPMCCS!G9,'MN IRP'!G35)</f>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>SUM(BPMCCS!H9,Sheet1!H35)</f>
+        <f>SUM(BPMCCS!H9,'MN IRP'!H35)</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>SUM(BPMCCS!I9,Sheet1!I35)</f>
+        <f>SUM(BPMCCS!I9,'MN IRP'!I35)</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f>SUM(BPMCCS!J9,Sheet1!J35)</f>
+        <f>SUM(BPMCCS!J9,'MN IRP'!J35)</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>SUM(BPMCCS!K9,Sheet1!K35)</f>
+        <f>SUM(BPMCCS!K9,'MN IRP'!K35)</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>SUM(BPMCCS!L9,Sheet1!L35)</f>
+        <f>SUM(BPMCCS!L9,'MN IRP'!L35)</f>
         <v>0</v>
       </c>
       <c r="O9">
-        <f>SUM(BPMCCS!M9,Sheet1!M35)</f>
+        <f>SUM(BPMCCS!M9,'MN IRP'!M35)</f>
         <v>0</v>
       </c>
       <c r="P9">
-        <f>SUM(BPMCCS!N9,Sheet1!N35)</f>
+        <f>SUM(BPMCCS!N9,'MN IRP'!N35)</f>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>SUM(BPMCCS!O9,Sheet1!O35)</f>
+        <f>SUM(BPMCCS!O9,'MN IRP'!O35)</f>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>SUM(BPMCCS!P9,Sheet1!P35)</f>
+        <f>SUM(BPMCCS!P9,'MN IRP'!P35)</f>
         <v>0</v>
       </c>
       <c r="S9">
-        <f>SUM(BPMCCS!Q9,Sheet1!Q35)</f>
+        <f>SUM(BPMCCS!Q9,'MN IRP'!Q35)</f>
         <v>0</v>
       </c>
       <c r="T9">
-        <f>SUM(BPMCCS!R9,Sheet1!R35)</f>
+        <f>SUM(BPMCCS!R9,'MN IRP'!R35)</f>
         <v>0</v>
       </c>
       <c r="U9">
-        <f>SUM(BPMCCS!S9,Sheet1!S35)</f>
+        <f>SUM(BPMCCS!S9,'MN IRP'!S35)</f>
         <v>0</v>
       </c>
       <c r="V9">
-        <f>SUM(BPMCCS!T9,Sheet1!T35)</f>
+        <f>SUM(BPMCCS!T9,'MN IRP'!T35)</f>
         <v>0</v>
       </c>
       <c r="W9">
-        <f>SUM(BPMCCS!U9,Sheet1!U35)</f>
+        <f>SUM(BPMCCS!U9,'MN IRP'!U35)</f>
         <v>0</v>
       </c>
       <c r="X9">
-        <f>SUM(BPMCCS!V9,Sheet1!V35)</f>
+        <f>SUM(BPMCCS!V9,'MN IRP'!V35)</f>
         <v>0</v>
       </c>
       <c r="Y9">
-        <f>SUM(BPMCCS!W9,Sheet1!W35)</f>
+        <f>SUM(BPMCCS!W9,'MN IRP'!W35)</f>
         <v>0</v>
       </c>
       <c r="Z9">
-        <f>SUM(BPMCCS!X9,Sheet1!X35)</f>
+        <f>SUM(BPMCCS!X9,'MN IRP'!X35)</f>
         <v>0</v>
       </c>
       <c r="AA9">
-        <f>SUM(BPMCCS!Y9,Sheet1!Y35)</f>
+        <f>SUM(BPMCCS!Y9,'MN IRP'!Y35)</f>
         <v>0</v>
       </c>
       <c r="AB9">
-        <f>SUM(BPMCCS!Z9,Sheet1!Z35)</f>
+        <f>SUM(BPMCCS!Z9,'MN IRP'!Z35)</f>
         <v>0</v>
       </c>
       <c r="AC9">
-        <f>SUM(BPMCCS!AA9,Sheet1!AA35)</f>
+        <f>SUM(BPMCCS!AA9,'MN IRP'!AA35)</f>
         <v>0</v>
       </c>
       <c r="AD9">
-        <f>SUM(BPMCCS!AB9,Sheet1!AB35)</f>
+        <f>SUM(BPMCCS!AB9,'MN IRP'!AB35)</f>
         <v>0</v>
       </c>
       <c r="AE9">
-        <f>SUM(BPMCCS!AC9,Sheet1!AC35)</f>
+        <f>SUM(BPMCCS!AC9,'MN IRP'!AC35)</f>
         <v>0</v>
       </c>
       <c r="AF9">
-        <f>SUM(BPMCCS!AD9,Sheet1!AD35)</f>
+        <f>SUM(BPMCCS!AD9,'MN IRP'!AD35)</f>
         <v>0</v>
       </c>
       <c r="AG9">
-        <f>SUM(BPMCCS!AE9,Sheet1!AE35)</f>
+        <f>SUM(BPMCCS!AE9,'MN IRP'!AE35)</f>
         <v>0</v>
       </c>
       <c r="AH9">
-        <f>SUM(BPMCCS!AF9,Sheet1!AF35)</f>
+        <f>SUM(BPMCCS!AF9,'MN IRP'!AF35)</f>
         <v>0</v>
       </c>
       <c r="AI9">
-        <f>SUM(BPMCCS!AG9,Sheet1!AG35)</f>
+        <f>SUM(BPMCCS!AG9,'MN IRP'!AG35)</f>
         <v>0</v>
       </c>
     </row>
@@ -4009,131 +4091,131 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>SUM(BPMCCS!B10,Sheet1!B36)</f>
+        <f>SUM(BPMCCS!B10,'MN IRP'!B36)</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>SUM(BPMCCS!C10,Sheet1!C36)</f>
+        <f>SUM(BPMCCS!C10,'MN IRP'!C36)</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>SUM(BPMCCS!D10,Sheet1!D36)</f>
+        <f>SUM(BPMCCS!D10,'MN IRP'!D36)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUM(BPMCCS!E10,Sheet1!E36)</f>
+        <f>SUM(BPMCCS!E10,'MN IRP'!E36)</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>SUM(BPMCCS!F10,Sheet1!F36)</f>
+        <f>SUM(BPMCCS!F10,'MN IRP'!F36)</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>SUM(BPMCCS!G10,Sheet1!G36)</f>
+        <f>SUM(BPMCCS!G10,'MN IRP'!G36)</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>SUM(BPMCCS!H10,Sheet1!H36)</f>
+        <f>SUM(BPMCCS!H10,'MN IRP'!H36)</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>SUM(BPMCCS!I10,Sheet1!I36)</f>
+        <f>SUM(BPMCCS!I10,'MN IRP'!I36)</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>SUM(BPMCCS!J10,Sheet1!J36)</f>
+        <f>SUM(BPMCCS!J10,'MN IRP'!J36)</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>SUM(BPMCCS!K10,Sheet1!K36)</f>
+        <f>SUM(BPMCCS!K10,'MN IRP'!K36)</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>SUM(BPMCCS!L10,Sheet1!L36)</f>
+        <f>SUM(BPMCCS!L10,'MN IRP'!L36)</f>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>SUM(BPMCCS!M10,Sheet1!M36)</f>
+        <f>SUM(BPMCCS!M10,'MN IRP'!M36)</f>
         <v>0</v>
       </c>
       <c r="P10">
-        <f>SUM(BPMCCS!N10,Sheet1!N36)</f>
+        <f>SUM(BPMCCS!N10,'MN IRP'!N36)</f>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>SUM(BPMCCS!O10,Sheet1!O36)</f>
+        <f>SUM(BPMCCS!O10,'MN IRP'!O36)</f>
         <v>0</v>
       </c>
       <c r="R10">
-        <f>SUM(BPMCCS!P10,Sheet1!P36)</f>
+        <f>SUM(BPMCCS!P10,'MN IRP'!P36)</f>
         <v>0</v>
       </c>
       <c r="S10">
-        <f>SUM(BPMCCS!Q10,Sheet1!Q36)</f>
+        <f>SUM(BPMCCS!Q10,'MN IRP'!Q36)</f>
         <v>0</v>
       </c>
       <c r="T10">
-        <f>SUM(BPMCCS!R10,Sheet1!R36)</f>
+        <f>SUM(BPMCCS!R10,'MN IRP'!R36)</f>
         <v>0</v>
       </c>
       <c r="U10">
-        <f>SUM(BPMCCS!S10,Sheet1!S36)</f>
+        <f>SUM(BPMCCS!S10,'MN IRP'!S36)</f>
         <v>0</v>
       </c>
       <c r="V10">
-        <f>SUM(BPMCCS!T10,Sheet1!T36)</f>
+        <f>SUM(BPMCCS!T10,'MN IRP'!T36)</f>
         <v>0</v>
       </c>
       <c r="W10">
-        <f>SUM(BPMCCS!U10,Sheet1!U36)</f>
+        <f>SUM(BPMCCS!U10,'MN IRP'!U36)</f>
         <v>0</v>
       </c>
       <c r="X10">
-        <f>SUM(BPMCCS!V10,Sheet1!V36)</f>
+        <f>SUM(BPMCCS!V10,'MN IRP'!V36)</f>
         <v>0</v>
       </c>
       <c r="Y10">
-        <f>SUM(BPMCCS!W10,Sheet1!W36)</f>
+        <f>SUM(BPMCCS!W10,'MN IRP'!W36)</f>
         <v>0</v>
       </c>
       <c r="Z10">
-        <f>SUM(BPMCCS!X10,Sheet1!X36)</f>
+        <f>SUM(BPMCCS!X10,'MN IRP'!X36)</f>
         <v>0</v>
       </c>
       <c r="AA10">
-        <f>SUM(BPMCCS!Y10,Sheet1!Y36)</f>
+        <f>SUM(BPMCCS!Y10,'MN IRP'!Y36)</f>
         <v>0</v>
       </c>
       <c r="AB10">
-        <f>SUM(BPMCCS!Z10,Sheet1!Z36)</f>
+        <f>SUM(BPMCCS!Z10,'MN IRP'!Z36)</f>
         <v>0</v>
       </c>
       <c r="AC10">
-        <f>SUM(BPMCCS!AA10,Sheet1!AA36)</f>
+        <f>SUM(BPMCCS!AA10,'MN IRP'!AA36)</f>
         <v>0</v>
       </c>
       <c r="AD10">
-        <f>SUM(BPMCCS!AB10,Sheet1!AB36)</f>
+        <f>SUM(BPMCCS!AB10,'MN IRP'!AB36)</f>
         <v>0</v>
       </c>
       <c r="AE10">
-        <f>SUM(BPMCCS!AC10,Sheet1!AC36)</f>
+        <f>SUM(BPMCCS!AC10,'MN IRP'!AC36)</f>
         <v>0</v>
       </c>
       <c r="AF10">
-        <f>SUM(BPMCCS!AD10,Sheet1!AD36)</f>
+        <f>SUM(BPMCCS!AD10,'MN IRP'!AD36)</f>
         <v>0</v>
       </c>
       <c r="AG10">
-        <f>SUM(BPMCCS!AE10,Sheet1!AE36)</f>
+        <f>SUM(BPMCCS!AE10,'MN IRP'!AE36)</f>
         <v>0</v>
       </c>
       <c r="AH10">
-        <f>SUM(BPMCCS!AF10,Sheet1!AF36)</f>
+        <f>SUM(BPMCCS!AF10,'MN IRP'!AF36)</f>
         <v>0</v>
       </c>
       <c r="AI10">
-        <f>SUM(BPMCCS!AG10,Sheet1!AG36)</f>
+        <f>SUM(BPMCCS!AG10,'MN IRP'!AG36)</f>
         <v>0</v>
       </c>
     </row>
@@ -4148,131 +4230,131 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>SUM(BPMCCS!B11,Sheet1!B37)</f>
+        <f>SUM(BPMCCS!B11,'MN IRP'!B37)</f>
         <v>0</v>
       </c>
       <c r="E11">
-        <f>SUM(BPMCCS!C11,Sheet1!C37)</f>
+        <f>SUM(BPMCCS!C11,'MN IRP'!C37)</f>
         <v>0</v>
       </c>
       <c r="F11">
-        <f>SUM(BPMCCS!D11,Sheet1!D37)</f>
+        <f>SUM(BPMCCS!D11,'MN IRP'!D37)</f>
         <v>0</v>
       </c>
       <c r="G11">
-        <f>SUM(BPMCCS!E11,Sheet1!E37)</f>
+        <f>SUM(BPMCCS!E11,'MN IRP'!E37)</f>
         <v>0</v>
       </c>
       <c r="H11">
-        <f>SUM(BPMCCS!F11,Sheet1!F37)</f>
+        <f>SUM(BPMCCS!F11,'MN IRP'!F37)</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f>SUM(BPMCCS!G11,Sheet1!G37)</f>
+        <f>SUM(BPMCCS!G11,'MN IRP'!G37)</f>
         <v>0</v>
       </c>
       <c r="J11">
-        <f>SUM(BPMCCS!H11,Sheet1!H37)</f>
+        <f>SUM(BPMCCS!H11,'MN IRP'!H37)</f>
         <v>0</v>
       </c>
       <c r="K11">
-        <f>SUM(BPMCCS!I11,Sheet1!I37)</f>
+        <f>SUM(BPMCCS!I11,'MN IRP'!I37)</f>
         <v>0</v>
       </c>
       <c r="L11">
-        <f>SUM(BPMCCS!J11,Sheet1!J37)</f>
+        <f>SUM(BPMCCS!J11,'MN IRP'!J37)</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>SUM(BPMCCS!K11,Sheet1!K37)</f>
+        <f>SUM(BPMCCS!K11,'MN IRP'!K37)</f>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>SUM(BPMCCS!L11,Sheet1!L37)</f>
+        <f>SUM(BPMCCS!L11,'MN IRP'!L37)</f>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>SUM(BPMCCS!M11,Sheet1!M37)</f>
+        <f>SUM(BPMCCS!M11,'MN IRP'!M37)</f>
         <v>0</v>
       </c>
       <c r="P11">
-        <f>SUM(BPMCCS!N11,Sheet1!N37)</f>
+        <f>SUM(BPMCCS!N11,'MN IRP'!N37)</f>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>SUM(BPMCCS!O11,Sheet1!O37)</f>
+        <f>SUM(BPMCCS!O11,'MN IRP'!O37)</f>
         <v>0</v>
       </c>
       <c r="R11">
-        <f>SUM(BPMCCS!P11,Sheet1!P37)</f>
+        <f>SUM(BPMCCS!P11,'MN IRP'!P37)</f>
         <v>0</v>
       </c>
       <c r="S11">
-        <f>SUM(BPMCCS!Q11,Sheet1!Q37)</f>
+        <f>SUM(BPMCCS!Q11,'MN IRP'!Q37)</f>
         <v>0</v>
       </c>
       <c r="T11">
-        <f>SUM(BPMCCS!R11,Sheet1!R37)</f>
+        <f>SUM(BPMCCS!R11,'MN IRP'!R37)</f>
         <v>0</v>
       </c>
       <c r="U11">
-        <f>SUM(BPMCCS!S11,Sheet1!S37)</f>
+        <f>SUM(BPMCCS!S11,'MN IRP'!S37)</f>
         <v>0</v>
       </c>
       <c r="V11">
-        <f>SUM(BPMCCS!T11,Sheet1!T37)</f>
+        <f>SUM(BPMCCS!T11,'MN IRP'!T37)</f>
         <v>0</v>
       </c>
       <c r="W11">
-        <f>SUM(BPMCCS!U11,Sheet1!U37)</f>
+        <f>SUM(BPMCCS!U11,'MN IRP'!U37)</f>
         <v>0</v>
       </c>
       <c r="X11">
-        <f>SUM(BPMCCS!V11,Sheet1!V37)</f>
+        <f>SUM(BPMCCS!V11,'MN IRP'!V37)</f>
         <v>0</v>
       </c>
       <c r="Y11">
-        <f>SUM(BPMCCS!W11,Sheet1!W37)</f>
+        <f>SUM(BPMCCS!W11,'MN IRP'!W37)</f>
         <v>0</v>
       </c>
       <c r="Z11">
-        <f>SUM(BPMCCS!X11,Sheet1!X37)</f>
+        <f>SUM(BPMCCS!X11,'MN IRP'!X37)</f>
         <v>0</v>
       </c>
       <c r="AA11">
-        <f>SUM(BPMCCS!Y11,Sheet1!Y37)</f>
+        <f>SUM(BPMCCS!Y11,'MN IRP'!Y37)</f>
         <v>0</v>
       </c>
       <c r="AB11">
-        <f>SUM(BPMCCS!Z11,Sheet1!Z37)</f>
+        <f>SUM(BPMCCS!Z11,'MN IRP'!Z37)</f>
         <v>0</v>
       </c>
       <c r="AC11">
-        <f>SUM(BPMCCS!AA11,Sheet1!AA37)</f>
+        <f>SUM(BPMCCS!AA11,'MN IRP'!AA37)</f>
         <v>0</v>
       </c>
       <c r="AD11">
-        <f>SUM(BPMCCS!AB11,Sheet1!AB37)</f>
+        <f>SUM(BPMCCS!AB11,'MN IRP'!AB37)</f>
         <v>0</v>
       </c>
       <c r="AE11">
-        <f>SUM(BPMCCS!AC11,Sheet1!AC37)</f>
+        <f>SUM(BPMCCS!AC11,'MN IRP'!AC37)</f>
         <v>0</v>
       </c>
       <c r="AF11">
-        <f>SUM(BPMCCS!AD11,Sheet1!AD37)</f>
+        <f>SUM(BPMCCS!AD11,'MN IRP'!AD37)</f>
         <v>0</v>
       </c>
       <c r="AG11">
-        <f>SUM(BPMCCS!AE11,Sheet1!AE37)</f>
+        <f>SUM(BPMCCS!AE11,'MN IRP'!AE37)</f>
         <v>0</v>
       </c>
       <c r="AH11">
-        <f>SUM(BPMCCS!AF11,Sheet1!AF37)</f>
+        <f>SUM(BPMCCS!AF11,'MN IRP'!AF37)</f>
         <v>0</v>
       </c>
       <c r="AI11">
-        <f>SUM(BPMCCS!AG11,Sheet1!AG37)</f>
+        <f>SUM(BPMCCS!AG11,'MN IRP'!AG37)</f>
         <v>0</v>
       </c>
     </row>
@@ -4287,131 +4369,131 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>SUM(BPMCCS!B12,Sheet1!B38)</f>
+        <f>SUM(BPMCCS!B12,'MN IRP'!B38)</f>
         <v>0</v>
       </c>
       <c r="E12">
-        <f>SUM(BPMCCS!C12,Sheet1!C38)</f>
+        <f>SUM(BPMCCS!C12,'MN IRP'!C38)</f>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>SUM(BPMCCS!D12,Sheet1!D38)</f>
+        <f>SUM(BPMCCS!D12,'MN IRP'!D38)</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <f>SUM(BPMCCS!E12,Sheet1!E38)</f>
+        <f>SUM(BPMCCS!E12,'MN IRP'!E38)</f>
         <v>0</v>
       </c>
       <c r="H12">
-        <f>SUM(BPMCCS!F12,Sheet1!F38)</f>
+        <f>SUM(BPMCCS!F12,'MN IRP'!F38)</f>
         <v>0</v>
       </c>
       <c r="I12">
-        <f>SUM(BPMCCS!G12,Sheet1!G38)</f>
+        <f>SUM(BPMCCS!G12,'MN IRP'!G38)</f>
         <v>0</v>
       </c>
       <c r="J12">
-        <f>SUM(BPMCCS!H12,Sheet1!H38)</f>
+        <f>SUM(BPMCCS!H12,'MN IRP'!H38)</f>
         <v>0</v>
       </c>
       <c r="K12">
-        <f>SUM(BPMCCS!I12,Sheet1!I38)</f>
+        <f>SUM(BPMCCS!I12,'MN IRP'!I38)</f>
         <v>0</v>
       </c>
       <c r="L12">
-        <f>SUM(BPMCCS!J12,Sheet1!J38)</f>
+        <f>SUM(BPMCCS!J12,'MN IRP'!J38)</f>
         <v>0</v>
       </c>
       <c r="M12">
-        <f>SUM(BPMCCS!K12,Sheet1!K38)</f>
+        <f>SUM(BPMCCS!K12,'MN IRP'!K38)</f>
         <v>0</v>
       </c>
       <c r="N12">
-        <f>SUM(BPMCCS!L12,Sheet1!L38)</f>
+        <f>SUM(BPMCCS!L12,'MN IRP'!L38)</f>
         <v>0</v>
       </c>
       <c r="O12">
-        <f>SUM(BPMCCS!M12,Sheet1!M38)</f>
+        <f>SUM(BPMCCS!M12,'MN IRP'!M38)</f>
         <v>0</v>
       </c>
       <c r="P12">
-        <f>SUM(BPMCCS!N12,Sheet1!N38)</f>
+        <f>SUM(BPMCCS!N12,'MN IRP'!N38)</f>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>SUM(BPMCCS!O12,Sheet1!O38)</f>
+        <f>SUM(BPMCCS!O12,'MN IRP'!O38)</f>
         <v>0</v>
       </c>
       <c r="R12">
-        <f>SUM(BPMCCS!P12,Sheet1!P38)</f>
+        <f>SUM(BPMCCS!P12,'MN IRP'!P38)</f>
         <v>0</v>
       </c>
       <c r="S12">
-        <f>SUM(BPMCCS!Q12,Sheet1!Q38)</f>
+        <f>SUM(BPMCCS!Q12,'MN IRP'!Q38)</f>
         <v>0</v>
       </c>
       <c r="T12">
-        <f>SUM(BPMCCS!R12,Sheet1!R38)</f>
+        <f>SUM(BPMCCS!R12,'MN IRP'!R38)</f>
         <v>0</v>
       </c>
       <c r="U12">
-        <f>SUM(BPMCCS!S12,Sheet1!S38)</f>
+        <f>SUM(BPMCCS!S12,'MN IRP'!S38)</f>
         <v>0</v>
       </c>
       <c r="V12">
-        <f>SUM(BPMCCS!T12,Sheet1!T38)</f>
+        <f>SUM(BPMCCS!T12,'MN IRP'!T38)</f>
         <v>0</v>
       </c>
       <c r="W12">
-        <f>SUM(BPMCCS!U12,Sheet1!U38)</f>
+        <f>SUM(BPMCCS!U12,'MN IRP'!U38)</f>
         <v>0</v>
       </c>
       <c r="X12">
-        <f>SUM(BPMCCS!V12,Sheet1!V38)</f>
+        <f>SUM(BPMCCS!V12,'MN IRP'!V38)</f>
         <v>0</v>
       </c>
       <c r="Y12">
-        <f>SUM(BPMCCS!W12,Sheet1!W38)</f>
+        <f>SUM(BPMCCS!W12,'MN IRP'!W38)</f>
         <v>0</v>
       </c>
       <c r="Z12">
-        <f>SUM(BPMCCS!X12,Sheet1!X38)</f>
+        <f>SUM(BPMCCS!X12,'MN IRP'!X38)</f>
         <v>0</v>
       </c>
       <c r="AA12">
-        <f>SUM(BPMCCS!Y12,Sheet1!Y38)</f>
+        <f>SUM(BPMCCS!Y12,'MN IRP'!Y38)</f>
         <v>0</v>
       </c>
       <c r="AB12">
-        <f>SUM(BPMCCS!Z12,Sheet1!Z38)</f>
+        <f>SUM(BPMCCS!Z12,'MN IRP'!Z38)</f>
         <v>0</v>
       </c>
       <c r="AC12">
-        <f>SUM(BPMCCS!AA12,Sheet1!AA38)</f>
+        <f>SUM(BPMCCS!AA12,'MN IRP'!AA38)</f>
         <v>0</v>
       </c>
       <c r="AD12">
-        <f>SUM(BPMCCS!AB12,Sheet1!AB38)</f>
+        <f>SUM(BPMCCS!AB12,'MN IRP'!AB38)</f>
         <v>0</v>
       </c>
       <c r="AE12">
-        <f>SUM(BPMCCS!AC12,Sheet1!AC38)</f>
+        <f>SUM(BPMCCS!AC12,'MN IRP'!AC38)</f>
         <v>0</v>
       </c>
       <c r="AF12">
-        <f>SUM(BPMCCS!AD12,Sheet1!AD38)</f>
+        <f>SUM(BPMCCS!AD12,'MN IRP'!AD38)</f>
         <v>0</v>
       </c>
       <c r="AG12">
-        <f>SUM(BPMCCS!AE12,Sheet1!AE38)</f>
+        <f>SUM(BPMCCS!AE12,'MN IRP'!AE38)</f>
         <v>0</v>
       </c>
       <c r="AH12">
-        <f>SUM(BPMCCS!AF12,Sheet1!AF38)</f>
+        <f>SUM(BPMCCS!AF12,'MN IRP'!AF38)</f>
         <v>0</v>
       </c>
       <c r="AI12">
-        <f>SUM(BPMCCS!AG12,Sheet1!AG38)</f>
+        <f>SUM(BPMCCS!AG12,'MN IRP'!AG38)</f>
         <v>0</v>
       </c>
     </row>
@@ -4426,131 +4508,131 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f>SUM(BPMCCS!B13,Sheet1!B39)</f>
+        <f>SUM(BPMCCS!B13,'MN IRP'!B39)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>SUM(BPMCCS!C13,Sheet1!C39)</f>
+        <f>SUM(BPMCCS!C13,'MN IRP'!C39)</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>SUM(BPMCCS!D13,Sheet1!D39)</f>
+        <f>SUM(BPMCCS!D13,'MN IRP'!D39)</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>SUM(BPMCCS!E13,Sheet1!E39)</f>
+        <f>SUM(BPMCCS!E13,'MN IRP'!E39)</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>SUM(BPMCCS!F13,Sheet1!F39)</f>
+        <f>SUM(BPMCCS!F13,'MN IRP'!F39)</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>SUM(BPMCCS!G13,Sheet1!G39)</f>
+        <f>SUM(BPMCCS!G13,'MN IRP'!G39)</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>SUM(BPMCCS!H13,Sheet1!H39)</f>
+        <f>SUM(BPMCCS!H13,'MN IRP'!H39)</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f>SUM(BPMCCS!I13,Sheet1!I39)</f>
+        <f>SUM(BPMCCS!I13,'MN IRP'!I39)</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f>SUM(BPMCCS!J13,Sheet1!J39)</f>
+        <f>SUM(BPMCCS!J13,'MN IRP'!J39)</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>SUM(BPMCCS!K13,Sheet1!K39)</f>
+        <f>SUM(BPMCCS!K13,'MN IRP'!K39)</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>SUM(BPMCCS!L13,Sheet1!L39)</f>
+        <f>SUM(BPMCCS!L13,'MN IRP'!L39)</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f>SUM(BPMCCS!M13,Sheet1!M39)</f>
+        <f>SUM(BPMCCS!M13,'MN IRP'!M39)</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>SUM(BPMCCS!N13,Sheet1!N39)</f>
+        <f>SUM(BPMCCS!N13,'MN IRP'!N39)</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>SUM(BPMCCS!O13,Sheet1!O39)</f>
+        <f>SUM(BPMCCS!O13,'MN IRP'!O39)</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>SUM(BPMCCS!P13,Sheet1!P39)</f>
+        <f>SUM(BPMCCS!P13,'MN IRP'!P39)</f>
         <v>0</v>
       </c>
       <c r="S13">
-        <f>SUM(BPMCCS!Q13,Sheet1!Q39)</f>
+        <f>SUM(BPMCCS!Q13,'MN IRP'!Q39)</f>
         <v>0</v>
       </c>
       <c r="T13">
-        <f>SUM(BPMCCS!R13,Sheet1!R39)</f>
+        <f>SUM(BPMCCS!R13,'MN IRP'!R39)</f>
         <v>0</v>
       </c>
       <c r="U13">
-        <f>SUM(BPMCCS!S13,Sheet1!S39)</f>
+        <f>SUM(BPMCCS!S13,'MN IRP'!S39)</f>
         <v>0</v>
       </c>
       <c r="V13">
-        <f>SUM(BPMCCS!T13,Sheet1!T39)</f>
+        <f>SUM(BPMCCS!T13,'MN IRP'!T39)</f>
         <v>0</v>
       </c>
       <c r="W13">
-        <f>SUM(BPMCCS!U13,Sheet1!U39)</f>
+        <f>SUM(BPMCCS!U13,'MN IRP'!U39)</f>
         <v>0</v>
       </c>
       <c r="X13">
-        <f>SUM(BPMCCS!V13,Sheet1!V39)</f>
+        <f>SUM(BPMCCS!V13,'MN IRP'!V39)</f>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f>SUM(BPMCCS!W13,Sheet1!W39)</f>
+        <f>SUM(BPMCCS!W13,'MN IRP'!W39)</f>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f>SUM(BPMCCS!X13,Sheet1!X39)</f>
+        <f>SUM(BPMCCS!X13,'MN IRP'!X39)</f>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f>SUM(BPMCCS!Y13,Sheet1!Y39)</f>
+        <f>SUM(BPMCCS!Y13,'MN IRP'!Y39)</f>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f>SUM(BPMCCS!Z13,Sheet1!Z39)</f>
+        <f>SUM(BPMCCS!Z13,'MN IRP'!Z39)</f>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f>SUM(BPMCCS!AA13,Sheet1!AA39)</f>
+        <f>SUM(BPMCCS!AA13,'MN IRP'!AA39)</f>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f>SUM(BPMCCS!AB13,Sheet1!AB39)</f>
+        <f>SUM(BPMCCS!AB13,'MN IRP'!AB39)</f>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f>SUM(BPMCCS!AC13,Sheet1!AC39)</f>
+        <f>SUM(BPMCCS!AC13,'MN IRP'!AC39)</f>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f>SUM(BPMCCS!AD13,Sheet1!AD39)</f>
+        <f>SUM(BPMCCS!AD13,'MN IRP'!AD39)</f>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f>SUM(BPMCCS!AE13,Sheet1!AE39)</f>
+        <f>SUM(BPMCCS!AE13,'MN IRP'!AE39)</f>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f>SUM(BPMCCS!AF13,Sheet1!AF39)</f>
+        <f>SUM(BPMCCS!AF13,'MN IRP'!AF39)</f>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f>SUM(BPMCCS!AG13,Sheet1!AG39)</f>
+        <f>SUM(BPMCCS!AG13,'MN IRP'!AG39)</f>
         <v>0</v>
       </c>
     </row>
@@ -4565,131 +4647,131 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>SUM(BPMCCS!B14,Sheet1!B40)</f>
+        <f>SUM(BPMCCS!B14,'MN IRP'!B40)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>SUM(BPMCCS!C14,Sheet1!C40)</f>
+        <f>SUM(BPMCCS!C14,'MN IRP'!C40)</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>SUM(BPMCCS!D14,Sheet1!D40)</f>
+        <f>SUM(BPMCCS!D14,'MN IRP'!D40)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>SUM(BPMCCS!E14,Sheet1!E40)</f>
+        <f>SUM(BPMCCS!E14,'MN IRP'!E40)</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f>SUM(BPMCCS!F14,Sheet1!F40)</f>
+        <f>SUM(BPMCCS!F14,'MN IRP'!F40)</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>SUM(BPMCCS!G14,Sheet1!G40)</f>
+        <f>SUM(BPMCCS!G14,'MN IRP'!G40)</f>
         <v>0</v>
       </c>
       <c r="J14">
-        <f>SUM(BPMCCS!H14,Sheet1!H40)</f>
+        <f>SUM(BPMCCS!H14,'MN IRP'!H40)</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>SUM(BPMCCS!I14,Sheet1!I40)</f>
+        <f>SUM(BPMCCS!I14,'MN IRP'!I40)</f>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>SUM(BPMCCS!J14,Sheet1!J40)</f>
+        <f>SUM(BPMCCS!J14,'MN IRP'!J40)</f>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>SUM(BPMCCS!K14,Sheet1!K40)</f>
+        <f>SUM(BPMCCS!K14,'MN IRP'!K40)</f>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>SUM(BPMCCS!L14,Sheet1!L40)</f>
+        <f>SUM(BPMCCS!L14,'MN IRP'!L40)</f>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>SUM(BPMCCS!M14,Sheet1!M40)</f>
+        <f>SUM(BPMCCS!M14,'MN IRP'!M40)</f>
         <v>0</v>
       </c>
       <c r="P14">
-        <f>SUM(BPMCCS!N14,Sheet1!N40)</f>
+        <f>SUM(BPMCCS!N14,'MN IRP'!N40)</f>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>SUM(BPMCCS!O14,Sheet1!O40)</f>
+        <f>SUM(BPMCCS!O14,'MN IRP'!O40)</f>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>SUM(BPMCCS!P14,Sheet1!P40)</f>
+        <f>SUM(BPMCCS!P14,'MN IRP'!P40)</f>
         <v>0</v>
       </c>
       <c r="S14">
-        <f>SUM(BPMCCS!Q14,Sheet1!Q40)</f>
+        <f>SUM(BPMCCS!Q14,'MN IRP'!Q40)</f>
         <v>0</v>
       </c>
       <c r="T14">
-        <f>SUM(BPMCCS!R14,Sheet1!R40)</f>
+        <f>SUM(BPMCCS!R14,'MN IRP'!R40)</f>
         <v>0</v>
       </c>
       <c r="U14">
-        <f>SUM(BPMCCS!S14,Sheet1!S40)</f>
+        <f>SUM(BPMCCS!S14,'MN IRP'!S40)</f>
         <v>0</v>
       </c>
       <c r="V14">
-        <f>SUM(BPMCCS!T14,Sheet1!T40)</f>
+        <f>SUM(BPMCCS!T14,'MN IRP'!T40)</f>
         <v>0</v>
       </c>
       <c r="W14">
-        <f>SUM(BPMCCS!U14,Sheet1!U40)</f>
+        <f>SUM(BPMCCS!U14,'MN IRP'!U40)</f>
         <v>0</v>
       </c>
       <c r="X14">
-        <f>SUM(BPMCCS!V14,Sheet1!V40)</f>
+        <f>SUM(BPMCCS!V14,'MN IRP'!V40)</f>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f>SUM(BPMCCS!W14,Sheet1!W40)</f>
+        <f>SUM(BPMCCS!W14,'MN IRP'!W40)</f>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f>SUM(BPMCCS!X14,Sheet1!X40)</f>
+        <f>SUM(BPMCCS!X14,'MN IRP'!X40)</f>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f>SUM(BPMCCS!Y14,Sheet1!Y40)</f>
+        <f>SUM(BPMCCS!Y14,'MN IRP'!Y40)</f>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f>SUM(BPMCCS!Z14,Sheet1!Z40)</f>
+        <f>SUM(BPMCCS!Z14,'MN IRP'!Z40)</f>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f>SUM(BPMCCS!AA14,Sheet1!AA40)</f>
+        <f>SUM(BPMCCS!AA14,'MN IRP'!AA40)</f>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f>SUM(BPMCCS!AB14,Sheet1!AB40)</f>
+        <f>SUM(BPMCCS!AB14,'MN IRP'!AB40)</f>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f>SUM(BPMCCS!AC14,Sheet1!AC40)</f>
+        <f>SUM(BPMCCS!AC14,'MN IRP'!AC40)</f>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f>SUM(BPMCCS!AD14,Sheet1!AD40)</f>
+        <f>SUM(BPMCCS!AD14,'MN IRP'!AD40)</f>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f>SUM(BPMCCS!AE14,Sheet1!AE40)</f>
+        <f>SUM(BPMCCS!AE14,'MN IRP'!AE40)</f>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f>SUM(BPMCCS!AF14,Sheet1!AF40)</f>
+        <f>SUM(BPMCCS!AF14,'MN IRP'!AF40)</f>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f>SUM(BPMCCS!AG14,Sheet1!AG40)</f>
+        <f>SUM(BPMCCS!AG14,'MN IRP'!AG40)</f>
         <v>0</v>
       </c>
     </row>
@@ -4704,131 +4786,131 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f>SUM(BPMCCS!B15,Sheet1!B41)</f>
+        <f>SUM(BPMCCS!B15,'MN IRP'!B41)</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>SUM(BPMCCS!C15,Sheet1!C41)</f>
+        <f>SUM(BPMCCS!C15,'MN IRP'!C41)</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>SUM(BPMCCS!D15,Sheet1!D41)</f>
+        <f>SUM(BPMCCS!D15,'MN IRP'!D41)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>SUM(BPMCCS!E15,Sheet1!E41)</f>
+        <f>SUM(BPMCCS!E15,'MN IRP'!E41)</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>SUM(BPMCCS!F15,Sheet1!F41)</f>
+        <f>SUM(BPMCCS!F15,'MN IRP'!F41)</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>SUM(BPMCCS!G15,Sheet1!G41)</f>
+        <f>SUM(BPMCCS!G15,'MN IRP'!G41)</f>
         <v>0</v>
       </c>
       <c r="J15">
-        <f>SUM(BPMCCS!H15,Sheet1!H41)</f>
+        <f>SUM(BPMCCS!H15,'MN IRP'!H41)</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>SUM(BPMCCS!I15,Sheet1!I41)</f>
+        <f>SUM(BPMCCS!I15,'MN IRP'!I41)</f>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>SUM(BPMCCS!J15,Sheet1!J41)</f>
+        <f>SUM(BPMCCS!J15,'MN IRP'!J41)</f>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>SUM(BPMCCS!K15,Sheet1!K41)</f>
+        <f>SUM(BPMCCS!K15,'MN IRP'!K41)</f>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>SUM(BPMCCS!L15,Sheet1!L41)</f>
+        <f>SUM(BPMCCS!L15,'MN IRP'!L41)</f>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>SUM(BPMCCS!M15,Sheet1!M41)</f>
+        <f>SUM(BPMCCS!M15,'MN IRP'!M41)</f>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>SUM(BPMCCS!N15,Sheet1!N41)</f>
+        <f>SUM(BPMCCS!N15,'MN IRP'!N41)</f>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>SUM(BPMCCS!O15,Sheet1!O41)</f>
+        <f>SUM(BPMCCS!O15,'MN IRP'!O41)</f>
         <v>0</v>
       </c>
       <c r="R15">
-        <f>SUM(BPMCCS!P15,Sheet1!P41)</f>
+        <f>SUM(BPMCCS!P15,'MN IRP'!P41)</f>
         <v>0</v>
       </c>
       <c r="S15">
-        <f>SUM(BPMCCS!Q15,Sheet1!Q41)</f>
+        <f>SUM(BPMCCS!Q15,'MN IRP'!Q41)</f>
         <v>0</v>
       </c>
       <c r="T15">
-        <f>SUM(BPMCCS!R15,Sheet1!R41)</f>
+        <f>SUM(BPMCCS!R15,'MN IRP'!R41)</f>
         <v>0</v>
       </c>
       <c r="U15">
-        <f>SUM(BPMCCS!S15,Sheet1!S41)</f>
+        <f>SUM(BPMCCS!S15,'MN IRP'!S41)</f>
         <v>0</v>
       </c>
       <c r="V15">
-        <f>SUM(BPMCCS!T15,Sheet1!T41)</f>
+        <f>SUM(BPMCCS!T15,'MN IRP'!T41)</f>
         <v>0</v>
       </c>
       <c r="W15">
-        <f>SUM(BPMCCS!U15,Sheet1!U41)</f>
+        <f>SUM(BPMCCS!U15,'MN IRP'!U41)</f>
         <v>0</v>
       </c>
       <c r="X15">
-        <f>SUM(BPMCCS!V15,Sheet1!V41)</f>
+        <f>SUM(BPMCCS!V15,'MN IRP'!V41)</f>
         <v>0</v>
       </c>
       <c r="Y15">
-        <f>SUM(BPMCCS!W15,Sheet1!W41)</f>
+        <f>SUM(BPMCCS!W15,'MN IRP'!W41)</f>
         <v>0</v>
       </c>
       <c r="Z15">
-        <f>SUM(BPMCCS!X15,Sheet1!X41)</f>
+        <f>SUM(BPMCCS!X15,'MN IRP'!X41)</f>
         <v>0</v>
       </c>
       <c r="AA15">
-        <f>SUM(BPMCCS!Y15,Sheet1!Y41)</f>
+        <f>SUM(BPMCCS!Y15,'MN IRP'!Y41)</f>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f>SUM(BPMCCS!Z15,Sheet1!Z41)</f>
+        <f>SUM(BPMCCS!Z15,'MN IRP'!Z41)</f>
         <v>0</v>
       </c>
       <c r="AC15">
-        <f>SUM(BPMCCS!AA15,Sheet1!AA41)</f>
+        <f>SUM(BPMCCS!AA15,'MN IRP'!AA41)</f>
         <v>0</v>
       </c>
       <c r="AD15">
-        <f>SUM(BPMCCS!AB15,Sheet1!AB41)</f>
+        <f>SUM(BPMCCS!AB15,'MN IRP'!AB41)</f>
         <v>0</v>
       </c>
       <c r="AE15">
-        <f>SUM(BPMCCS!AC15,Sheet1!AC41)</f>
+        <f>SUM(BPMCCS!AC15,'MN IRP'!AC41)</f>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f>SUM(BPMCCS!AD15,Sheet1!AD41)</f>
+        <f>SUM(BPMCCS!AD15,'MN IRP'!AD41)</f>
         <v>0</v>
       </c>
       <c r="AG15">
-        <f>SUM(BPMCCS!AE15,Sheet1!AE41)</f>
+        <f>SUM(BPMCCS!AE15,'MN IRP'!AE41)</f>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f>SUM(BPMCCS!AF15,Sheet1!AF41)</f>
+        <f>SUM(BPMCCS!AF15,'MN IRP'!AF41)</f>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f>SUM(BPMCCS!AG15,Sheet1!AG41)</f>
+        <f>SUM(BPMCCS!AG15,'MN IRP'!AG41)</f>
         <v>0</v>
       </c>
     </row>
@@ -4843,131 +4925,131 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f>SUM(BPMCCS!B16,Sheet1!B42)</f>
+        <f>SUM(BPMCCS!B16,'MN IRP'!B42)</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>SUM(BPMCCS!C16,Sheet1!C42)</f>
+        <f>SUM(BPMCCS!C16,'MN IRP'!C42)</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>SUM(BPMCCS!D16,Sheet1!D42)</f>
+        <f>SUM(BPMCCS!D16,'MN IRP'!D42)</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>SUM(BPMCCS!E16,Sheet1!E42)</f>
+        <f>SUM(BPMCCS!E16,'MN IRP'!E42)</f>
         <v>0</v>
       </c>
       <c r="H16">
-        <f>SUM(BPMCCS!F16,Sheet1!F42)</f>
+        <f>SUM(BPMCCS!F16,'MN IRP'!F42)</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>SUM(BPMCCS!G16,Sheet1!G42)</f>
+        <f>SUM(BPMCCS!G16,'MN IRP'!G42)</f>
         <v>0</v>
       </c>
       <c r="J16">
-        <f>SUM(BPMCCS!H16,Sheet1!H42)</f>
+        <f>SUM(BPMCCS!H16,'MN IRP'!H42)</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f>SUM(BPMCCS!I16,Sheet1!I42)</f>
+        <f>SUM(BPMCCS!I16,'MN IRP'!I42)</f>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>SUM(BPMCCS!J16,Sheet1!J42)</f>
+        <f>SUM(BPMCCS!J16,'MN IRP'!J42)</f>
         <v>0</v>
       </c>
       <c r="M16">
-        <f>SUM(BPMCCS!K16,Sheet1!K42)</f>
+        <f>SUM(BPMCCS!K16,'MN IRP'!K42)</f>
         <v>0</v>
       </c>
       <c r="N16">
-        <f>SUM(BPMCCS!L16,Sheet1!L42)</f>
+        <f>SUM(BPMCCS!L16,'MN IRP'!L42)</f>
         <v>0</v>
       </c>
       <c r="O16">
-        <f>SUM(BPMCCS!M16,Sheet1!M42)</f>
+        <f>SUM(BPMCCS!M16,'MN IRP'!M42)</f>
         <v>0</v>
       </c>
       <c r="P16">
-        <f>SUM(BPMCCS!N16,Sheet1!N42)</f>
+        <f>SUM(BPMCCS!N16,'MN IRP'!N42)</f>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>SUM(BPMCCS!O16,Sheet1!O42)</f>
+        <f>SUM(BPMCCS!O16,'MN IRP'!O42)</f>
         <v>0</v>
       </c>
       <c r="R16">
-        <f>SUM(BPMCCS!P16,Sheet1!P42)</f>
+        <f>SUM(BPMCCS!P16,'MN IRP'!P42)</f>
         <v>0</v>
       </c>
       <c r="S16">
-        <f>SUM(BPMCCS!Q16,Sheet1!Q42)</f>
+        <f>SUM(BPMCCS!Q16,'MN IRP'!Q42)</f>
         <v>0</v>
       </c>
       <c r="T16">
-        <f>SUM(BPMCCS!R16,Sheet1!R42)</f>
+        <f>SUM(BPMCCS!R16,'MN IRP'!R42)</f>
         <v>0</v>
       </c>
       <c r="U16">
-        <f>SUM(BPMCCS!S16,Sheet1!S42)</f>
+        <f>SUM(BPMCCS!S16,'MN IRP'!S42)</f>
         <v>0</v>
       </c>
       <c r="V16">
-        <f>SUM(BPMCCS!T16,Sheet1!T42)</f>
+        <f>SUM(BPMCCS!T16,'MN IRP'!T42)</f>
         <v>0</v>
       </c>
       <c r="W16">
-        <f>SUM(BPMCCS!U16,Sheet1!U42)</f>
+        <f>SUM(BPMCCS!U16,'MN IRP'!U42)</f>
         <v>0</v>
       </c>
       <c r="X16">
-        <f>SUM(BPMCCS!V16,Sheet1!V42)</f>
+        <f>SUM(BPMCCS!V16,'MN IRP'!V42)</f>
         <v>0</v>
       </c>
       <c r="Y16">
-        <f>SUM(BPMCCS!W16,Sheet1!W42)</f>
+        <f>SUM(BPMCCS!W16,'MN IRP'!W42)</f>
         <v>0</v>
       </c>
       <c r="Z16">
-        <f>SUM(BPMCCS!X16,Sheet1!X42)</f>
+        <f>SUM(BPMCCS!X16,'MN IRP'!X42)</f>
         <v>0</v>
       </c>
       <c r="AA16">
-        <f>SUM(BPMCCS!Y16,Sheet1!Y42)</f>
+        <f>SUM(BPMCCS!Y16,'MN IRP'!Y42)</f>
         <v>0</v>
       </c>
       <c r="AB16">
-        <f>SUM(BPMCCS!Z16,Sheet1!Z42)</f>
+        <f>SUM(BPMCCS!Z16,'MN IRP'!Z42)</f>
         <v>0</v>
       </c>
       <c r="AC16">
-        <f>SUM(BPMCCS!AA16,Sheet1!AA42)</f>
+        <f>SUM(BPMCCS!AA16,'MN IRP'!AA42)</f>
         <v>0</v>
       </c>
       <c r="AD16">
-        <f>SUM(BPMCCS!AB16,Sheet1!AB42)</f>
+        <f>SUM(BPMCCS!AB16,'MN IRP'!AB42)</f>
         <v>0</v>
       </c>
       <c r="AE16">
-        <f>SUM(BPMCCS!AC16,Sheet1!AC42)</f>
+        <f>SUM(BPMCCS!AC16,'MN IRP'!AC42)</f>
         <v>0</v>
       </c>
       <c r="AF16">
-        <f>SUM(BPMCCS!AD16,Sheet1!AD42)</f>
+        <f>SUM(BPMCCS!AD16,'MN IRP'!AD42)</f>
         <v>0</v>
       </c>
       <c r="AG16">
-        <f>SUM(BPMCCS!AE16,Sheet1!AE42)</f>
+        <f>SUM(BPMCCS!AE16,'MN IRP'!AE42)</f>
         <v>0</v>
       </c>
       <c r="AH16">
-        <f>SUM(BPMCCS!AF16,Sheet1!AF42)</f>
+        <f>SUM(BPMCCS!AF16,'MN IRP'!AF42)</f>
         <v>0</v>
       </c>
       <c r="AI16">
-        <f>SUM(BPMCCS!AG16,Sheet1!AG42)</f>
+        <f>SUM(BPMCCS!AG16,'MN IRP'!AG42)</f>
         <v>0</v>
       </c>
     </row>
@@ -4982,131 +5064,131 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f>SUM(BPMCCS!B17,Sheet1!B43)</f>
+        <f>SUM(BPMCCS!B17,'MN IRP'!B43)</f>
         <v>0</v>
       </c>
       <c r="E17">
-        <f>SUM(BPMCCS!C17,Sheet1!C43)</f>
+        <f>SUM(BPMCCS!C17,'MN IRP'!C43)</f>
         <v>0</v>
       </c>
       <c r="F17">
-        <f>SUM(BPMCCS!D17,Sheet1!D43)</f>
+        <f>SUM(BPMCCS!D17,'MN IRP'!D43)</f>
         <v>0</v>
       </c>
       <c r="G17">
-        <f>SUM(BPMCCS!E17,Sheet1!E43)</f>
+        <f>SUM(BPMCCS!E17,'MN IRP'!E43)</f>
         <v>0</v>
       </c>
       <c r="H17">
-        <f>SUM(BPMCCS!F17,Sheet1!F43)</f>
+        <f>SUM(BPMCCS!F17,'MN IRP'!F43)</f>
         <v>0</v>
       </c>
       <c r="I17">
-        <f>SUM(BPMCCS!G17,Sheet1!G43)</f>
+        <f>SUM(BPMCCS!G17,'MN IRP'!G43)</f>
         <v>0</v>
       </c>
       <c r="J17">
-        <f>SUM(BPMCCS!H17,Sheet1!H43)</f>
+        <f>SUM(BPMCCS!H17,'MN IRP'!H43)</f>
         <v>0</v>
       </c>
       <c r="K17">
-        <f>SUM(BPMCCS!I17,Sheet1!I43)</f>
+        <f>SUM(BPMCCS!I17,'MN IRP'!I43)</f>
         <v>0</v>
       </c>
       <c r="L17">
-        <f>SUM(BPMCCS!J17,Sheet1!J43)</f>
+        <f>SUM(BPMCCS!J17,'MN IRP'!J43)</f>
         <v>0</v>
       </c>
       <c r="M17">
-        <f>SUM(BPMCCS!K17,Sheet1!K43)</f>
+        <f>SUM(BPMCCS!K17,'MN IRP'!K43)</f>
         <v>0</v>
       </c>
       <c r="N17">
-        <f>SUM(BPMCCS!L17,Sheet1!L43)</f>
+        <f>SUM(BPMCCS!L17,'MN IRP'!L43)</f>
         <v>0</v>
       </c>
       <c r="O17">
-        <f>SUM(BPMCCS!M17,Sheet1!M43)</f>
+        <f>SUM(BPMCCS!M17,'MN IRP'!M43)</f>
         <v>0</v>
       </c>
       <c r="P17">
-        <f>SUM(BPMCCS!N17,Sheet1!N43)</f>
+        <f>SUM(BPMCCS!N17,'MN IRP'!N43)</f>
         <v>0</v>
       </c>
       <c r="Q17">
-        <f>SUM(BPMCCS!O17,Sheet1!O43)</f>
+        <f>SUM(BPMCCS!O17,'MN IRP'!O43)</f>
         <v>0</v>
       </c>
       <c r="R17">
-        <f>SUM(BPMCCS!P17,Sheet1!P43)</f>
+        <f>SUM(BPMCCS!P17,'MN IRP'!P43)</f>
         <v>0</v>
       </c>
       <c r="S17">
-        <f>SUM(BPMCCS!Q17,Sheet1!Q43)</f>
+        <f>SUM(BPMCCS!Q17,'MN IRP'!Q43)</f>
         <v>0</v>
       </c>
       <c r="T17">
-        <f>SUM(BPMCCS!R17,Sheet1!R43)</f>
+        <f>SUM(BPMCCS!R17,'MN IRP'!R43)</f>
         <v>0</v>
       </c>
       <c r="U17">
-        <f>SUM(BPMCCS!S17,Sheet1!S43)</f>
+        <f>SUM(BPMCCS!S17,'MN IRP'!S43)</f>
         <v>0</v>
       </c>
       <c r="V17">
-        <f>SUM(BPMCCS!T17,Sheet1!T43)</f>
+        <f>SUM(BPMCCS!T17,'MN IRP'!T43)</f>
         <v>0</v>
       </c>
       <c r="W17">
-        <f>SUM(BPMCCS!U17,Sheet1!U43)</f>
+        <f>SUM(BPMCCS!U17,'MN IRP'!U43)</f>
         <v>0</v>
       </c>
       <c r="X17">
-        <f>SUM(BPMCCS!V17,Sheet1!V43)</f>
+        <f>SUM(BPMCCS!V17,'MN IRP'!V43)</f>
         <v>0</v>
       </c>
       <c r="Y17">
-        <f>SUM(BPMCCS!W17,Sheet1!W43)</f>
+        <f>SUM(BPMCCS!W17,'MN IRP'!W43)</f>
         <v>0</v>
       </c>
       <c r="Z17">
-        <f>SUM(BPMCCS!X17,Sheet1!X43)</f>
+        <f>SUM(BPMCCS!X17,'MN IRP'!X43)</f>
         <v>0</v>
       </c>
       <c r="AA17">
-        <f>SUM(BPMCCS!Y17,Sheet1!Y43)</f>
+        <f>SUM(BPMCCS!Y17,'MN IRP'!Y43)</f>
         <v>0</v>
       </c>
       <c r="AB17">
-        <f>SUM(BPMCCS!Z17,Sheet1!Z43)</f>
+        <f>SUM(BPMCCS!Z17,'MN IRP'!Z43)</f>
         <v>0</v>
       </c>
       <c r="AC17">
-        <f>SUM(BPMCCS!AA17,Sheet1!AA43)</f>
+        <f>SUM(BPMCCS!AA17,'MN IRP'!AA43)</f>
         <v>0</v>
       </c>
       <c r="AD17">
-        <f>SUM(BPMCCS!AB17,Sheet1!AB43)</f>
+        <f>SUM(BPMCCS!AB17,'MN IRP'!AB43)</f>
         <v>0</v>
       </c>
       <c r="AE17">
-        <f>SUM(BPMCCS!AC17,Sheet1!AC43)</f>
+        <f>SUM(BPMCCS!AC17,'MN IRP'!AC43)</f>
         <v>0</v>
       </c>
       <c r="AF17">
-        <f>SUM(BPMCCS!AD17,Sheet1!AD43)</f>
+        <f>SUM(BPMCCS!AD17,'MN IRP'!AD43)</f>
         <v>0</v>
       </c>
       <c r="AG17">
-        <f>SUM(BPMCCS!AE17,Sheet1!AE43)</f>
+        <f>SUM(BPMCCS!AE17,'MN IRP'!AE43)</f>
         <v>0</v>
       </c>
       <c r="AH17">
-        <f>SUM(BPMCCS!AF17,Sheet1!AF43)</f>
+        <f>SUM(BPMCCS!AF17,'MN IRP'!AF43)</f>
         <v>0</v>
       </c>
       <c r="AI17">
-        <f>SUM(BPMCCS!AG17,Sheet1!AG43)</f>
+        <f>SUM(BPMCCS!AG17,'MN IRP'!AG43)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated reference scenario with Xcel IRP feedback
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Minnesota\MN_mod\InputData\elec\PMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FCD70C-5506-49AF-B266-C9EBE6F83EAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350912C-2B54-43D8-878F-2BDAD6FAE660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="480" windowWidth="24810" windowHeight="16350" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8460" yWindow="1635" windowWidth="19980" windowHeight="15225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -111,15 +111,6 @@
     <t>municipal solid waste</t>
   </si>
   <si>
-    <t>Xcel IRP</t>
-  </si>
-  <si>
-    <t>https://www.greentechmedia.com/articles/read/xcel-energy-accelerates-coal-plant-closures-to-meet-100-clean-energy-goal</t>
-  </si>
-  <si>
-    <t>https://www.xcelenergy.com/staticfiles/xe-responsive/Company/Rates%20&amp;%20Regulations/The-Resource-Plan-No-Appendices.pdf</t>
-  </si>
-  <si>
     <t>Additional capacity:</t>
   </si>
   <si>
@@ -135,16 +126,25 @@
     <t>Total</t>
   </si>
   <si>
-    <t>already have 1000 MW of solar</t>
-  </si>
-  <si>
-    <t>https://www.greentechmedia.com/articles/read/xcel-targets-1.4b-in-wind-solar-investments-outlines-broader-carbon-reduction-goals</t>
-  </si>
-  <si>
     <t>Mandated Construction (MW)</t>
   </si>
   <si>
     <t>per year</t>
+  </si>
+  <si>
+    <t>https://www.xcelenergy.com/staticfiles/xe-responsive/Company/Rates%20&amp;%20Regulations/Resource%20Plans/Upper-Midwest-Energy-Plan-Supplement-063020.PDF</t>
+  </si>
+  <si>
+    <t>Xcel IRP (2020)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Resources and Renewable Resources</t>
+  </si>
+  <si>
+    <t>NG CC</t>
+  </si>
+  <si>
+    <t>Sherco</t>
   </si>
 </sst>
 </file>
@@ -174,7 +174,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +184,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,13 +221,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,143 +246,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>129117</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>356850</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>82069</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B63054-7A12-430D-BE43-D031E4B40FDC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17316450" y="234950"/>
-          <a:ext cx="6979900" cy="3847619"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>589781</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161493</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEC915B4-35B8-4896-B271-1A35E886D8BA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10788650" y="279400"/>
-          <a:ext cx="6088881" cy="3501593"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>411692</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>115359</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>410929</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19883</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EAA7526-2650-4B17-B1FB-9A8D24EC0D87}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4708525" y="877359"/>
-          <a:ext cx="6137571" cy="1809524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,45 +621,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF686BE5-FC61-4D3A-AC20-612E5D71A1AB}">
-  <dimension ref="A1:AG46"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -800,316 +665,329 @@
         <v>2034</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4">
-        <v>450</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="4">
-        <f>4000-C9</f>
-        <v>3550</v>
+        <v>3500</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="5">
         <f>SUM(C9:E9)</f>
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="G9">
         <f>D9/(30-25)</f>
-        <v>710</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>700</v>
+      </c>
+      <c r="H9">
+        <f>SUM(I24:M24)</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="4">
-        <v>650</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4">
-        <f>1850-C10</f>
-        <v>1200</v>
+        <v>2250</v>
       </c>
       <c r="F10" s="5">
         <f>SUM(E10:E10)</f>
-        <v>1200</v>
+        <v>2250</v>
       </c>
       <c r="G10">
         <f>F10/(34-25)</f>
-        <v>133.33333333333334</v>
+        <v>250</v>
+      </c>
+      <c r="H10">
+        <f>SUM(I23:Q23)</f>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>800</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2019</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2021</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2022</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2023</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2024</v>
+      </c>
+      <c r="H18" s="7">
+        <v>2025</v>
+      </c>
+      <c r="I18" s="7">
+        <v>2026</v>
+      </c>
+      <c r="J18" s="7">
+        <v>2027</v>
+      </c>
+      <c r="K18" s="7">
+        <v>2028</v>
+      </c>
+      <c r="L18" s="7">
+        <v>2029</v>
+      </c>
+      <c r="M18" s="7">
+        <v>2030</v>
+      </c>
+      <c r="N18" s="7">
+        <v>2031</v>
+      </c>
+      <c r="O18" s="7">
+        <v>2032</v>
+      </c>
+      <c r="P18" s="7">
+        <v>2033</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>2034</v>
+      </c>
+      <c r="R18" s="7">
+        <v>2035</v>
+      </c>
+      <c r="S18" s="7">
+        <v>2036</v>
+      </c>
+      <c r="T18" s="7">
+        <v>2037</v>
+      </c>
+      <c r="U18" s="7">
+        <v>2038</v>
+      </c>
+      <c r="V18" s="7">
+        <v>2039</v>
+      </c>
+      <c r="W18" s="7">
+        <v>2040</v>
+      </c>
+      <c r="X18" s="7">
+        <v>2041</v>
+      </c>
+      <c r="Y18" s="7">
+        <v>2042</v>
+      </c>
+      <c r="Z18" s="7">
+        <v>2043</v>
+      </c>
+      <c r="AA18" s="7">
+        <v>2044</v>
+      </c>
+      <c r="AB18" s="7">
+        <v>2045</v>
+      </c>
+      <c r="AC18" s="7">
+        <v>2046</v>
+      </c>
+      <c r="AD18" s="7">
+        <v>2047</v>
+      </c>
+      <c r="AE18" s="7">
+        <v>2048</v>
+      </c>
+      <c r="AF18" s="7">
+        <v>2049</v>
+      </c>
+      <c r="AG18" s="7">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <f>C14</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23">
+        <f>$G$10</f>
+        <v>250</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:Q23" si="0">$G$10</f>
+        <v>250</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24">
+        <f>$G$9</f>
+        <v>700</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:M24" si="1">$G$9</f>
+        <v>700</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27">
-        <v>2019</v>
-      </c>
-      <c r="C27">
-        <v>2020</v>
-      </c>
-      <c r="D27">
-        <v>2021</v>
-      </c>
-      <c r="E27">
-        <v>2022</v>
-      </c>
-      <c r="F27">
-        <v>2023</v>
-      </c>
-      <c r="G27">
-        <v>2024</v>
-      </c>
-      <c r="H27">
-        <v>2025</v>
-      </c>
-      <c r="I27">
-        <v>2026</v>
-      </c>
-      <c r="J27">
-        <v>2027</v>
-      </c>
-      <c r="K27">
-        <v>2028</v>
-      </c>
-      <c r="L27">
-        <v>2029</v>
-      </c>
-      <c r="M27">
-        <v>2030</v>
-      </c>
-      <c r="N27">
-        <v>2031</v>
-      </c>
-      <c r="O27">
-        <v>2032</v>
-      </c>
-      <c r="P27">
-        <v>2033</v>
-      </c>
-      <c r="Q27">
-        <v>2034</v>
-      </c>
-      <c r="R27">
-        <v>2035</v>
-      </c>
-      <c r="S27">
-        <v>2036</v>
-      </c>
-      <c r="T27">
-        <v>2037</v>
-      </c>
-      <c r="U27">
-        <v>2038</v>
-      </c>
-      <c r="V27">
-        <v>2039</v>
-      </c>
-      <c r="W27">
-        <v>2040</v>
-      </c>
-      <c r="X27">
-        <v>2041</v>
-      </c>
-      <c r="Y27">
-        <v>2042</v>
-      </c>
-      <c r="Z27">
-        <v>2043</v>
-      </c>
-      <c r="AA27">
-        <v>2044</v>
-      </c>
-      <c r="AB27">
-        <v>2045</v>
-      </c>
-      <c r="AC27">
-        <v>2046</v>
-      </c>
-      <c r="AD27">
-        <v>2047</v>
-      </c>
-      <c r="AE27">
-        <v>2048</v>
-      </c>
-      <c r="AF27">
-        <v>2049</v>
-      </c>
-      <c r="AG27">
-        <v>2050</v>
+      <c r="A27" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>9</v>
+      <c r="A28" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>10</v>
+      <c r="A29" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32">
-        <f>C10</f>
-        <v>650</v>
-      </c>
-      <c r="I32">
-        <f>$G$10</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="J32">
-        <f t="shared" ref="J32:Q32" si="0">$G$10</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="0"/>
-        <v>133.33333333333334</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33">
-        <f>C9</f>
-        <v>450</v>
-      </c>
-      <c r="I33">
-        <f>$G$9</f>
-        <v>710</v>
-      </c>
-      <c r="J33">
-        <f t="shared" ref="J33:M33" si="1">$G$9</f>
-        <v>710</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="1"/>
-        <v>710</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="1"/>
-        <v>710</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="1"/>
-        <v>710</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="31" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J46" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1122,10 +1000,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1">
         <v>2019</v>
@@ -2853,7 +2734,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,131 +2860,131 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>SUM(BPMCCS!B2,'MN IRP'!B28)</f>
+        <f>SUM(BPMCCS!B2,'MN IRP'!B19)</f>
         <v>22.599999999999909</v>
       </c>
       <c r="E2">
-        <f>SUM(BPMCCS!C2,'MN IRP'!C28)</f>
+        <f>SUM(BPMCCS!C2,'MN IRP'!C19)</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>SUM(BPMCCS!D2,'MN IRP'!D28)</f>
+        <f>SUM(BPMCCS!D2,'MN IRP'!D19)</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUM(BPMCCS!E2,'MN IRP'!E28)</f>
+        <f>SUM(BPMCCS!E2,'MN IRP'!E19)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>SUM(BPMCCS!F2,'MN IRP'!F28)</f>
+        <f>SUM(BPMCCS!F2,'MN IRP'!F19)</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>SUM(BPMCCS!G2,'MN IRP'!G28)</f>
+        <f>SUM(BPMCCS!G2,'MN IRP'!G19)</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>SUM(BPMCCS!H2,'MN IRP'!H28)</f>
+        <f>SUM(BPMCCS!H2,'MN IRP'!H19)</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>SUM(BPMCCS!I2,'MN IRP'!I28)</f>
+        <f>SUM(BPMCCS!I2,'MN IRP'!I19)</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>SUM(BPMCCS!J2,'MN IRP'!J28)</f>
+        <f>SUM(BPMCCS!J2,'MN IRP'!J19)</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>SUM(BPMCCS!K2,'MN IRP'!K28)</f>
+        <f>SUM(BPMCCS!K2,'MN IRP'!K19)</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>SUM(BPMCCS!L2,'MN IRP'!L28)</f>
+        <f>SUM(BPMCCS!L2,'MN IRP'!L19)</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f>SUM(BPMCCS!M2,'MN IRP'!M28)</f>
+        <f>SUM(BPMCCS!M2,'MN IRP'!M19)</f>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>SUM(BPMCCS!N2,'MN IRP'!N28)</f>
+        <f>SUM(BPMCCS!N2,'MN IRP'!N19)</f>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>SUM(BPMCCS!O2,'MN IRP'!O28)</f>
+        <f>SUM(BPMCCS!O2,'MN IRP'!O19)</f>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>SUM(BPMCCS!P2,'MN IRP'!P28)</f>
+        <f>SUM(BPMCCS!P2,'MN IRP'!P19)</f>
         <v>0</v>
       </c>
       <c r="S2">
-        <f>SUM(BPMCCS!Q2,'MN IRP'!Q28)</f>
+        <f>SUM(BPMCCS!Q2,'MN IRP'!Q19)</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f>SUM(BPMCCS!R2,'MN IRP'!R28)</f>
+        <f>SUM(BPMCCS!R2,'MN IRP'!R19)</f>
         <v>0</v>
       </c>
       <c r="U2">
-        <f>SUM(BPMCCS!S2,'MN IRP'!S28)</f>
+        <f>SUM(BPMCCS!S2,'MN IRP'!S19)</f>
         <v>0</v>
       </c>
       <c r="V2">
-        <f>SUM(BPMCCS!T2,'MN IRP'!T28)</f>
+        <f>SUM(BPMCCS!T2,'MN IRP'!T19)</f>
         <v>0</v>
       </c>
       <c r="W2">
-        <f>SUM(BPMCCS!U2,'MN IRP'!U28)</f>
+        <f>SUM(BPMCCS!U2,'MN IRP'!U19)</f>
         <v>0</v>
       </c>
       <c r="X2">
-        <f>SUM(BPMCCS!V2,'MN IRP'!V28)</f>
+        <f>SUM(BPMCCS!V2,'MN IRP'!V19)</f>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f>SUM(BPMCCS!W2,'MN IRP'!W28)</f>
+        <f>SUM(BPMCCS!W2,'MN IRP'!W19)</f>
         <v>0</v>
       </c>
       <c r="Z2">
-        <f>SUM(BPMCCS!X2,'MN IRP'!X28)</f>
+        <f>SUM(BPMCCS!X2,'MN IRP'!X19)</f>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f>SUM(BPMCCS!Y2,'MN IRP'!Y28)</f>
+        <f>SUM(BPMCCS!Y2,'MN IRP'!Y19)</f>
         <v>0</v>
       </c>
       <c r="AB2">
-        <f>SUM(BPMCCS!Z2,'MN IRP'!Z28)</f>
+        <f>SUM(BPMCCS!Z2,'MN IRP'!Z19)</f>
         <v>0</v>
       </c>
       <c r="AC2">
-        <f>SUM(BPMCCS!AA2,'MN IRP'!AA28)</f>
+        <f>SUM(BPMCCS!AA2,'MN IRP'!AA19)</f>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f>SUM(BPMCCS!AB2,'MN IRP'!AB28)</f>
+        <f>SUM(BPMCCS!AB2,'MN IRP'!AB19)</f>
         <v>0</v>
       </c>
       <c r="AE2">
-        <f>SUM(BPMCCS!AC2,'MN IRP'!AC28)</f>
+        <f>SUM(BPMCCS!AC2,'MN IRP'!AC19)</f>
         <v>0</v>
       </c>
       <c r="AF2">
-        <f>SUM(BPMCCS!AD2,'MN IRP'!AD28)</f>
+        <f>SUM(BPMCCS!AD2,'MN IRP'!AD19)</f>
         <v>0</v>
       </c>
       <c r="AG2">
-        <f>SUM(BPMCCS!AE2,'MN IRP'!AE28)</f>
+        <f>SUM(BPMCCS!AE2,'MN IRP'!AE19)</f>
         <v>0</v>
       </c>
       <c r="AH2">
-        <f>SUM(BPMCCS!AF2,'MN IRP'!AF28)</f>
+        <f>SUM(BPMCCS!AF2,'MN IRP'!AF19)</f>
         <v>0</v>
       </c>
       <c r="AI2">
-        <f>SUM(BPMCCS!AG2,'MN IRP'!AG28)</f>
+        <f>SUM(BPMCCS!AG2,'MN IRP'!AG19)</f>
         <v>0</v>
       </c>
     </row>
@@ -3118,131 +2999,131 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>SUM(BPMCCS!B3,'MN IRP'!B29)</f>
+        <f>SUM(BPMCCS!B3,'MN IRP'!B20)</f>
         <v>324</v>
       </c>
       <c r="E3">
-        <f>SUM(BPMCCS!C3,'MN IRP'!C29)</f>
+        <f>SUM(BPMCCS!C3,'MN IRP'!C20)</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f>SUM(BPMCCS!D3,'MN IRP'!D29)</f>
+        <f>SUM(BPMCCS!D3,'MN IRP'!D20)</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f>SUM(BPMCCS!E3,'MN IRP'!E29)</f>
+        <f>SUM(BPMCCS!E3,'MN IRP'!E20)</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f>SUM(BPMCCS!F3,'MN IRP'!F29)</f>
+        <f>SUM(BPMCCS!F3,'MN IRP'!F20)</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f>SUM(BPMCCS!G3,'MN IRP'!G29)</f>
+        <f>SUM(BPMCCS!G3,'MN IRP'!G20)</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f>SUM(BPMCCS!H3,'MN IRP'!H29)</f>
+        <f>SUM(BPMCCS!H3,'MN IRP'!H20)</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f>SUM(BPMCCS!I3,'MN IRP'!I29)</f>
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <f>SUM(BPMCCS!J3,'MN IRP'!J29)</f>
-        <v>0</v>
+        <f>SUM(BPMCCS!I3,'MN IRP'!I20)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <f>SUM(BPMCCS!J3,'MN IRP'!J20)</f>
+        <v>800</v>
       </c>
       <c r="M3">
-        <f>SUM(BPMCCS!K3,'MN IRP'!K29)</f>
+        <f>SUM(BPMCCS!K3,'MN IRP'!K20)</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>SUM(BPMCCS!L3,'MN IRP'!L29)</f>
+        <f>SUM(BPMCCS!L3,'MN IRP'!L20)</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f>SUM(BPMCCS!M3,'MN IRP'!M29)</f>
+        <f>SUM(BPMCCS!M3,'MN IRP'!M20)</f>
         <v>0</v>
       </c>
       <c r="P3">
-        <f>SUM(BPMCCS!N3,'MN IRP'!N29)</f>
+        <f>SUM(BPMCCS!N3,'MN IRP'!N20)</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f>SUM(BPMCCS!O3,'MN IRP'!O29)</f>
+        <f>SUM(BPMCCS!O3,'MN IRP'!O20)</f>
         <v>0</v>
       </c>
       <c r="R3">
-        <f>SUM(BPMCCS!P3,'MN IRP'!P29)</f>
+        <f>SUM(BPMCCS!P3,'MN IRP'!P20)</f>
         <v>0</v>
       </c>
       <c r="S3">
-        <f>SUM(BPMCCS!Q3,'MN IRP'!Q29)</f>
+        <f>SUM(BPMCCS!Q3,'MN IRP'!Q20)</f>
         <v>0</v>
       </c>
       <c r="T3">
-        <f>SUM(BPMCCS!R3,'MN IRP'!R29)</f>
+        <f>SUM(BPMCCS!R3,'MN IRP'!R20)</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f>SUM(BPMCCS!S3,'MN IRP'!S29)</f>
+        <f>SUM(BPMCCS!S3,'MN IRP'!S20)</f>
         <v>0</v>
       </c>
       <c r="V3">
-        <f>SUM(BPMCCS!T3,'MN IRP'!T29)</f>
+        <f>SUM(BPMCCS!T3,'MN IRP'!T20)</f>
         <v>0</v>
       </c>
       <c r="W3">
-        <f>SUM(BPMCCS!U3,'MN IRP'!U29)</f>
+        <f>SUM(BPMCCS!U3,'MN IRP'!U20)</f>
         <v>0</v>
       </c>
       <c r="X3">
-        <f>SUM(BPMCCS!V3,'MN IRP'!V29)</f>
+        <f>SUM(BPMCCS!V3,'MN IRP'!V20)</f>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f>SUM(BPMCCS!W3,'MN IRP'!W29)</f>
+        <f>SUM(BPMCCS!W3,'MN IRP'!W20)</f>
         <v>0</v>
       </c>
       <c r="Z3">
-        <f>SUM(BPMCCS!X3,'MN IRP'!X29)</f>
+        <f>SUM(BPMCCS!X3,'MN IRP'!X20)</f>
         <v>0</v>
       </c>
       <c r="AA3">
-        <f>SUM(BPMCCS!Y3,'MN IRP'!Y29)</f>
+        <f>SUM(BPMCCS!Y3,'MN IRP'!Y20)</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f>SUM(BPMCCS!Z3,'MN IRP'!Z29)</f>
+        <f>SUM(BPMCCS!Z3,'MN IRP'!Z20)</f>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f>SUM(BPMCCS!AA3,'MN IRP'!AA29)</f>
+        <f>SUM(BPMCCS!AA3,'MN IRP'!AA20)</f>
         <v>0</v>
       </c>
       <c r="AD3">
-        <f>SUM(BPMCCS!AB3,'MN IRP'!AB29)</f>
+        <f>SUM(BPMCCS!AB3,'MN IRP'!AB20)</f>
         <v>0</v>
       </c>
       <c r="AE3">
-        <f>SUM(BPMCCS!AC3,'MN IRP'!AC29)</f>
+        <f>SUM(BPMCCS!AC3,'MN IRP'!AC20)</f>
         <v>0</v>
       </c>
       <c r="AF3">
-        <f>SUM(BPMCCS!AD3,'MN IRP'!AD29)</f>
+        <f>SUM(BPMCCS!AD3,'MN IRP'!AD20)</f>
         <v>0</v>
       </c>
       <c r="AG3">
-        <f>SUM(BPMCCS!AE3,'MN IRP'!AE29)</f>
+        <f>SUM(BPMCCS!AE3,'MN IRP'!AE20)</f>
         <v>0</v>
       </c>
       <c r="AH3">
-        <f>SUM(BPMCCS!AF3,'MN IRP'!AF29)</f>
+        <f>SUM(BPMCCS!AF3,'MN IRP'!AF20)</f>
         <v>0</v>
       </c>
       <c r="AI3">
-        <f>SUM(BPMCCS!AG3,'MN IRP'!AG29)</f>
+        <f>SUM(BPMCCS!AG3,'MN IRP'!AG20)</f>
         <v>0</v>
       </c>
     </row>
@@ -3257,131 +3138,131 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>SUM(BPMCCS!B4,'MN IRP'!B30)</f>
+        <f>SUM(BPMCCS!B4,'MN IRP'!B21)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>SUM(BPMCCS!C4,'MN IRP'!C30)</f>
+        <f>SUM(BPMCCS!C4,'MN IRP'!C21)</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>SUM(BPMCCS!D4,'MN IRP'!D30)</f>
+        <f>SUM(BPMCCS!D4,'MN IRP'!D21)</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>SUM(BPMCCS!E4,'MN IRP'!E30)</f>
+        <f>SUM(BPMCCS!E4,'MN IRP'!E21)</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>SUM(BPMCCS!F4,'MN IRP'!F30)</f>
+        <f>SUM(BPMCCS!F4,'MN IRP'!F21)</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>SUM(BPMCCS!G4,'MN IRP'!G30)</f>
+        <f>SUM(BPMCCS!G4,'MN IRP'!G21)</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>SUM(BPMCCS!H4,'MN IRP'!H30)</f>
+        <f>SUM(BPMCCS!H4,'MN IRP'!H21)</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>SUM(BPMCCS!I4,'MN IRP'!I30)</f>
+        <f>SUM(BPMCCS!I4,'MN IRP'!I21)</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>SUM(BPMCCS!J4,'MN IRP'!J30)</f>
+        <f>SUM(BPMCCS!J4,'MN IRP'!J21)</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f>SUM(BPMCCS!K4,'MN IRP'!K30)</f>
+        <f>SUM(BPMCCS!K4,'MN IRP'!K21)</f>
         <v>0</v>
       </c>
       <c r="N4">
-        <f>SUM(BPMCCS!L4,'MN IRP'!L30)</f>
+        <f>SUM(BPMCCS!L4,'MN IRP'!L21)</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>SUM(BPMCCS!M4,'MN IRP'!M30)</f>
+        <f>SUM(BPMCCS!M4,'MN IRP'!M21)</f>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>SUM(BPMCCS!N4,'MN IRP'!N30)</f>
+        <f>SUM(BPMCCS!N4,'MN IRP'!N21)</f>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>SUM(BPMCCS!O4,'MN IRP'!O30)</f>
+        <f>SUM(BPMCCS!O4,'MN IRP'!O21)</f>
         <v>0</v>
       </c>
       <c r="R4">
-        <f>SUM(BPMCCS!P4,'MN IRP'!P30)</f>
+        <f>SUM(BPMCCS!P4,'MN IRP'!P21)</f>
         <v>0</v>
       </c>
       <c r="S4">
-        <f>SUM(BPMCCS!Q4,'MN IRP'!Q30)</f>
+        <f>SUM(BPMCCS!Q4,'MN IRP'!Q21)</f>
         <v>0</v>
       </c>
       <c r="T4">
-        <f>SUM(BPMCCS!R4,'MN IRP'!R30)</f>
+        <f>SUM(BPMCCS!R4,'MN IRP'!R21)</f>
         <v>0</v>
       </c>
       <c r="U4">
-        <f>SUM(BPMCCS!S4,'MN IRP'!S30)</f>
+        <f>SUM(BPMCCS!S4,'MN IRP'!S21)</f>
         <v>0</v>
       </c>
       <c r="V4">
-        <f>SUM(BPMCCS!T4,'MN IRP'!T30)</f>
+        <f>SUM(BPMCCS!T4,'MN IRP'!T21)</f>
         <v>0</v>
       </c>
       <c r="W4">
-        <f>SUM(BPMCCS!U4,'MN IRP'!U30)</f>
+        <f>SUM(BPMCCS!U4,'MN IRP'!U21)</f>
         <v>0</v>
       </c>
       <c r="X4">
-        <f>SUM(BPMCCS!V4,'MN IRP'!V30)</f>
+        <f>SUM(BPMCCS!V4,'MN IRP'!V21)</f>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f>SUM(BPMCCS!W4,'MN IRP'!W30)</f>
+        <f>SUM(BPMCCS!W4,'MN IRP'!W21)</f>
         <v>0</v>
       </c>
       <c r="Z4">
-        <f>SUM(BPMCCS!X4,'MN IRP'!X30)</f>
+        <f>SUM(BPMCCS!X4,'MN IRP'!X21)</f>
         <v>0</v>
       </c>
       <c r="AA4">
-        <f>SUM(BPMCCS!Y4,'MN IRP'!Y30)</f>
+        <f>SUM(BPMCCS!Y4,'MN IRP'!Y21)</f>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f>SUM(BPMCCS!Z4,'MN IRP'!Z30)</f>
+        <f>SUM(BPMCCS!Z4,'MN IRP'!Z21)</f>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f>SUM(BPMCCS!AA4,'MN IRP'!AA30)</f>
+        <f>SUM(BPMCCS!AA4,'MN IRP'!AA21)</f>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f>SUM(BPMCCS!AB4,'MN IRP'!AB30)</f>
+        <f>SUM(BPMCCS!AB4,'MN IRP'!AB21)</f>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>SUM(BPMCCS!AC4,'MN IRP'!AC30)</f>
+        <f>SUM(BPMCCS!AC4,'MN IRP'!AC21)</f>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f>SUM(BPMCCS!AD4,'MN IRP'!AD30)</f>
+        <f>SUM(BPMCCS!AD4,'MN IRP'!AD21)</f>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f>SUM(BPMCCS!AE4,'MN IRP'!AE30)</f>
+        <f>SUM(BPMCCS!AE4,'MN IRP'!AE21)</f>
         <v>0</v>
       </c>
       <c r="AH4">
-        <f>SUM(BPMCCS!AF4,'MN IRP'!AF30)</f>
+        <f>SUM(BPMCCS!AF4,'MN IRP'!AF21)</f>
         <v>0</v>
       </c>
       <c r="AI4">
-        <f>SUM(BPMCCS!AG4,'MN IRP'!AG30)</f>
+        <f>SUM(BPMCCS!AG4,'MN IRP'!AG21)</f>
         <v>0</v>
       </c>
     </row>
@@ -3396,131 +3277,131 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>SUM(BPMCCS!B5,'MN IRP'!B31)</f>
+        <f>SUM(BPMCCS!B5,'MN IRP'!B22)</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>SUM(BPMCCS!C5,'MN IRP'!C31)</f>
+        <f>SUM(BPMCCS!C5,'MN IRP'!C22)</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>SUM(BPMCCS!D5,'MN IRP'!D31)</f>
+        <f>SUM(BPMCCS!D5,'MN IRP'!D22)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>SUM(BPMCCS!E5,'MN IRP'!E31)</f>
+        <f>SUM(BPMCCS!E5,'MN IRP'!E22)</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>SUM(BPMCCS!F5,'MN IRP'!F31)</f>
+        <f>SUM(BPMCCS!F5,'MN IRP'!F22)</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f>SUM(BPMCCS!G5,'MN IRP'!G31)</f>
+        <f>SUM(BPMCCS!G5,'MN IRP'!G22)</f>
         <v>0</v>
       </c>
       <c r="J5">
-        <f>SUM(BPMCCS!H5,'MN IRP'!H31)</f>
+        <f>SUM(BPMCCS!H5,'MN IRP'!H22)</f>
         <v>0</v>
       </c>
       <c r="K5">
-        <f>SUM(BPMCCS!I5,'MN IRP'!I31)</f>
+        <f>SUM(BPMCCS!I5,'MN IRP'!I22)</f>
         <v>0</v>
       </c>
       <c r="L5">
-        <f>SUM(BPMCCS!J5,'MN IRP'!J31)</f>
+        <f>SUM(BPMCCS!J5,'MN IRP'!J22)</f>
         <v>0</v>
       </c>
       <c r="M5">
-        <f>SUM(BPMCCS!K5,'MN IRP'!K31)</f>
+        <f>SUM(BPMCCS!K5,'MN IRP'!K22)</f>
         <v>0</v>
       </c>
       <c r="N5">
-        <f>SUM(BPMCCS!L5,'MN IRP'!L31)</f>
+        <f>SUM(BPMCCS!L5,'MN IRP'!L22)</f>
         <v>0</v>
       </c>
       <c r="O5">
-        <f>SUM(BPMCCS!M5,'MN IRP'!M31)</f>
+        <f>SUM(BPMCCS!M5,'MN IRP'!M22)</f>
         <v>0</v>
       </c>
       <c r="P5">
-        <f>SUM(BPMCCS!N5,'MN IRP'!N31)</f>
+        <f>SUM(BPMCCS!N5,'MN IRP'!N22)</f>
         <v>0</v>
       </c>
       <c r="Q5">
-        <f>SUM(BPMCCS!O5,'MN IRP'!O31)</f>
+        <f>SUM(BPMCCS!O5,'MN IRP'!O22)</f>
         <v>0</v>
       </c>
       <c r="R5">
-        <f>SUM(BPMCCS!P5,'MN IRP'!P31)</f>
+        <f>SUM(BPMCCS!P5,'MN IRP'!P22)</f>
         <v>0</v>
       </c>
       <c r="S5">
-        <f>SUM(BPMCCS!Q5,'MN IRP'!Q31)</f>
+        <f>SUM(BPMCCS!Q5,'MN IRP'!Q22)</f>
         <v>0</v>
       </c>
       <c r="T5">
-        <f>SUM(BPMCCS!R5,'MN IRP'!R31)</f>
+        <f>SUM(BPMCCS!R5,'MN IRP'!R22)</f>
         <v>0</v>
       </c>
       <c r="U5">
-        <f>SUM(BPMCCS!S5,'MN IRP'!S31)</f>
+        <f>SUM(BPMCCS!S5,'MN IRP'!S22)</f>
         <v>0</v>
       </c>
       <c r="V5">
-        <f>SUM(BPMCCS!T5,'MN IRP'!T31)</f>
+        <f>SUM(BPMCCS!T5,'MN IRP'!T22)</f>
         <v>0</v>
       </c>
       <c r="W5">
-        <f>SUM(BPMCCS!U5,'MN IRP'!U31)</f>
+        <f>SUM(BPMCCS!U5,'MN IRP'!U22)</f>
         <v>0</v>
       </c>
       <c r="X5">
-        <f>SUM(BPMCCS!V5,'MN IRP'!V31)</f>
+        <f>SUM(BPMCCS!V5,'MN IRP'!V22)</f>
         <v>0</v>
       </c>
       <c r="Y5">
-        <f>SUM(BPMCCS!W5,'MN IRP'!W31)</f>
+        <f>SUM(BPMCCS!W5,'MN IRP'!W22)</f>
         <v>0</v>
       </c>
       <c r="Z5">
-        <f>SUM(BPMCCS!X5,'MN IRP'!X31)</f>
+        <f>SUM(BPMCCS!X5,'MN IRP'!X22)</f>
         <v>0</v>
       </c>
       <c r="AA5">
-        <f>SUM(BPMCCS!Y5,'MN IRP'!Y31)</f>
+        <f>SUM(BPMCCS!Y5,'MN IRP'!Y22)</f>
         <v>0</v>
       </c>
       <c r="AB5">
-        <f>SUM(BPMCCS!Z5,'MN IRP'!Z31)</f>
+        <f>SUM(BPMCCS!Z5,'MN IRP'!Z22)</f>
         <v>0</v>
       </c>
       <c r="AC5">
-        <f>SUM(BPMCCS!AA5,'MN IRP'!AA31)</f>
+        <f>SUM(BPMCCS!AA5,'MN IRP'!AA22)</f>
         <v>0</v>
       </c>
       <c r="AD5">
-        <f>SUM(BPMCCS!AB5,'MN IRP'!AB31)</f>
+        <f>SUM(BPMCCS!AB5,'MN IRP'!AB22)</f>
         <v>0</v>
       </c>
       <c r="AE5">
-        <f>SUM(BPMCCS!AC5,'MN IRP'!AC31)</f>
+        <f>SUM(BPMCCS!AC5,'MN IRP'!AC22)</f>
         <v>0</v>
       </c>
       <c r="AF5">
-        <f>SUM(BPMCCS!AD5,'MN IRP'!AD31)</f>
+        <f>SUM(BPMCCS!AD5,'MN IRP'!AD22)</f>
         <v>0</v>
       </c>
       <c r="AG5">
-        <f>SUM(BPMCCS!AE5,'MN IRP'!AE31)</f>
+        <f>SUM(BPMCCS!AE5,'MN IRP'!AE22)</f>
         <v>0</v>
       </c>
       <c r="AH5">
-        <f>SUM(BPMCCS!AF5,'MN IRP'!AF31)</f>
+        <f>SUM(BPMCCS!AF5,'MN IRP'!AF22)</f>
         <v>0</v>
       </c>
       <c r="AI5">
-        <f>SUM(BPMCCS!AG5,'MN IRP'!AG31)</f>
+        <f>SUM(BPMCCS!AG5,'MN IRP'!AG22)</f>
         <v>0</v>
       </c>
     </row>
@@ -3535,131 +3416,131 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>SUM(BPMCCS!B6,'MN IRP'!B32)</f>
+        <f>SUM(BPMCCS!B6,'MN IRP'!B23)</f>
         <v>79.200000000000728</v>
       </c>
       <c r="E6">
-        <f>SUM(BPMCCS!C6,'MN IRP'!C32)</f>
+        <f>SUM(BPMCCS!C6,'MN IRP'!C23)</f>
         <v>454.6</v>
       </c>
       <c r="F6">
-        <f>SUM(BPMCCS!D6,'MN IRP'!D32)</f>
+        <f>SUM(BPMCCS!D6,'MN IRP'!D23)</f>
         <v>400</v>
       </c>
       <c r="G6">
-        <f>SUM(BPMCCS!E6,'MN IRP'!E32)</f>
+        <f>SUM(BPMCCS!E6,'MN IRP'!E23)</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>SUM(BPMCCS!F6,'MN IRP'!F32)</f>
+        <f>SUM(BPMCCS!F6,'MN IRP'!F23)</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>SUM(BPMCCS!G6,'MN IRP'!G32)</f>
+        <f>SUM(BPMCCS!G6,'MN IRP'!G23)</f>
         <v>0</v>
       </c>
       <c r="J6">
-        <f>SUM(BPMCCS!H6,'MN IRP'!H32)</f>
-        <v>650</v>
-      </c>
-      <c r="K6">
-        <f>SUM(BPMCCS!I6,'MN IRP'!I32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="L6">
-        <f>SUM(BPMCCS!J6,'MN IRP'!J32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="M6">
-        <f>SUM(BPMCCS!K6,'MN IRP'!K32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="N6">
-        <f>SUM(BPMCCS!L6,'MN IRP'!L32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="O6">
-        <f>SUM(BPMCCS!M6,'MN IRP'!M32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="P6">
-        <f>SUM(BPMCCS!N6,'MN IRP'!N32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="Q6">
-        <f>SUM(BPMCCS!O6,'MN IRP'!O32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="R6">
-        <f>SUM(BPMCCS!P6,'MN IRP'!P32)</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="S6">
-        <f>SUM(BPMCCS!Q6,'MN IRP'!Q32)</f>
-        <v>133.33333333333334</v>
+        <f>SUM(BPMCCS!H6,'MN IRP'!H23)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <f>SUM(BPMCCS!I6,'MN IRP'!I23)</f>
+        <v>250</v>
+      </c>
+      <c r="L6" s="8">
+        <f>SUM(BPMCCS!J6,'MN IRP'!J23)</f>
+        <v>250</v>
+      </c>
+      <c r="M6" s="8">
+        <f>SUM(BPMCCS!K6,'MN IRP'!K23)</f>
+        <v>250</v>
+      </c>
+      <c r="N6" s="8">
+        <f>SUM(BPMCCS!L6,'MN IRP'!L23)</f>
+        <v>250</v>
+      </c>
+      <c r="O6" s="8">
+        <f>SUM(BPMCCS!M6,'MN IRP'!M23)</f>
+        <v>250</v>
+      </c>
+      <c r="P6" s="8">
+        <f>SUM(BPMCCS!N6,'MN IRP'!N23)</f>
+        <v>250</v>
+      </c>
+      <c r="Q6" s="8">
+        <f>SUM(BPMCCS!O6,'MN IRP'!O23)</f>
+        <v>250</v>
+      </c>
+      <c r="R6" s="8">
+        <f>SUM(BPMCCS!P6,'MN IRP'!P23)</f>
+        <v>250</v>
+      </c>
+      <c r="S6" s="8">
+        <f>SUM(BPMCCS!Q6,'MN IRP'!Q23)</f>
+        <v>250</v>
       </c>
       <c r="T6">
-        <f>SUM(BPMCCS!R6,'MN IRP'!R32)</f>
+        <f>SUM(BPMCCS!R6,'MN IRP'!R23)</f>
         <v>0</v>
       </c>
       <c r="U6">
-        <f>SUM(BPMCCS!S6,'MN IRP'!S32)</f>
+        <f>SUM(BPMCCS!S6,'MN IRP'!S23)</f>
         <v>0</v>
       </c>
       <c r="V6">
-        <f>SUM(BPMCCS!T6,'MN IRP'!T32)</f>
+        <f>SUM(BPMCCS!T6,'MN IRP'!T23)</f>
         <v>0</v>
       </c>
       <c r="W6">
-        <f>SUM(BPMCCS!U6,'MN IRP'!U32)</f>
+        <f>SUM(BPMCCS!U6,'MN IRP'!U23)</f>
         <v>0</v>
       </c>
       <c r="X6">
-        <f>SUM(BPMCCS!V6,'MN IRP'!V32)</f>
+        <f>SUM(BPMCCS!V6,'MN IRP'!V23)</f>
         <v>0</v>
       </c>
       <c r="Y6">
-        <f>SUM(BPMCCS!W6,'MN IRP'!W32)</f>
+        <f>SUM(BPMCCS!W6,'MN IRP'!W23)</f>
         <v>0</v>
       </c>
       <c r="Z6">
-        <f>SUM(BPMCCS!X6,'MN IRP'!X32)</f>
+        <f>SUM(BPMCCS!X6,'MN IRP'!X23)</f>
         <v>0</v>
       </c>
       <c r="AA6">
-        <f>SUM(BPMCCS!Y6,'MN IRP'!Y32)</f>
+        <f>SUM(BPMCCS!Y6,'MN IRP'!Y23)</f>
         <v>0</v>
       </c>
       <c r="AB6">
-        <f>SUM(BPMCCS!Z6,'MN IRP'!Z32)</f>
+        <f>SUM(BPMCCS!Z6,'MN IRP'!Z23)</f>
         <v>0</v>
       </c>
       <c r="AC6">
-        <f>SUM(BPMCCS!AA6,'MN IRP'!AA32)</f>
+        <f>SUM(BPMCCS!AA6,'MN IRP'!AA23)</f>
         <v>0</v>
       </c>
       <c r="AD6">
-        <f>SUM(BPMCCS!AB6,'MN IRP'!AB32)</f>
+        <f>SUM(BPMCCS!AB6,'MN IRP'!AB23)</f>
         <v>0</v>
       </c>
       <c r="AE6">
-        <f>SUM(BPMCCS!AC6,'MN IRP'!AC32)</f>
+        <f>SUM(BPMCCS!AC6,'MN IRP'!AC23)</f>
         <v>0</v>
       </c>
       <c r="AF6">
-        <f>SUM(BPMCCS!AD6,'MN IRP'!AD32)</f>
+        <f>SUM(BPMCCS!AD6,'MN IRP'!AD23)</f>
         <v>0</v>
       </c>
       <c r="AG6">
-        <f>SUM(BPMCCS!AE6,'MN IRP'!AE32)</f>
+        <f>SUM(BPMCCS!AE6,'MN IRP'!AE23)</f>
         <v>0</v>
       </c>
       <c r="AH6">
-        <f>SUM(BPMCCS!AF6,'MN IRP'!AF32)</f>
+        <f>SUM(BPMCCS!AF6,'MN IRP'!AF23)</f>
         <v>0</v>
       </c>
       <c r="AI6">
-        <f>SUM(BPMCCS!AG6,'MN IRP'!AG32)</f>
+        <f>SUM(BPMCCS!AG6,'MN IRP'!AG23)</f>
         <v>0</v>
       </c>
     </row>
@@ -3674,131 +3555,131 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>SUM(BPMCCS!B7,'MN IRP'!B33)</f>
+        <f>SUM(BPMCCS!B7,'MN IRP'!B24)</f>
         <v>107.79999999999995</v>
       </c>
       <c r="E7">
-        <f>SUM(BPMCCS!C7,'MN IRP'!C33)</f>
+        <f>SUM(BPMCCS!C7,'MN IRP'!C24)</f>
         <v>68.400000000000006</v>
       </c>
       <c r="F7">
-        <f>SUM(BPMCCS!D7,'MN IRP'!D33)</f>
+        <f>SUM(BPMCCS!D7,'MN IRP'!D24)</f>
         <v>97</v>
       </c>
       <c r="G7">
-        <f>SUM(BPMCCS!E7,'MN IRP'!E33)</f>
+        <f>SUM(BPMCCS!E7,'MN IRP'!E24)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>SUM(BPMCCS!F7,'MN IRP'!F33)</f>
+        <f>SUM(BPMCCS!F7,'MN IRP'!F24)</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>SUM(BPMCCS!G7,'MN IRP'!G33)</f>
+        <f>SUM(BPMCCS!G7,'MN IRP'!G24)</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f>SUM(BPMCCS!H7,'MN IRP'!H33)</f>
-        <v>450</v>
-      </c>
-      <c r="K7">
-        <f>SUM(BPMCCS!I7,'MN IRP'!I33)</f>
-        <v>710</v>
-      </c>
-      <c r="L7">
-        <f>SUM(BPMCCS!J7,'MN IRP'!J33)</f>
-        <v>710</v>
-      </c>
-      <c r="M7">
-        <f>SUM(BPMCCS!K7,'MN IRP'!K33)</f>
-        <v>710</v>
-      </c>
-      <c r="N7">
-        <f>SUM(BPMCCS!L7,'MN IRP'!L33)</f>
-        <v>710</v>
-      </c>
-      <c r="O7">
-        <f>SUM(BPMCCS!M7,'MN IRP'!M33)</f>
-        <v>710</v>
+        <f>SUM(BPMCCS!H7,'MN IRP'!H24)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <f>SUM(BPMCCS!I7,'MN IRP'!I24)</f>
+        <v>700</v>
+      </c>
+      <c r="L7" s="8">
+        <f>SUM(BPMCCS!J7,'MN IRP'!J24)</f>
+        <v>700</v>
+      </c>
+      <c r="M7" s="8">
+        <f>SUM(BPMCCS!K7,'MN IRP'!K24)</f>
+        <v>700</v>
+      </c>
+      <c r="N7" s="8">
+        <f>SUM(BPMCCS!L7,'MN IRP'!L24)</f>
+        <v>700</v>
+      </c>
+      <c r="O7" s="8">
+        <f>SUM(BPMCCS!M7,'MN IRP'!M24)</f>
+        <v>700</v>
       </c>
       <c r="P7">
-        <f>SUM(BPMCCS!N7,'MN IRP'!N33)</f>
+        <f>SUM(BPMCCS!N7,'MN IRP'!N24)</f>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>SUM(BPMCCS!O7,'MN IRP'!O33)</f>
+        <f>SUM(BPMCCS!O7,'MN IRP'!O24)</f>
         <v>0</v>
       </c>
       <c r="R7">
-        <f>SUM(BPMCCS!P7,'MN IRP'!P33)</f>
+        <f>SUM(BPMCCS!P7,'MN IRP'!P24)</f>
         <v>0</v>
       </c>
       <c r="S7">
-        <f>SUM(BPMCCS!Q7,'MN IRP'!Q33)</f>
+        <f>SUM(BPMCCS!Q7,'MN IRP'!Q24)</f>
         <v>0</v>
       </c>
       <c r="T7">
-        <f>SUM(BPMCCS!R7,'MN IRP'!R33)</f>
+        <f>SUM(BPMCCS!R7,'MN IRP'!R24)</f>
         <v>0</v>
       </c>
       <c r="U7">
-        <f>SUM(BPMCCS!S7,'MN IRP'!S33)</f>
+        <f>SUM(BPMCCS!S7,'MN IRP'!S24)</f>
         <v>0</v>
       </c>
       <c r="V7">
-        <f>SUM(BPMCCS!T7,'MN IRP'!T33)</f>
+        <f>SUM(BPMCCS!T7,'MN IRP'!T24)</f>
         <v>0</v>
       </c>
       <c r="W7">
-        <f>SUM(BPMCCS!U7,'MN IRP'!U33)</f>
+        <f>SUM(BPMCCS!U7,'MN IRP'!U24)</f>
         <v>0</v>
       </c>
       <c r="X7">
-        <f>SUM(BPMCCS!V7,'MN IRP'!V33)</f>
+        <f>SUM(BPMCCS!V7,'MN IRP'!V24)</f>
         <v>0</v>
       </c>
       <c r="Y7">
-        <f>SUM(BPMCCS!W7,'MN IRP'!W33)</f>
+        <f>SUM(BPMCCS!W7,'MN IRP'!W24)</f>
         <v>0</v>
       </c>
       <c r="Z7">
-        <f>SUM(BPMCCS!X7,'MN IRP'!X33)</f>
+        <f>SUM(BPMCCS!X7,'MN IRP'!X24)</f>
         <v>0</v>
       </c>
       <c r="AA7">
-        <f>SUM(BPMCCS!Y7,'MN IRP'!Y33)</f>
+        <f>SUM(BPMCCS!Y7,'MN IRP'!Y24)</f>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f>SUM(BPMCCS!Z7,'MN IRP'!Z33)</f>
+        <f>SUM(BPMCCS!Z7,'MN IRP'!Z24)</f>
         <v>0</v>
       </c>
       <c r="AC7">
-        <f>SUM(BPMCCS!AA7,'MN IRP'!AA33)</f>
+        <f>SUM(BPMCCS!AA7,'MN IRP'!AA24)</f>
         <v>0</v>
       </c>
       <c r="AD7">
-        <f>SUM(BPMCCS!AB7,'MN IRP'!AB33)</f>
+        <f>SUM(BPMCCS!AB7,'MN IRP'!AB24)</f>
         <v>0</v>
       </c>
       <c r="AE7">
-        <f>SUM(BPMCCS!AC7,'MN IRP'!AC33)</f>
+        <f>SUM(BPMCCS!AC7,'MN IRP'!AC24)</f>
         <v>0</v>
       </c>
       <c r="AF7">
-        <f>SUM(BPMCCS!AD7,'MN IRP'!AD33)</f>
+        <f>SUM(BPMCCS!AD7,'MN IRP'!AD24)</f>
         <v>0</v>
       </c>
       <c r="AG7">
-        <f>SUM(BPMCCS!AE7,'MN IRP'!AE33)</f>
+        <f>SUM(BPMCCS!AE7,'MN IRP'!AE24)</f>
         <v>0</v>
       </c>
       <c r="AH7">
-        <f>SUM(BPMCCS!AF7,'MN IRP'!AF33)</f>
+        <f>SUM(BPMCCS!AF7,'MN IRP'!AF24)</f>
         <v>0</v>
       </c>
       <c r="AI7">
-        <f>SUM(BPMCCS!AG7,'MN IRP'!AG33)</f>
+        <f>SUM(BPMCCS!AG7,'MN IRP'!AG24)</f>
         <v>0</v>
       </c>
     </row>
@@ -3813,131 +3694,131 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>SUM(BPMCCS!B8,'MN IRP'!B34)</f>
+        <f>SUM(BPMCCS!B8,'MN IRP'!B25)</f>
         <v>0</v>
       </c>
       <c r="E8">
-        <f>SUM(BPMCCS!C8,'MN IRP'!C34)</f>
+        <f>SUM(BPMCCS!C8,'MN IRP'!C25)</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>SUM(BPMCCS!D8,'MN IRP'!D34)</f>
+        <f>SUM(BPMCCS!D8,'MN IRP'!D25)</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>SUM(BPMCCS!E8,'MN IRP'!E34)</f>
+        <f>SUM(BPMCCS!E8,'MN IRP'!E25)</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>SUM(BPMCCS!F8,'MN IRP'!F34)</f>
+        <f>SUM(BPMCCS!F8,'MN IRP'!F25)</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>SUM(BPMCCS!G8,'MN IRP'!G34)</f>
+        <f>SUM(BPMCCS!G8,'MN IRP'!G25)</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>SUM(BPMCCS!H8,'MN IRP'!H34)</f>
+        <f>SUM(BPMCCS!H8,'MN IRP'!H25)</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>SUM(BPMCCS!I8,'MN IRP'!I34)</f>
+        <f>SUM(BPMCCS!I8,'MN IRP'!I25)</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>SUM(BPMCCS!J8,'MN IRP'!J34)</f>
+        <f>SUM(BPMCCS!J8,'MN IRP'!J25)</f>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>SUM(BPMCCS!K8,'MN IRP'!K34)</f>
+        <f>SUM(BPMCCS!K8,'MN IRP'!K25)</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>SUM(BPMCCS!L8,'MN IRP'!L34)</f>
+        <f>SUM(BPMCCS!L8,'MN IRP'!L25)</f>
         <v>0</v>
       </c>
       <c r="O8">
-        <f>SUM(BPMCCS!M8,'MN IRP'!M34)</f>
+        <f>SUM(BPMCCS!M8,'MN IRP'!M25)</f>
         <v>0</v>
       </c>
       <c r="P8">
-        <f>SUM(BPMCCS!N8,'MN IRP'!N34)</f>
+        <f>SUM(BPMCCS!N8,'MN IRP'!N25)</f>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>SUM(BPMCCS!O8,'MN IRP'!O34)</f>
+        <f>SUM(BPMCCS!O8,'MN IRP'!O25)</f>
         <v>0</v>
       </c>
       <c r="R8">
-        <f>SUM(BPMCCS!P8,'MN IRP'!P34)</f>
+        <f>SUM(BPMCCS!P8,'MN IRP'!P25)</f>
         <v>0</v>
       </c>
       <c r="S8">
-        <f>SUM(BPMCCS!Q8,'MN IRP'!Q34)</f>
+        <f>SUM(BPMCCS!Q8,'MN IRP'!Q25)</f>
         <v>0</v>
       </c>
       <c r="T8">
-        <f>SUM(BPMCCS!R8,'MN IRP'!R34)</f>
+        <f>SUM(BPMCCS!R8,'MN IRP'!R25)</f>
         <v>0</v>
       </c>
       <c r="U8">
-        <f>SUM(BPMCCS!S8,'MN IRP'!S34)</f>
+        <f>SUM(BPMCCS!S8,'MN IRP'!S25)</f>
         <v>0</v>
       </c>
       <c r="V8">
-        <f>SUM(BPMCCS!T8,'MN IRP'!T34)</f>
+        <f>SUM(BPMCCS!T8,'MN IRP'!T25)</f>
         <v>0</v>
       </c>
       <c r="W8">
-        <f>SUM(BPMCCS!U8,'MN IRP'!U34)</f>
+        <f>SUM(BPMCCS!U8,'MN IRP'!U25)</f>
         <v>0</v>
       </c>
       <c r="X8">
-        <f>SUM(BPMCCS!V8,'MN IRP'!V34)</f>
+        <f>SUM(BPMCCS!V8,'MN IRP'!V25)</f>
         <v>0</v>
       </c>
       <c r="Y8">
-        <f>SUM(BPMCCS!W8,'MN IRP'!W34)</f>
+        <f>SUM(BPMCCS!W8,'MN IRP'!W25)</f>
         <v>0</v>
       </c>
       <c r="Z8">
-        <f>SUM(BPMCCS!X8,'MN IRP'!X34)</f>
+        <f>SUM(BPMCCS!X8,'MN IRP'!X25)</f>
         <v>0</v>
       </c>
       <c r="AA8">
-        <f>SUM(BPMCCS!Y8,'MN IRP'!Y34)</f>
+        <f>SUM(BPMCCS!Y8,'MN IRP'!Y25)</f>
         <v>0</v>
       </c>
       <c r="AB8">
-        <f>SUM(BPMCCS!Z8,'MN IRP'!Z34)</f>
+        <f>SUM(BPMCCS!Z8,'MN IRP'!Z25)</f>
         <v>0</v>
       </c>
       <c r="AC8">
-        <f>SUM(BPMCCS!AA8,'MN IRP'!AA34)</f>
+        <f>SUM(BPMCCS!AA8,'MN IRP'!AA25)</f>
         <v>0</v>
       </c>
       <c r="AD8">
-        <f>SUM(BPMCCS!AB8,'MN IRP'!AB34)</f>
+        <f>SUM(BPMCCS!AB8,'MN IRP'!AB25)</f>
         <v>0</v>
       </c>
       <c r="AE8">
-        <f>SUM(BPMCCS!AC8,'MN IRP'!AC34)</f>
+        <f>SUM(BPMCCS!AC8,'MN IRP'!AC25)</f>
         <v>0</v>
       </c>
       <c r="AF8">
-        <f>SUM(BPMCCS!AD8,'MN IRP'!AD34)</f>
+        <f>SUM(BPMCCS!AD8,'MN IRP'!AD25)</f>
         <v>0</v>
       </c>
       <c r="AG8">
-        <f>SUM(BPMCCS!AE8,'MN IRP'!AE34)</f>
+        <f>SUM(BPMCCS!AE8,'MN IRP'!AE25)</f>
         <v>0</v>
       </c>
       <c r="AH8">
-        <f>SUM(BPMCCS!AF8,'MN IRP'!AF34)</f>
+        <f>SUM(BPMCCS!AF8,'MN IRP'!AF25)</f>
         <v>0</v>
       </c>
       <c r="AI8">
-        <f>SUM(BPMCCS!AG8,'MN IRP'!AG34)</f>
+        <f>SUM(BPMCCS!AG8,'MN IRP'!AG25)</f>
         <v>0</v>
       </c>
     </row>
@@ -3952,131 +3833,131 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>SUM(BPMCCS!B9,'MN IRP'!B35)</f>
+        <f>SUM(BPMCCS!B9,'MN IRP'!B26)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>SUM(BPMCCS!C9,'MN IRP'!C35)</f>
+        <f>SUM(BPMCCS!C9,'MN IRP'!C26)</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>SUM(BPMCCS!D9,'MN IRP'!D35)</f>
+        <f>SUM(BPMCCS!D9,'MN IRP'!D26)</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>SUM(BPMCCS!E9,'MN IRP'!E35)</f>
+        <f>SUM(BPMCCS!E9,'MN IRP'!E26)</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>SUM(BPMCCS!F9,'MN IRP'!F35)</f>
+        <f>SUM(BPMCCS!F9,'MN IRP'!F26)</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>SUM(BPMCCS!G9,'MN IRP'!G35)</f>
+        <f>SUM(BPMCCS!G9,'MN IRP'!G26)</f>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>SUM(BPMCCS!H9,'MN IRP'!H35)</f>
+        <f>SUM(BPMCCS!H9,'MN IRP'!H26)</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>SUM(BPMCCS!I9,'MN IRP'!I35)</f>
+        <f>SUM(BPMCCS!I9,'MN IRP'!I26)</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f>SUM(BPMCCS!J9,'MN IRP'!J35)</f>
+        <f>SUM(BPMCCS!J9,'MN IRP'!J26)</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>SUM(BPMCCS!K9,'MN IRP'!K35)</f>
+        <f>SUM(BPMCCS!K9,'MN IRP'!K26)</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>SUM(BPMCCS!L9,'MN IRP'!L35)</f>
+        <f>SUM(BPMCCS!L9,'MN IRP'!L26)</f>
         <v>0</v>
       </c>
       <c r="O9">
-        <f>SUM(BPMCCS!M9,'MN IRP'!M35)</f>
+        <f>SUM(BPMCCS!M9,'MN IRP'!M26)</f>
         <v>0</v>
       </c>
       <c r="P9">
-        <f>SUM(BPMCCS!N9,'MN IRP'!N35)</f>
+        <f>SUM(BPMCCS!N9,'MN IRP'!N26)</f>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>SUM(BPMCCS!O9,'MN IRP'!O35)</f>
+        <f>SUM(BPMCCS!O9,'MN IRP'!O26)</f>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>SUM(BPMCCS!P9,'MN IRP'!P35)</f>
+        <f>SUM(BPMCCS!P9,'MN IRP'!P26)</f>
         <v>0</v>
       </c>
       <c r="S9">
-        <f>SUM(BPMCCS!Q9,'MN IRP'!Q35)</f>
+        <f>SUM(BPMCCS!Q9,'MN IRP'!Q26)</f>
         <v>0</v>
       </c>
       <c r="T9">
-        <f>SUM(BPMCCS!R9,'MN IRP'!R35)</f>
+        <f>SUM(BPMCCS!R9,'MN IRP'!R26)</f>
         <v>0</v>
       </c>
       <c r="U9">
-        <f>SUM(BPMCCS!S9,'MN IRP'!S35)</f>
+        <f>SUM(BPMCCS!S9,'MN IRP'!S26)</f>
         <v>0</v>
       </c>
       <c r="V9">
-        <f>SUM(BPMCCS!T9,'MN IRP'!T35)</f>
+        <f>SUM(BPMCCS!T9,'MN IRP'!T26)</f>
         <v>0</v>
       </c>
       <c r="W9">
-        <f>SUM(BPMCCS!U9,'MN IRP'!U35)</f>
+        <f>SUM(BPMCCS!U9,'MN IRP'!U26)</f>
         <v>0</v>
       </c>
       <c r="X9">
-        <f>SUM(BPMCCS!V9,'MN IRP'!V35)</f>
+        <f>SUM(BPMCCS!V9,'MN IRP'!V26)</f>
         <v>0</v>
       </c>
       <c r="Y9">
-        <f>SUM(BPMCCS!W9,'MN IRP'!W35)</f>
+        <f>SUM(BPMCCS!W9,'MN IRP'!W26)</f>
         <v>0</v>
       </c>
       <c r="Z9">
-        <f>SUM(BPMCCS!X9,'MN IRP'!X35)</f>
+        <f>SUM(BPMCCS!X9,'MN IRP'!X26)</f>
         <v>0</v>
       </c>
       <c r="AA9">
-        <f>SUM(BPMCCS!Y9,'MN IRP'!Y35)</f>
+        <f>SUM(BPMCCS!Y9,'MN IRP'!Y26)</f>
         <v>0</v>
       </c>
       <c r="AB9">
-        <f>SUM(BPMCCS!Z9,'MN IRP'!Z35)</f>
+        <f>SUM(BPMCCS!Z9,'MN IRP'!Z26)</f>
         <v>0</v>
       </c>
       <c r="AC9">
-        <f>SUM(BPMCCS!AA9,'MN IRP'!AA35)</f>
+        <f>SUM(BPMCCS!AA9,'MN IRP'!AA26)</f>
         <v>0</v>
       </c>
       <c r="AD9">
-        <f>SUM(BPMCCS!AB9,'MN IRP'!AB35)</f>
+        <f>SUM(BPMCCS!AB9,'MN IRP'!AB26)</f>
         <v>0</v>
       </c>
       <c r="AE9">
-        <f>SUM(BPMCCS!AC9,'MN IRP'!AC35)</f>
+        <f>SUM(BPMCCS!AC9,'MN IRP'!AC26)</f>
         <v>0</v>
       </c>
       <c r="AF9">
-        <f>SUM(BPMCCS!AD9,'MN IRP'!AD35)</f>
+        <f>SUM(BPMCCS!AD9,'MN IRP'!AD26)</f>
         <v>0</v>
       </c>
       <c r="AG9">
-        <f>SUM(BPMCCS!AE9,'MN IRP'!AE35)</f>
+        <f>SUM(BPMCCS!AE9,'MN IRP'!AE26)</f>
         <v>0</v>
       </c>
       <c r="AH9">
-        <f>SUM(BPMCCS!AF9,'MN IRP'!AF35)</f>
+        <f>SUM(BPMCCS!AF9,'MN IRP'!AF26)</f>
         <v>0</v>
       </c>
       <c r="AI9">
-        <f>SUM(BPMCCS!AG9,'MN IRP'!AG35)</f>
+        <f>SUM(BPMCCS!AG9,'MN IRP'!AG26)</f>
         <v>0</v>
       </c>
     </row>
@@ -4091,131 +3972,131 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>SUM(BPMCCS!B10,'MN IRP'!B36)</f>
+        <f>SUM(BPMCCS!B10,'MN IRP'!B27)</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>SUM(BPMCCS!C10,'MN IRP'!C36)</f>
+        <f>SUM(BPMCCS!C10,'MN IRP'!C27)</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>SUM(BPMCCS!D10,'MN IRP'!D36)</f>
+        <f>SUM(BPMCCS!D10,'MN IRP'!D27)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>SUM(BPMCCS!E10,'MN IRP'!E36)</f>
+        <f>SUM(BPMCCS!E10,'MN IRP'!E27)</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>SUM(BPMCCS!F10,'MN IRP'!F36)</f>
+        <f>SUM(BPMCCS!F10,'MN IRP'!F27)</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>SUM(BPMCCS!G10,'MN IRP'!G36)</f>
+        <f>SUM(BPMCCS!G10,'MN IRP'!G27)</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>SUM(BPMCCS!H10,'MN IRP'!H36)</f>
+        <f>SUM(BPMCCS!H10,'MN IRP'!H27)</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>SUM(BPMCCS!I10,'MN IRP'!I36)</f>
+        <f>SUM(BPMCCS!I10,'MN IRP'!I27)</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>SUM(BPMCCS!J10,'MN IRP'!J36)</f>
+        <f>SUM(BPMCCS!J10,'MN IRP'!J27)</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>SUM(BPMCCS!K10,'MN IRP'!K36)</f>
+        <f>SUM(BPMCCS!K10,'MN IRP'!K27)</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>SUM(BPMCCS!L10,'MN IRP'!L36)</f>
+        <f>SUM(BPMCCS!L10,'MN IRP'!L27)</f>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>SUM(BPMCCS!M10,'MN IRP'!M36)</f>
+        <f>SUM(BPMCCS!M10,'MN IRP'!M27)</f>
         <v>0</v>
       </c>
       <c r="P10">
-        <f>SUM(BPMCCS!N10,'MN IRP'!N36)</f>
+        <f>SUM(BPMCCS!N10,'MN IRP'!N27)</f>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>SUM(BPMCCS!O10,'MN IRP'!O36)</f>
+        <f>SUM(BPMCCS!O10,'MN IRP'!O27)</f>
         <v>0</v>
       </c>
       <c r="R10">
-        <f>SUM(BPMCCS!P10,'MN IRP'!P36)</f>
+        <f>SUM(BPMCCS!P10,'MN IRP'!P27)</f>
         <v>0</v>
       </c>
       <c r="S10">
-        <f>SUM(BPMCCS!Q10,'MN IRP'!Q36)</f>
+        <f>SUM(BPMCCS!Q10,'MN IRP'!Q27)</f>
         <v>0</v>
       </c>
       <c r="T10">
-        <f>SUM(BPMCCS!R10,'MN IRP'!R36)</f>
+        <f>SUM(BPMCCS!R10,'MN IRP'!R27)</f>
         <v>0</v>
       </c>
       <c r="U10">
-        <f>SUM(BPMCCS!S10,'MN IRP'!S36)</f>
+        <f>SUM(BPMCCS!S10,'MN IRP'!S27)</f>
         <v>0</v>
       </c>
       <c r="V10">
-        <f>SUM(BPMCCS!T10,'MN IRP'!T36)</f>
+        <f>SUM(BPMCCS!T10,'MN IRP'!T27)</f>
         <v>0</v>
       </c>
       <c r="W10">
-        <f>SUM(BPMCCS!U10,'MN IRP'!U36)</f>
+        <f>SUM(BPMCCS!U10,'MN IRP'!U27)</f>
         <v>0</v>
       </c>
       <c r="X10">
-        <f>SUM(BPMCCS!V10,'MN IRP'!V36)</f>
+        <f>SUM(BPMCCS!V10,'MN IRP'!V27)</f>
         <v>0</v>
       </c>
       <c r="Y10">
-        <f>SUM(BPMCCS!W10,'MN IRP'!W36)</f>
+        <f>SUM(BPMCCS!W10,'MN IRP'!W27)</f>
         <v>0</v>
       </c>
       <c r="Z10">
-        <f>SUM(BPMCCS!X10,'MN IRP'!X36)</f>
+        <f>SUM(BPMCCS!X10,'MN IRP'!X27)</f>
         <v>0</v>
       </c>
       <c r="AA10">
-        <f>SUM(BPMCCS!Y10,'MN IRP'!Y36)</f>
+        <f>SUM(BPMCCS!Y10,'MN IRP'!Y27)</f>
         <v>0</v>
       </c>
       <c r="AB10">
-        <f>SUM(BPMCCS!Z10,'MN IRP'!Z36)</f>
+        <f>SUM(BPMCCS!Z10,'MN IRP'!Z27)</f>
         <v>0</v>
       </c>
       <c r="AC10">
-        <f>SUM(BPMCCS!AA10,'MN IRP'!AA36)</f>
+        <f>SUM(BPMCCS!AA10,'MN IRP'!AA27)</f>
         <v>0</v>
       </c>
       <c r="AD10">
-        <f>SUM(BPMCCS!AB10,'MN IRP'!AB36)</f>
+        <f>SUM(BPMCCS!AB10,'MN IRP'!AB27)</f>
         <v>0</v>
       </c>
       <c r="AE10">
-        <f>SUM(BPMCCS!AC10,'MN IRP'!AC36)</f>
+        <f>SUM(BPMCCS!AC10,'MN IRP'!AC27)</f>
         <v>0</v>
       </c>
       <c r="AF10">
-        <f>SUM(BPMCCS!AD10,'MN IRP'!AD36)</f>
+        <f>SUM(BPMCCS!AD10,'MN IRP'!AD27)</f>
         <v>0</v>
       </c>
       <c r="AG10">
-        <f>SUM(BPMCCS!AE10,'MN IRP'!AE36)</f>
+        <f>SUM(BPMCCS!AE10,'MN IRP'!AE27)</f>
         <v>0</v>
       </c>
       <c r="AH10">
-        <f>SUM(BPMCCS!AF10,'MN IRP'!AF36)</f>
+        <f>SUM(BPMCCS!AF10,'MN IRP'!AF27)</f>
         <v>0</v>
       </c>
       <c r="AI10">
-        <f>SUM(BPMCCS!AG10,'MN IRP'!AG36)</f>
+        <f>SUM(BPMCCS!AG10,'MN IRP'!AG27)</f>
         <v>0</v>
       </c>
     </row>
@@ -4230,131 +4111,131 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>SUM(BPMCCS!B11,'MN IRP'!B37)</f>
+        <f>SUM(BPMCCS!B11,'MN IRP'!B28)</f>
         <v>0</v>
       </c>
       <c r="E11">
-        <f>SUM(BPMCCS!C11,'MN IRP'!C37)</f>
+        <f>SUM(BPMCCS!C11,'MN IRP'!C28)</f>
         <v>0</v>
       </c>
       <c r="F11">
-        <f>SUM(BPMCCS!D11,'MN IRP'!D37)</f>
+        <f>SUM(BPMCCS!D11,'MN IRP'!D28)</f>
         <v>0</v>
       </c>
       <c r="G11">
-        <f>SUM(BPMCCS!E11,'MN IRP'!E37)</f>
+        <f>SUM(BPMCCS!E11,'MN IRP'!E28)</f>
         <v>0</v>
       </c>
       <c r="H11">
-        <f>SUM(BPMCCS!F11,'MN IRP'!F37)</f>
+        <f>SUM(BPMCCS!F11,'MN IRP'!F28)</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f>SUM(BPMCCS!G11,'MN IRP'!G37)</f>
+        <f>SUM(BPMCCS!G11,'MN IRP'!G28)</f>
         <v>0</v>
       </c>
       <c r="J11">
-        <f>SUM(BPMCCS!H11,'MN IRP'!H37)</f>
+        <f>SUM(BPMCCS!H11,'MN IRP'!H28)</f>
         <v>0</v>
       </c>
       <c r="K11">
-        <f>SUM(BPMCCS!I11,'MN IRP'!I37)</f>
+        <f>SUM(BPMCCS!I11,'MN IRP'!I28)</f>
         <v>0</v>
       </c>
       <c r="L11">
-        <f>SUM(BPMCCS!J11,'MN IRP'!J37)</f>
+        <f>SUM(BPMCCS!J11,'MN IRP'!J28)</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>SUM(BPMCCS!K11,'MN IRP'!K37)</f>
+        <f>SUM(BPMCCS!K11,'MN IRP'!K28)</f>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>SUM(BPMCCS!L11,'MN IRP'!L37)</f>
+        <f>SUM(BPMCCS!L11,'MN IRP'!L28)</f>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>SUM(BPMCCS!M11,'MN IRP'!M37)</f>
+        <f>SUM(BPMCCS!M11,'MN IRP'!M28)</f>
         <v>0</v>
       </c>
       <c r="P11">
-        <f>SUM(BPMCCS!N11,'MN IRP'!N37)</f>
+        <f>SUM(BPMCCS!N11,'MN IRP'!N28)</f>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>SUM(BPMCCS!O11,'MN IRP'!O37)</f>
+        <f>SUM(BPMCCS!O11,'MN IRP'!O28)</f>
         <v>0</v>
       </c>
       <c r="R11">
-        <f>SUM(BPMCCS!P11,'MN IRP'!P37)</f>
+        <f>SUM(BPMCCS!P11,'MN IRP'!P28)</f>
         <v>0</v>
       </c>
       <c r="S11">
-        <f>SUM(BPMCCS!Q11,'MN IRP'!Q37)</f>
+        <f>SUM(BPMCCS!Q11,'MN IRP'!Q28)</f>
         <v>0</v>
       </c>
       <c r="T11">
-        <f>SUM(BPMCCS!R11,'MN IRP'!R37)</f>
+        <f>SUM(BPMCCS!R11,'MN IRP'!R28)</f>
         <v>0</v>
       </c>
       <c r="U11">
-        <f>SUM(BPMCCS!S11,'MN IRP'!S37)</f>
+        <f>SUM(BPMCCS!S11,'MN IRP'!S28)</f>
         <v>0</v>
       </c>
       <c r="V11">
-        <f>SUM(BPMCCS!T11,'MN IRP'!T37)</f>
+        <f>SUM(BPMCCS!T11,'MN IRP'!T28)</f>
         <v>0</v>
       </c>
       <c r="W11">
-        <f>SUM(BPMCCS!U11,'MN IRP'!U37)</f>
+        <f>SUM(BPMCCS!U11,'MN IRP'!U28)</f>
         <v>0</v>
       </c>
       <c r="X11">
-        <f>SUM(BPMCCS!V11,'MN IRP'!V37)</f>
+        <f>SUM(BPMCCS!V11,'MN IRP'!V28)</f>
         <v>0</v>
       </c>
       <c r="Y11">
-        <f>SUM(BPMCCS!W11,'MN IRP'!W37)</f>
+        <f>SUM(BPMCCS!W11,'MN IRP'!W28)</f>
         <v>0</v>
       </c>
       <c r="Z11">
-        <f>SUM(BPMCCS!X11,'MN IRP'!X37)</f>
+        <f>SUM(BPMCCS!X11,'MN IRP'!X28)</f>
         <v>0</v>
       </c>
       <c r="AA11">
-        <f>SUM(BPMCCS!Y11,'MN IRP'!Y37)</f>
+        <f>SUM(BPMCCS!Y11,'MN IRP'!Y28)</f>
         <v>0</v>
       </c>
       <c r="AB11">
-        <f>SUM(BPMCCS!Z11,'MN IRP'!Z37)</f>
+        <f>SUM(BPMCCS!Z11,'MN IRP'!Z28)</f>
         <v>0</v>
       </c>
       <c r="AC11">
-        <f>SUM(BPMCCS!AA11,'MN IRP'!AA37)</f>
+        <f>SUM(BPMCCS!AA11,'MN IRP'!AA28)</f>
         <v>0</v>
       </c>
       <c r="AD11">
-        <f>SUM(BPMCCS!AB11,'MN IRP'!AB37)</f>
+        <f>SUM(BPMCCS!AB11,'MN IRP'!AB28)</f>
         <v>0</v>
       </c>
       <c r="AE11">
-        <f>SUM(BPMCCS!AC11,'MN IRP'!AC37)</f>
+        <f>SUM(BPMCCS!AC11,'MN IRP'!AC28)</f>
         <v>0</v>
       </c>
       <c r="AF11">
-        <f>SUM(BPMCCS!AD11,'MN IRP'!AD37)</f>
+        <f>SUM(BPMCCS!AD11,'MN IRP'!AD28)</f>
         <v>0</v>
       </c>
       <c r="AG11">
-        <f>SUM(BPMCCS!AE11,'MN IRP'!AE37)</f>
+        <f>SUM(BPMCCS!AE11,'MN IRP'!AE28)</f>
         <v>0</v>
       </c>
       <c r="AH11">
-        <f>SUM(BPMCCS!AF11,'MN IRP'!AF37)</f>
+        <f>SUM(BPMCCS!AF11,'MN IRP'!AF28)</f>
         <v>0</v>
       </c>
       <c r="AI11">
-        <f>SUM(BPMCCS!AG11,'MN IRP'!AG37)</f>
+        <f>SUM(BPMCCS!AG11,'MN IRP'!AG28)</f>
         <v>0</v>
       </c>
     </row>
@@ -4369,131 +4250,131 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>SUM(BPMCCS!B12,'MN IRP'!B38)</f>
+        <f>SUM(BPMCCS!B12,'MN IRP'!B29)</f>
         <v>0</v>
       </c>
       <c r="E12">
-        <f>SUM(BPMCCS!C12,'MN IRP'!C38)</f>
+        <f>SUM(BPMCCS!C12,'MN IRP'!C29)</f>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>SUM(BPMCCS!D12,'MN IRP'!D38)</f>
+        <f>SUM(BPMCCS!D12,'MN IRP'!D29)</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <f>SUM(BPMCCS!E12,'MN IRP'!E38)</f>
+        <f>SUM(BPMCCS!E12,'MN IRP'!E29)</f>
         <v>0</v>
       </c>
       <c r="H12">
-        <f>SUM(BPMCCS!F12,'MN IRP'!F38)</f>
+        <f>SUM(BPMCCS!F12,'MN IRP'!F29)</f>
         <v>0</v>
       </c>
       <c r="I12">
-        <f>SUM(BPMCCS!G12,'MN IRP'!G38)</f>
+        <f>SUM(BPMCCS!G12,'MN IRP'!G29)</f>
         <v>0</v>
       </c>
       <c r="J12">
-        <f>SUM(BPMCCS!H12,'MN IRP'!H38)</f>
+        <f>SUM(BPMCCS!H12,'MN IRP'!H29)</f>
         <v>0</v>
       </c>
       <c r="K12">
-        <f>SUM(BPMCCS!I12,'MN IRP'!I38)</f>
+        <f>SUM(BPMCCS!I12,'MN IRP'!I29)</f>
         <v>0</v>
       </c>
       <c r="L12">
-        <f>SUM(BPMCCS!J12,'MN IRP'!J38)</f>
+        <f>SUM(BPMCCS!J12,'MN IRP'!J29)</f>
         <v>0</v>
       </c>
       <c r="M12">
-        <f>SUM(BPMCCS!K12,'MN IRP'!K38)</f>
+        <f>SUM(BPMCCS!K12,'MN IRP'!K29)</f>
         <v>0</v>
       </c>
       <c r="N12">
-        <f>SUM(BPMCCS!L12,'MN IRP'!L38)</f>
+        <f>SUM(BPMCCS!L12,'MN IRP'!L29)</f>
         <v>0</v>
       </c>
       <c r="O12">
-        <f>SUM(BPMCCS!M12,'MN IRP'!M38)</f>
+        <f>SUM(BPMCCS!M12,'MN IRP'!M29)</f>
         <v>0</v>
       </c>
       <c r="P12">
-        <f>SUM(BPMCCS!N12,'MN IRP'!N38)</f>
+        <f>SUM(BPMCCS!N12,'MN IRP'!N29)</f>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>SUM(BPMCCS!O12,'MN IRP'!O38)</f>
+        <f>SUM(BPMCCS!O12,'MN IRP'!O29)</f>
         <v>0</v>
       </c>
       <c r="R12">
-        <f>SUM(BPMCCS!P12,'MN IRP'!P38)</f>
+        <f>SUM(BPMCCS!P12,'MN IRP'!P29)</f>
         <v>0</v>
       </c>
       <c r="S12">
-        <f>SUM(BPMCCS!Q12,'MN IRP'!Q38)</f>
+        <f>SUM(BPMCCS!Q12,'MN IRP'!Q29)</f>
         <v>0</v>
       </c>
       <c r="T12">
-        <f>SUM(BPMCCS!R12,'MN IRP'!R38)</f>
+        <f>SUM(BPMCCS!R12,'MN IRP'!R29)</f>
         <v>0</v>
       </c>
       <c r="U12">
-        <f>SUM(BPMCCS!S12,'MN IRP'!S38)</f>
+        <f>SUM(BPMCCS!S12,'MN IRP'!S29)</f>
         <v>0</v>
       </c>
       <c r="V12">
-        <f>SUM(BPMCCS!T12,'MN IRP'!T38)</f>
+        <f>SUM(BPMCCS!T12,'MN IRP'!T29)</f>
         <v>0</v>
       </c>
       <c r="W12">
-        <f>SUM(BPMCCS!U12,'MN IRP'!U38)</f>
+        <f>SUM(BPMCCS!U12,'MN IRP'!U29)</f>
         <v>0</v>
       </c>
       <c r="X12">
-        <f>SUM(BPMCCS!V12,'MN IRP'!V38)</f>
+        <f>SUM(BPMCCS!V12,'MN IRP'!V29)</f>
         <v>0</v>
       </c>
       <c r="Y12">
-        <f>SUM(BPMCCS!W12,'MN IRP'!W38)</f>
+        <f>SUM(BPMCCS!W12,'MN IRP'!W29)</f>
         <v>0</v>
       </c>
       <c r="Z12">
-        <f>SUM(BPMCCS!X12,'MN IRP'!X38)</f>
+        <f>SUM(BPMCCS!X12,'MN IRP'!X29)</f>
         <v>0</v>
       </c>
       <c r="AA12">
-        <f>SUM(BPMCCS!Y12,'MN IRP'!Y38)</f>
+        <f>SUM(BPMCCS!Y12,'MN IRP'!Y29)</f>
         <v>0</v>
       </c>
       <c r="AB12">
-        <f>SUM(BPMCCS!Z12,'MN IRP'!Z38)</f>
+        <f>SUM(BPMCCS!Z12,'MN IRP'!Z29)</f>
         <v>0</v>
       </c>
       <c r="AC12">
-        <f>SUM(BPMCCS!AA12,'MN IRP'!AA38)</f>
+        <f>SUM(BPMCCS!AA12,'MN IRP'!AA29)</f>
         <v>0</v>
       </c>
       <c r="AD12">
-        <f>SUM(BPMCCS!AB12,'MN IRP'!AB38)</f>
+        <f>SUM(BPMCCS!AB12,'MN IRP'!AB29)</f>
         <v>0</v>
       </c>
       <c r="AE12">
-        <f>SUM(BPMCCS!AC12,'MN IRP'!AC38)</f>
+        <f>SUM(BPMCCS!AC12,'MN IRP'!AC29)</f>
         <v>0</v>
       </c>
       <c r="AF12">
-        <f>SUM(BPMCCS!AD12,'MN IRP'!AD38)</f>
+        <f>SUM(BPMCCS!AD12,'MN IRP'!AD29)</f>
         <v>0</v>
       </c>
       <c r="AG12">
-        <f>SUM(BPMCCS!AE12,'MN IRP'!AE38)</f>
+        <f>SUM(BPMCCS!AE12,'MN IRP'!AE29)</f>
         <v>0</v>
       </c>
       <c r="AH12">
-        <f>SUM(BPMCCS!AF12,'MN IRP'!AF38)</f>
+        <f>SUM(BPMCCS!AF12,'MN IRP'!AF29)</f>
         <v>0</v>
       </c>
       <c r="AI12">
-        <f>SUM(BPMCCS!AG12,'MN IRP'!AG38)</f>
+        <f>SUM(BPMCCS!AG12,'MN IRP'!AG29)</f>
         <v>0</v>
       </c>
     </row>
@@ -4508,131 +4389,131 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f>SUM(BPMCCS!B13,'MN IRP'!B39)</f>
+        <f>SUM(BPMCCS!B13,'MN IRP'!B30)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>SUM(BPMCCS!C13,'MN IRP'!C39)</f>
+        <f>SUM(BPMCCS!C13,'MN IRP'!C30)</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>SUM(BPMCCS!D13,'MN IRP'!D39)</f>
+        <f>SUM(BPMCCS!D13,'MN IRP'!D30)</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>SUM(BPMCCS!E13,'MN IRP'!E39)</f>
+        <f>SUM(BPMCCS!E13,'MN IRP'!E30)</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>SUM(BPMCCS!F13,'MN IRP'!F39)</f>
+        <f>SUM(BPMCCS!F13,'MN IRP'!F30)</f>
         <v>0</v>
       </c>
       <c r="I13">
-        <f>SUM(BPMCCS!G13,'MN IRP'!G39)</f>
+        <f>SUM(BPMCCS!G13,'MN IRP'!G30)</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>SUM(BPMCCS!H13,'MN IRP'!H39)</f>
+        <f>SUM(BPMCCS!H13,'MN IRP'!H30)</f>
         <v>0</v>
       </c>
       <c r="K13">
-        <f>SUM(BPMCCS!I13,'MN IRP'!I39)</f>
+        <f>SUM(BPMCCS!I13,'MN IRP'!I30)</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f>SUM(BPMCCS!J13,'MN IRP'!J39)</f>
+        <f>SUM(BPMCCS!J13,'MN IRP'!J30)</f>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>SUM(BPMCCS!K13,'MN IRP'!K39)</f>
+        <f>SUM(BPMCCS!K13,'MN IRP'!K30)</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>SUM(BPMCCS!L13,'MN IRP'!L39)</f>
+        <f>SUM(BPMCCS!L13,'MN IRP'!L30)</f>
         <v>0</v>
       </c>
       <c r="O13">
-        <f>SUM(BPMCCS!M13,'MN IRP'!M39)</f>
+        <f>SUM(BPMCCS!M13,'MN IRP'!M30)</f>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>SUM(BPMCCS!N13,'MN IRP'!N39)</f>
+        <f>SUM(BPMCCS!N13,'MN IRP'!N30)</f>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>SUM(BPMCCS!O13,'MN IRP'!O39)</f>
+        <f>SUM(BPMCCS!O13,'MN IRP'!O30)</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>SUM(BPMCCS!P13,'MN IRP'!P39)</f>
+        <f>SUM(BPMCCS!P13,'MN IRP'!P30)</f>
         <v>0</v>
       </c>
       <c r="S13">
-        <f>SUM(BPMCCS!Q13,'MN IRP'!Q39)</f>
+        <f>SUM(BPMCCS!Q13,'MN IRP'!Q30)</f>
         <v>0</v>
       </c>
       <c r="T13">
-        <f>SUM(BPMCCS!R13,'MN IRP'!R39)</f>
+        <f>SUM(BPMCCS!R13,'MN IRP'!R30)</f>
         <v>0</v>
       </c>
       <c r="U13">
-        <f>SUM(BPMCCS!S13,'MN IRP'!S39)</f>
+        <f>SUM(BPMCCS!S13,'MN IRP'!S30)</f>
         <v>0</v>
       </c>
       <c r="V13">
-        <f>SUM(BPMCCS!T13,'MN IRP'!T39)</f>
+        <f>SUM(BPMCCS!T13,'MN IRP'!T30)</f>
         <v>0</v>
       </c>
       <c r="W13">
-        <f>SUM(BPMCCS!U13,'MN IRP'!U39)</f>
+        <f>SUM(BPMCCS!U13,'MN IRP'!U30)</f>
         <v>0</v>
       </c>
       <c r="X13">
-        <f>SUM(BPMCCS!V13,'MN IRP'!V39)</f>
+        <f>SUM(BPMCCS!V13,'MN IRP'!V30)</f>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f>SUM(BPMCCS!W13,'MN IRP'!W39)</f>
+        <f>SUM(BPMCCS!W13,'MN IRP'!W30)</f>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f>SUM(BPMCCS!X13,'MN IRP'!X39)</f>
+        <f>SUM(BPMCCS!X13,'MN IRP'!X30)</f>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f>SUM(BPMCCS!Y13,'MN IRP'!Y39)</f>
+        <f>SUM(BPMCCS!Y13,'MN IRP'!Y30)</f>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f>SUM(BPMCCS!Z13,'MN IRP'!Z39)</f>
+        <f>SUM(BPMCCS!Z13,'MN IRP'!Z30)</f>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f>SUM(BPMCCS!AA13,'MN IRP'!AA39)</f>
+        <f>SUM(BPMCCS!AA13,'MN IRP'!AA30)</f>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f>SUM(BPMCCS!AB13,'MN IRP'!AB39)</f>
+        <f>SUM(BPMCCS!AB13,'MN IRP'!AB30)</f>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f>SUM(BPMCCS!AC13,'MN IRP'!AC39)</f>
+        <f>SUM(BPMCCS!AC13,'MN IRP'!AC30)</f>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f>SUM(BPMCCS!AD13,'MN IRP'!AD39)</f>
+        <f>SUM(BPMCCS!AD13,'MN IRP'!AD30)</f>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f>SUM(BPMCCS!AE13,'MN IRP'!AE39)</f>
+        <f>SUM(BPMCCS!AE13,'MN IRP'!AE30)</f>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f>SUM(BPMCCS!AF13,'MN IRP'!AF39)</f>
+        <f>SUM(BPMCCS!AF13,'MN IRP'!AF30)</f>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f>SUM(BPMCCS!AG13,'MN IRP'!AG39)</f>
+        <f>SUM(BPMCCS!AG13,'MN IRP'!AG30)</f>
         <v>0</v>
       </c>
     </row>
@@ -4647,131 +4528,131 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>SUM(BPMCCS!B14,'MN IRP'!B40)</f>
+        <f>SUM(BPMCCS!B14,'MN IRP'!B31)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>SUM(BPMCCS!C14,'MN IRP'!C40)</f>
+        <f>SUM(BPMCCS!C14,'MN IRP'!C31)</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>SUM(BPMCCS!D14,'MN IRP'!D40)</f>
+        <f>SUM(BPMCCS!D14,'MN IRP'!D31)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>SUM(BPMCCS!E14,'MN IRP'!E40)</f>
+        <f>SUM(BPMCCS!E14,'MN IRP'!E31)</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f>SUM(BPMCCS!F14,'MN IRP'!F40)</f>
+        <f>SUM(BPMCCS!F14,'MN IRP'!F31)</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>SUM(BPMCCS!G14,'MN IRP'!G40)</f>
+        <f>SUM(BPMCCS!G14,'MN IRP'!G31)</f>
         <v>0</v>
       </c>
       <c r="J14">
-        <f>SUM(BPMCCS!H14,'MN IRP'!H40)</f>
+        <f>SUM(BPMCCS!H14,'MN IRP'!H31)</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>SUM(BPMCCS!I14,'MN IRP'!I40)</f>
+        <f>SUM(BPMCCS!I14,'MN IRP'!I31)</f>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>SUM(BPMCCS!J14,'MN IRP'!J40)</f>
+        <f>SUM(BPMCCS!J14,'MN IRP'!J31)</f>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>SUM(BPMCCS!K14,'MN IRP'!K40)</f>
+        <f>SUM(BPMCCS!K14,'MN IRP'!K31)</f>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>SUM(BPMCCS!L14,'MN IRP'!L40)</f>
+        <f>SUM(BPMCCS!L14,'MN IRP'!L31)</f>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>SUM(BPMCCS!M14,'MN IRP'!M40)</f>
+        <f>SUM(BPMCCS!M14,'MN IRP'!M31)</f>
         <v>0</v>
       </c>
       <c r="P14">
-        <f>SUM(BPMCCS!N14,'MN IRP'!N40)</f>
+        <f>SUM(BPMCCS!N14,'MN IRP'!N31)</f>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>SUM(BPMCCS!O14,'MN IRP'!O40)</f>
+        <f>SUM(BPMCCS!O14,'MN IRP'!O31)</f>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>SUM(BPMCCS!P14,'MN IRP'!P40)</f>
+        <f>SUM(BPMCCS!P14,'MN IRP'!P31)</f>
         <v>0</v>
       </c>
       <c r="S14">
-        <f>SUM(BPMCCS!Q14,'MN IRP'!Q40)</f>
+        <f>SUM(BPMCCS!Q14,'MN IRP'!Q31)</f>
         <v>0</v>
       </c>
       <c r="T14">
-        <f>SUM(BPMCCS!R14,'MN IRP'!R40)</f>
+        <f>SUM(BPMCCS!R14,'MN IRP'!R31)</f>
         <v>0</v>
       </c>
       <c r="U14">
-        <f>SUM(BPMCCS!S14,'MN IRP'!S40)</f>
+        <f>SUM(BPMCCS!S14,'MN IRP'!S31)</f>
         <v>0</v>
       </c>
       <c r="V14">
-        <f>SUM(BPMCCS!T14,'MN IRP'!T40)</f>
+        <f>SUM(BPMCCS!T14,'MN IRP'!T31)</f>
         <v>0</v>
       </c>
       <c r="W14">
-        <f>SUM(BPMCCS!U14,'MN IRP'!U40)</f>
+        <f>SUM(BPMCCS!U14,'MN IRP'!U31)</f>
         <v>0</v>
       </c>
       <c r="X14">
-        <f>SUM(BPMCCS!V14,'MN IRP'!V40)</f>
+        <f>SUM(BPMCCS!V14,'MN IRP'!V31)</f>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f>SUM(BPMCCS!W14,'MN IRP'!W40)</f>
+        <f>SUM(BPMCCS!W14,'MN IRP'!W31)</f>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f>SUM(BPMCCS!X14,'MN IRP'!X40)</f>
+        <f>SUM(BPMCCS!X14,'MN IRP'!X31)</f>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f>SUM(BPMCCS!Y14,'MN IRP'!Y40)</f>
+        <f>SUM(BPMCCS!Y14,'MN IRP'!Y31)</f>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f>SUM(BPMCCS!Z14,'MN IRP'!Z40)</f>
+        <f>SUM(BPMCCS!Z14,'MN IRP'!Z31)</f>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f>SUM(BPMCCS!AA14,'MN IRP'!AA40)</f>
+        <f>SUM(BPMCCS!AA14,'MN IRP'!AA31)</f>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f>SUM(BPMCCS!AB14,'MN IRP'!AB40)</f>
+        <f>SUM(BPMCCS!AB14,'MN IRP'!AB31)</f>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f>SUM(BPMCCS!AC14,'MN IRP'!AC40)</f>
+        <f>SUM(BPMCCS!AC14,'MN IRP'!AC31)</f>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f>SUM(BPMCCS!AD14,'MN IRP'!AD40)</f>
+        <f>SUM(BPMCCS!AD14,'MN IRP'!AD31)</f>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f>SUM(BPMCCS!AE14,'MN IRP'!AE40)</f>
+        <f>SUM(BPMCCS!AE14,'MN IRP'!AE31)</f>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f>SUM(BPMCCS!AF14,'MN IRP'!AF40)</f>
+        <f>SUM(BPMCCS!AF14,'MN IRP'!AF31)</f>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f>SUM(BPMCCS!AG14,'MN IRP'!AG40)</f>
+        <f>SUM(BPMCCS!AG14,'MN IRP'!AG31)</f>
         <v>0</v>
       </c>
     </row>
@@ -4786,131 +4667,131 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f>SUM(BPMCCS!B15,'MN IRP'!B41)</f>
+        <f>SUM(BPMCCS!B15,'MN IRP'!B32)</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>SUM(BPMCCS!C15,'MN IRP'!C41)</f>
+        <f>SUM(BPMCCS!C15,'MN IRP'!C32)</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>SUM(BPMCCS!D15,'MN IRP'!D41)</f>
+        <f>SUM(BPMCCS!D15,'MN IRP'!D32)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>SUM(BPMCCS!E15,'MN IRP'!E41)</f>
+        <f>SUM(BPMCCS!E15,'MN IRP'!E32)</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>SUM(BPMCCS!F15,'MN IRP'!F41)</f>
+        <f>SUM(BPMCCS!F15,'MN IRP'!F32)</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>SUM(BPMCCS!G15,'MN IRP'!G41)</f>
+        <f>SUM(BPMCCS!G15,'MN IRP'!G32)</f>
         <v>0</v>
       </c>
       <c r="J15">
-        <f>SUM(BPMCCS!H15,'MN IRP'!H41)</f>
+        <f>SUM(BPMCCS!H15,'MN IRP'!H32)</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>SUM(BPMCCS!I15,'MN IRP'!I41)</f>
+        <f>SUM(BPMCCS!I15,'MN IRP'!I32)</f>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>SUM(BPMCCS!J15,'MN IRP'!J41)</f>
+        <f>SUM(BPMCCS!J15,'MN IRP'!J32)</f>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>SUM(BPMCCS!K15,'MN IRP'!K41)</f>
+        <f>SUM(BPMCCS!K15,'MN IRP'!K32)</f>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>SUM(BPMCCS!L15,'MN IRP'!L41)</f>
+        <f>SUM(BPMCCS!L15,'MN IRP'!L32)</f>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>SUM(BPMCCS!M15,'MN IRP'!M41)</f>
+        <f>SUM(BPMCCS!M15,'MN IRP'!M32)</f>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>SUM(BPMCCS!N15,'MN IRP'!N41)</f>
+        <f>SUM(BPMCCS!N15,'MN IRP'!N32)</f>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>SUM(BPMCCS!O15,'MN IRP'!O41)</f>
+        <f>SUM(BPMCCS!O15,'MN IRP'!O32)</f>
         <v>0</v>
       </c>
       <c r="R15">
-        <f>SUM(BPMCCS!P15,'MN IRP'!P41)</f>
+        <f>SUM(BPMCCS!P15,'MN IRP'!P32)</f>
         <v>0</v>
       </c>
       <c r="S15">
-        <f>SUM(BPMCCS!Q15,'MN IRP'!Q41)</f>
+        <f>SUM(BPMCCS!Q15,'MN IRP'!Q32)</f>
         <v>0</v>
       </c>
       <c r="T15">
-        <f>SUM(BPMCCS!R15,'MN IRP'!R41)</f>
+        <f>SUM(BPMCCS!R15,'MN IRP'!R32)</f>
         <v>0</v>
       </c>
       <c r="U15">
-        <f>SUM(BPMCCS!S15,'MN IRP'!S41)</f>
+        <f>SUM(BPMCCS!S15,'MN IRP'!S32)</f>
         <v>0</v>
       </c>
       <c r="V15">
-        <f>SUM(BPMCCS!T15,'MN IRP'!T41)</f>
+        <f>SUM(BPMCCS!T15,'MN IRP'!T32)</f>
         <v>0</v>
       </c>
       <c r="W15">
-        <f>SUM(BPMCCS!U15,'MN IRP'!U41)</f>
+        <f>SUM(BPMCCS!U15,'MN IRP'!U32)</f>
         <v>0</v>
       </c>
       <c r="X15">
-        <f>SUM(BPMCCS!V15,'MN IRP'!V41)</f>
+        <f>SUM(BPMCCS!V15,'MN IRP'!V32)</f>
         <v>0</v>
       </c>
       <c r="Y15">
-        <f>SUM(BPMCCS!W15,'MN IRP'!W41)</f>
+        <f>SUM(BPMCCS!W15,'MN IRP'!W32)</f>
         <v>0</v>
       </c>
       <c r="Z15">
-        <f>SUM(BPMCCS!X15,'MN IRP'!X41)</f>
+        <f>SUM(BPMCCS!X15,'MN IRP'!X32)</f>
         <v>0</v>
       </c>
       <c r="AA15">
-        <f>SUM(BPMCCS!Y15,'MN IRP'!Y41)</f>
+        <f>SUM(BPMCCS!Y15,'MN IRP'!Y32)</f>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f>SUM(BPMCCS!Z15,'MN IRP'!Z41)</f>
+        <f>SUM(BPMCCS!Z15,'MN IRP'!Z32)</f>
         <v>0</v>
       </c>
       <c r="AC15">
-        <f>SUM(BPMCCS!AA15,'MN IRP'!AA41)</f>
+        <f>SUM(BPMCCS!AA15,'MN IRP'!AA32)</f>
         <v>0</v>
       </c>
       <c r="AD15">
-        <f>SUM(BPMCCS!AB15,'MN IRP'!AB41)</f>
+        <f>SUM(BPMCCS!AB15,'MN IRP'!AB32)</f>
         <v>0</v>
       </c>
       <c r="AE15">
-        <f>SUM(BPMCCS!AC15,'MN IRP'!AC41)</f>
+        <f>SUM(BPMCCS!AC15,'MN IRP'!AC32)</f>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f>SUM(BPMCCS!AD15,'MN IRP'!AD41)</f>
+        <f>SUM(BPMCCS!AD15,'MN IRP'!AD32)</f>
         <v>0</v>
       </c>
       <c r="AG15">
-        <f>SUM(BPMCCS!AE15,'MN IRP'!AE41)</f>
+        <f>SUM(BPMCCS!AE15,'MN IRP'!AE32)</f>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f>SUM(BPMCCS!AF15,'MN IRP'!AF41)</f>
+        <f>SUM(BPMCCS!AF15,'MN IRP'!AF32)</f>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f>SUM(BPMCCS!AG15,'MN IRP'!AG41)</f>
+        <f>SUM(BPMCCS!AG15,'MN IRP'!AG32)</f>
         <v>0</v>
       </c>
     </row>
@@ -4925,131 +4806,131 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f>SUM(BPMCCS!B16,'MN IRP'!B42)</f>
+        <f>SUM(BPMCCS!B16,'MN IRP'!B33)</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>SUM(BPMCCS!C16,'MN IRP'!C42)</f>
+        <f>SUM(BPMCCS!C16,'MN IRP'!C33)</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>SUM(BPMCCS!D16,'MN IRP'!D42)</f>
+        <f>SUM(BPMCCS!D16,'MN IRP'!D33)</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>SUM(BPMCCS!E16,'MN IRP'!E42)</f>
+        <f>SUM(BPMCCS!E16,'MN IRP'!E33)</f>
         <v>0</v>
       </c>
       <c r="H16">
-        <f>SUM(BPMCCS!F16,'MN IRP'!F42)</f>
+        <f>SUM(BPMCCS!F16,'MN IRP'!F33)</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>SUM(BPMCCS!G16,'MN IRP'!G42)</f>
+        <f>SUM(BPMCCS!G16,'MN IRP'!G33)</f>
         <v>0</v>
       </c>
       <c r="J16">
-        <f>SUM(BPMCCS!H16,'MN IRP'!H42)</f>
+        <f>SUM(BPMCCS!H16,'MN IRP'!H33)</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f>SUM(BPMCCS!I16,'MN IRP'!I42)</f>
+        <f>SUM(BPMCCS!I16,'MN IRP'!I33)</f>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>SUM(BPMCCS!J16,'MN IRP'!J42)</f>
+        <f>SUM(BPMCCS!J16,'MN IRP'!J33)</f>
         <v>0</v>
       </c>
       <c r="M16">
-        <f>SUM(BPMCCS!K16,'MN IRP'!K42)</f>
+        <f>SUM(BPMCCS!K16,'MN IRP'!K33)</f>
         <v>0</v>
       </c>
       <c r="N16">
-        <f>SUM(BPMCCS!L16,'MN IRP'!L42)</f>
+        <f>SUM(BPMCCS!L16,'MN IRP'!L33)</f>
         <v>0</v>
       </c>
       <c r="O16">
-        <f>SUM(BPMCCS!M16,'MN IRP'!M42)</f>
+        <f>SUM(BPMCCS!M16,'MN IRP'!M33)</f>
         <v>0</v>
       </c>
       <c r="P16">
-        <f>SUM(BPMCCS!N16,'MN IRP'!N42)</f>
+        <f>SUM(BPMCCS!N16,'MN IRP'!N33)</f>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>SUM(BPMCCS!O16,'MN IRP'!O42)</f>
+        <f>SUM(BPMCCS!O16,'MN IRP'!O33)</f>
         <v>0</v>
       </c>
       <c r="R16">
-        <f>SUM(BPMCCS!P16,'MN IRP'!P42)</f>
+        <f>SUM(BPMCCS!P16,'MN IRP'!P33)</f>
         <v>0</v>
       </c>
       <c r="S16">
-        <f>SUM(BPMCCS!Q16,'MN IRP'!Q42)</f>
+        <f>SUM(BPMCCS!Q16,'MN IRP'!Q33)</f>
         <v>0</v>
       </c>
       <c r="T16">
-        <f>SUM(BPMCCS!R16,'MN IRP'!R42)</f>
+        <f>SUM(BPMCCS!R16,'MN IRP'!R33)</f>
         <v>0</v>
       </c>
       <c r="U16">
-        <f>SUM(BPMCCS!S16,'MN IRP'!S42)</f>
+        <f>SUM(BPMCCS!S16,'MN IRP'!S33)</f>
         <v>0</v>
       </c>
       <c r="V16">
-        <f>SUM(BPMCCS!T16,'MN IRP'!T42)</f>
+        <f>SUM(BPMCCS!T16,'MN IRP'!T33)</f>
         <v>0</v>
       </c>
       <c r="W16">
-        <f>SUM(BPMCCS!U16,'MN IRP'!U42)</f>
+        <f>SUM(BPMCCS!U16,'MN IRP'!U33)</f>
         <v>0</v>
       </c>
       <c r="X16">
-        <f>SUM(BPMCCS!V16,'MN IRP'!V42)</f>
+        <f>SUM(BPMCCS!V16,'MN IRP'!V33)</f>
         <v>0</v>
       </c>
       <c r="Y16">
-        <f>SUM(BPMCCS!W16,'MN IRP'!W42)</f>
+        <f>SUM(BPMCCS!W16,'MN IRP'!W33)</f>
         <v>0</v>
       </c>
       <c r="Z16">
-        <f>SUM(BPMCCS!X16,'MN IRP'!X42)</f>
+        <f>SUM(BPMCCS!X16,'MN IRP'!X33)</f>
         <v>0</v>
       </c>
       <c r="AA16">
-        <f>SUM(BPMCCS!Y16,'MN IRP'!Y42)</f>
+        <f>SUM(BPMCCS!Y16,'MN IRP'!Y33)</f>
         <v>0</v>
       </c>
       <c r="AB16">
-        <f>SUM(BPMCCS!Z16,'MN IRP'!Z42)</f>
+        <f>SUM(BPMCCS!Z16,'MN IRP'!Z33)</f>
         <v>0</v>
       </c>
       <c r="AC16">
-        <f>SUM(BPMCCS!AA16,'MN IRP'!AA42)</f>
+        <f>SUM(BPMCCS!AA16,'MN IRP'!AA33)</f>
         <v>0</v>
       </c>
       <c r="AD16">
-        <f>SUM(BPMCCS!AB16,'MN IRP'!AB42)</f>
+        <f>SUM(BPMCCS!AB16,'MN IRP'!AB33)</f>
         <v>0</v>
       </c>
       <c r="AE16">
-        <f>SUM(BPMCCS!AC16,'MN IRP'!AC42)</f>
+        <f>SUM(BPMCCS!AC16,'MN IRP'!AC33)</f>
         <v>0</v>
       </c>
       <c r="AF16">
-        <f>SUM(BPMCCS!AD16,'MN IRP'!AD42)</f>
+        <f>SUM(BPMCCS!AD16,'MN IRP'!AD33)</f>
         <v>0</v>
       </c>
       <c r="AG16">
-        <f>SUM(BPMCCS!AE16,'MN IRP'!AE42)</f>
+        <f>SUM(BPMCCS!AE16,'MN IRP'!AE33)</f>
         <v>0</v>
       </c>
       <c r="AH16">
-        <f>SUM(BPMCCS!AF16,'MN IRP'!AF42)</f>
+        <f>SUM(BPMCCS!AF16,'MN IRP'!AF33)</f>
         <v>0</v>
       </c>
       <c r="AI16">
-        <f>SUM(BPMCCS!AG16,'MN IRP'!AG42)</f>
+        <f>SUM(BPMCCS!AG16,'MN IRP'!AG33)</f>
         <v>0</v>
       </c>
     </row>
@@ -5064,131 +4945,131 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f>SUM(BPMCCS!B17,'MN IRP'!B43)</f>
+        <f>SUM(BPMCCS!B17,'MN IRP'!B34)</f>
         <v>0</v>
       </c>
       <c r="E17">
-        <f>SUM(BPMCCS!C17,'MN IRP'!C43)</f>
+        <f>SUM(BPMCCS!C17,'MN IRP'!C34)</f>
         <v>0</v>
       </c>
       <c r="F17">
-        <f>SUM(BPMCCS!D17,'MN IRP'!D43)</f>
+        <f>SUM(BPMCCS!D17,'MN IRP'!D34)</f>
         <v>0</v>
       </c>
       <c r="G17">
-        <f>SUM(BPMCCS!E17,'MN IRP'!E43)</f>
+        <f>SUM(BPMCCS!E17,'MN IRP'!E34)</f>
         <v>0</v>
       </c>
       <c r="H17">
-        <f>SUM(BPMCCS!F17,'MN IRP'!F43)</f>
+        <f>SUM(BPMCCS!F17,'MN IRP'!F34)</f>
         <v>0</v>
       </c>
       <c r="I17">
-        <f>SUM(BPMCCS!G17,'MN IRP'!G43)</f>
+        <f>SUM(BPMCCS!G17,'MN IRP'!G34)</f>
         <v>0</v>
       </c>
       <c r="J17">
-        <f>SUM(BPMCCS!H17,'MN IRP'!H43)</f>
+        <f>SUM(BPMCCS!H17,'MN IRP'!H34)</f>
         <v>0</v>
       </c>
       <c r="K17">
-        <f>SUM(BPMCCS!I17,'MN IRP'!I43)</f>
+        <f>SUM(BPMCCS!I17,'MN IRP'!I34)</f>
         <v>0</v>
       </c>
       <c r="L17">
-        <f>SUM(BPMCCS!J17,'MN IRP'!J43)</f>
+        <f>SUM(BPMCCS!J17,'MN IRP'!J34)</f>
         <v>0</v>
       </c>
       <c r="M17">
-        <f>SUM(BPMCCS!K17,'MN IRP'!K43)</f>
+        <f>SUM(BPMCCS!K17,'MN IRP'!K34)</f>
         <v>0</v>
       </c>
       <c r="N17">
-        <f>SUM(BPMCCS!L17,'MN IRP'!L43)</f>
+        <f>SUM(BPMCCS!L17,'MN IRP'!L34)</f>
         <v>0</v>
       </c>
       <c r="O17">
-        <f>SUM(BPMCCS!M17,'MN IRP'!M43)</f>
+        <f>SUM(BPMCCS!M17,'MN IRP'!M34)</f>
         <v>0</v>
       </c>
       <c r="P17">
-        <f>SUM(BPMCCS!N17,'MN IRP'!N43)</f>
+        <f>SUM(BPMCCS!N17,'MN IRP'!N34)</f>
         <v>0</v>
       </c>
       <c r="Q17">
-        <f>SUM(BPMCCS!O17,'MN IRP'!O43)</f>
+        <f>SUM(BPMCCS!O17,'MN IRP'!O34)</f>
         <v>0</v>
       </c>
       <c r="R17">
-        <f>SUM(BPMCCS!P17,'MN IRP'!P43)</f>
+        <f>SUM(BPMCCS!P17,'MN IRP'!P34)</f>
         <v>0</v>
       </c>
       <c r="S17">
-        <f>SUM(BPMCCS!Q17,'MN IRP'!Q43)</f>
+        <f>SUM(BPMCCS!Q17,'MN IRP'!Q34)</f>
         <v>0</v>
       </c>
       <c r="T17">
-        <f>SUM(BPMCCS!R17,'MN IRP'!R43)</f>
+        <f>SUM(BPMCCS!R17,'MN IRP'!R34)</f>
         <v>0</v>
       </c>
       <c r="U17">
-        <f>SUM(BPMCCS!S17,'MN IRP'!S43)</f>
+        <f>SUM(BPMCCS!S17,'MN IRP'!S34)</f>
         <v>0</v>
       </c>
       <c r="V17">
-        <f>SUM(BPMCCS!T17,'MN IRP'!T43)</f>
+        <f>SUM(BPMCCS!T17,'MN IRP'!T34)</f>
         <v>0</v>
       </c>
       <c r="W17">
-        <f>SUM(BPMCCS!U17,'MN IRP'!U43)</f>
+        <f>SUM(BPMCCS!U17,'MN IRP'!U34)</f>
         <v>0</v>
       </c>
       <c r="X17">
-        <f>SUM(BPMCCS!V17,'MN IRP'!V43)</f>
+        <f>SUM(BPMCCS!V17,'MN IRP'!V34)</f>
         <v>0</v>
       </c>
       <c r="Y17">
-        <f>SUM(BPMCCS!W17,'MN IRP'!W43)</f>
+        <f>SUM(BPMCCS!W17,'MN IRP'!W34)</f>
         <v>0</v>
       </c>
       <c r="Z17">
-        <f>SUM(BPMCCS!X17,'MN IRP'!X43)</f>
+        <f>SUM(BPMCCS!X17,'MN IRP'!X34)</f>
         <v>0</v>
       </c>
       <c r="AA17">
-        <f>SUM(BPMCCS!Y17,'MN IRP'!Y43)</f>
+        <f>SUM(BPMCCS!Y17,'MN IRP'!Y34)</f>
         <v>0</v>
       </c>
       <c r="AB17">
-        <f>SUM(BPMCCS!Z17,'MN IRP'!Z43)</f>
+        <f>SUM(BPMCCS!Z17,'MN IRP'!Z34)</f>
         <v>0</v>
       </c>
       <c r="AC17">
-        <f>SUM(BPMCCS!AA17,'MN IRP'!AA43)</f>
+        <f>SUM(BPMCCS!AA17,'MN IRP'!AA34)</f>
         <v>0</v>
       </c>
       <c r="AD17">
-        <f>SUM(BPMCCS!AB17,'MN IRP'!AB43)</f>
+        <f>SUM(BPMCCS!AB17,'MN IRP'!AB34)</f>
         <v>0</v>
       </c>
       <c r="AE17">
-        <f>SUM(BPMCCS!AC17,'MN IRP'!AC43)</f>
+        <f>SUM(BPMCCS!AC17,'MN IRP'!AC34)</f>
         <v>0</v>
       </c>
       <c r="AF17">
-        <f>SUM(BPMCCS!AD17,'MN IRP'!AD43)</f>
+        <f>SUM(BPMCCS!AD17,'MN IRP'!AD34)</f>
         <v>0</v>
       </c>
       <c r="AG17">
-        <f>SUM(BPMCCS!AE17,'MN IRP'!AE43)</f>
+        <f>SUM(BPMCCS!AE17,'MN IRP'!AE34)</f>
         <v>0</v>
       </c>
       <c r="AH17">
-        <f>SUM(BPMCCS!AF17,'MN IRP'!AF43)</f>
+        <f>SUM(BPMCCS!AF17,'MN IRP'!AF34)</f>
         <v>0</v>
       </c>
       <c r="AI17">
-        <f>SUM(BPMCCS!AG17,'MN IRP'!AG43)</f>
+        <f>SUM(BPMCCS!AG17,'MN IRP'!AG34)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 2600 MWs gas peaker
</commit_message>
<xml_diff>
--- a/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/PMCCS/Pol Mandated Cap Const Sched.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Minnesota\MN_mod\InputData\elec\PMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350912C-2B54-43D8-878F-2BDAD6FAE660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F613C0-45E3-4DEE-B1C2-0DF7CE6571D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="1635" windowWidth="19980" windowHeight="15225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>PMCCS Policy Mandated Capacity Construction Schedule</t>
   </si>
@@ -141,17 +141,26 @@
     <t>Combined Cycle Resources and Renewable Resources</t>
   </si>
   <si>
-    <t>NG CC</t>
+    <t>Renewables</t>
   </si>
   <si>
-    <t>Sherco</t>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>NG peaker</t>
+  </si>
+  <si>
+    <t>NG nonpeaker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +181,21 @@
       <color rgb="FF313131"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -218,10 +242,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -231,8 +257,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -246,6 +277,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>310431</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>6353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>55553</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B09004B8-95AD-4635-8F98-E32A717965BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6988514" y="387353"/>
+          <a:ext cx="3393736" cy="2525700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -624,19 +704,21 @@
   <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -646,13 +728,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -715,20 +800,53 @@
         <v>2250</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>2027</v>
       </c>
+      <c r="D13">
+        <v>2034</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4">
         <v>800</v>
       </c>
-      <c r="D14" t="s">
-        <v>36</v>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5">
+        <f>SUM(C14:D14)</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4">
+        <v>2600</v>
+      </c>
+      <c r="E15" s="5">
+        <f>SUM(D15:D15)</f>
+        <v>2600</v>
+      </c>
+      <c r="F15" s="10">
+        <f>E15/5</f>
+        <v>520</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
@@ -946,6 +1064,27 @@
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="M29" s="11">
+        <f>$F$15</f>
+        <v>520</v>
+      </c>
+      <c r="N29" s="11">
+        <f>$F$15</f>
+        <v>520</v>
+      </c>
+      <c r="O29" s="11">
+        <f>$F$15</f>
+        <v>520</v>
+      </c>
+      <c r="P29" s="11">
+        <f>$F$15</f>
+        <v>520</v>
+      </c>
+      <c r="Q29" s="11">
+        <f>$F$15</f>
+        <v>520</v>
+      </c>
+      <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -986,8 +1125,12 @@
       <c r="J37" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{81FA8E87-B72A-4B7A-86B8-9D79B2E06D2A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -996,7 +1139,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4293,25 +4436,25 @@
         <f>SUM(BPMCCS!L12,'MN IRP'!L29)</f>
         <v>0</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="8">
         <f>SUM(BPMCCS!M12,'MN IRP'!M29)</f>
-        <v>0</v>
-      </c>
-      <c r="P12">
+        <v>520</v>
+      </c>
+      <c r="P12" s="8">
         <f>SUM(BPMCCS!N12,'MN IRP'!N29)</f>
-        <v>0</v>
-      </c>
-      <c r="Q12">
+        <v>520</v>
+      </c>
+      <c r="Q12" s="8">
         <f>SUM(BPMCCS!O12,'MN IRP'!O29)</f>
-        <v>0</v>
-      </c>
-      <c r="R12">
+        <v>520</v>
+      </c>
+      <c r="R12" s="8">
         <f>SUM(BPMCCS!P12,'MN IRP'!P29)</f>
-        <v>0</v>
-      </c>
-      <c r="S12">
+        <v>520</v>
+      </c>
+      <c r="S12" s="8">
         <f>SUM(BPMCCS!Q12,'MN IRP'!Q29)</f>
-        <v>0</v>
+        <v>520</v>
       </c>
       <c r="T12">
         <f>SUM(BPMCCS!R12,'MN IRP'!R29)</f>

</xml_diff>